<commit_message>
F03: adding the conceptual mapping file
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -31,15 +31,15 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="I165">
+    <comment authorId="0" ref="C64">
       <text>
-        <t xml:space="preserve">is it a isSubjectToLotSpecificTerm? (new epo)
+        <t xml:space="preserve">It should be /P and no /p/FT/@TYPE?
 	-ibrahim dellal</t>
       </text>
     </comment>
     <comment authorId="0" ref="I92">
       <text>
-        <t xml:space="preserve">isCompetitionTermination is deleted
+        <t xml:space="preserve">isCompetitionTermination is deleted. Changed name =&gt; XXXX on the XXXX class
 	-ibrahim dellal</t>
       </text>
     </comment>
@@ -782,7 +782,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasTelephone ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:telephone ?</t>
     </r>
     <r>
       <rPr>
@@ -839,7 +839,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasEmail ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:email ?</t>
     </r>
     <r>
       <rPr>
@@ -1829,7 +1829,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:isSubjectToLotTerm / epo:definesSpecificPlaceOfPerformance / epo:hasNutsCode </t>
+      <t xml:space="preserve"> epo:isSubjectToLotSpecificTerm / epo:definesSpecificPlaceOfPerformance / epo:hasNutsCode </t>
     </r>
     <r>
       <rPr>
@@ -1859,7 +1859,7 @@
     <t>epo:Lot / epo:ContractTerm / dct:Location / locn:Address / rdf:langString</t>
   </si>
   <si>
-    <t>?this epo:isSubjectToLotTerm / epo:definesSpecificPlaceOfPerformance / locn:address / locn:fullAddress ?value .</t>
+    <t>?this epo:isSubjectToLotSpecificTerm / epo:definesSpecificPlaceOfPerformance / locn:address / locn:fullAddress ?value .</t>
   </si>
   <si>
     <t>II.2.4</t>
@@ -2571,7 +2571,7 @@
   <si>
     <r>
       <rPr/>
-      <t>?this epo:isSubjectToLotTerm / epo:hasFrameworkAgreementType &lt;</t>
+      <t>?this epo:isSubjectToLotSpecificTerm / epo:hasFrameworkAgreementType &lt;</t>
     </r>
     <r>
       <rPr>
@@ -3709,7 +3709,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasEmail ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:email ?</t>
     </r>
     <r>
       <rPr>
@@ -3754,7 +3754,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasTelephone ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:telephone ?</t>
     </r>
     <r>
       <rPr>
@@ -4675,7 +4675,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasEmail ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:email ?</t>
     </r>
     <r>
       <rPr>
@@ -4725,7 +4725,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasTelephone ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:telephone ?</t>
     </r>
     <r>
       <rPr>
@@ -5132,7 +5132,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasEmail ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:email ?</t>
     </r>
     <r>
       <rPr>
@@ -5182,7 +5182,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasTelephone ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:telephone ?</t>
     </r>
     <r>
       <rPr>
@@ -5316,7 +5316,7 @@
     <t>epo:Lot / epo:ReviewTerm</t>
   </si>
   <si>
-    <t>?this epo:isSubjectToLotTerm / epo:hasReviewDeadlineInformation ?value .</t>
+    <t>?this epo:isSubjectToLotSpecificTerm / epo:hasReviewDeadlineInformation ?value .</t>
   </si>
   <si>
     <t>VI.4.4</t>
@@ -5607,7 +5607,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasEmail ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:email ?</t>
     </r>
     <r>
       <rPr>
@@ -5657,7 +5657,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:hasTelephone ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasPrimaryContactPoint  / cpov:telephone ?</t>
     </r>
     <r>
       <rPr>
@@ -6427,7 +6427,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="140">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6774,13 +6774,10 @@
     <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -7228,7 +7225,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -7263,7 +7260,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -7298,7 +7295,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -7333,7 +7330,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -7368,7 +7365,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -7403,7 +7400,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -15039,21 +15036,21 @@
       <c r="B165" s="36" t="s">
         <v>768</v>
       </c>
-      <c r="C165" s="124" t="s">
+      <c r="C165" s="95" t="s">
         <v>769</v>
       </c>
-      <c r="D165" s="124" t="s">
+      <c r="D165" s="95" t="s">
         <v>770</v>
       </c>
-      <c r="E165" s="124"/>
-      <c r="F165" s="125" t="s">
+      <c r="E165" s="95"/>
+      <c r="F165" s="96" t="s">
         <v>771</v>
       </c>
-      <c r="G165" s="125"/>
-      <c r="H165" s="126" t="s">
+      <c r="G165" s="124"/>
+      <c r="H165" s="125" t="s">
         <v>772</v>
       </c>
-      <c r="I165" s="126" t="s">
+      <c r="I165" s="125" t="s">
         <v>773</v>
       </c>
     </row>
@@ -15308,17 +15305,17 @@
       <c r="B176" s="36" t="s">
         <v>805</v>
       </c>
-      <c r="C176" s="127" t="s">
+      <c r="C176" s="126" t="s">
         <v>806</v>
       </c>
-      <c r="D176" s="127" t="s">
+      <c r="D176" s="126" t="s">
         <v>807</v>
       </c>
       <c r="E176" s="109"/>
-      <c r="F176" s="128" t="s">
+      <c r="F176" s="127" t="s">
         <v>808</v>
       </c>
-      <c r="G176" s="128"/>
+      <c r="G176" s="127"/>
       <c r="H176" s="113" t="s">
         <v>809</v>
       </c>
@@ -20499,7 +20496,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>853</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -20507,7 +20504,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="129" t="s">
         <v>855</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -20515,7 +20512,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="130" t="s">
         <v>857</v>
       </c>
     </row>
@@ -20552,28 +20549,28 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="132" t="s">
+      <c r="B12" s="131" t="s">
         <v>864</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="35"/>
-      <c r="B13" s="133" t="s">
+      <c r="B13" s="132" t="s">
         <v>865</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="133" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="134" t="s">
         <v>867</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="135" t="s">
         <v>868</v>
       </c>
     </row>
@@ -20593,7 +20590,7 @@
       <c r="A19" s="10" t="s">
         <v>871</v>
       </c>
-      <c r="B19" s="137"/>
+      <c r="B19" s="136"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
@@ -20717,34 +20714,34 @@
       <c r="AB2" s="32"/>
     </row>
     <row r="5">
-      <c r="A5" s="138" t="s">
+      <c r="A5" s="137" t="s">
         <v>288</v>
       </c>
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="138" t="s">
+      <c r="C5" s="137" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="138" t="s">
+      <c r="D5" s="137" t="s">
         <v>874</v>
       </c>
-      <c r="E5" s="139" t="s">
+      <c r="E5" s="138" t="s">
         <v>875</v>
       </c>
-      <c r="F5" s="139" t="s">
+      <c r="F5" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="139" t="s">
+      <c r="G5" s="138" t="s">
         <v>876</v>
       </c>
-      <c r="H5" s="139" t="s">
+      <c r="H5" s="138" t="s">
         <v>877</v>
       </c>
-      <c r="I5" s="138" t="s">
+      <c r="I5" s="137" t="s">
         <v>878</v>
       </c>
-      <c r="J5" s="138" t="s">
+      <c r="J5" s="137" t="s">
         <v>879</v>
       </c>
     </row>
@@ -20776,7 +20773,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -20872,7 +20869,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>
@@ -20923,7 +20920,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>880</v>
       </c>
     </row>

</xml_diff>

<commit_message>
F03: adding link from Procedure to Lot (hasProcurementScopeDividedIntoLot)
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="966">
   <si>
     <t>Field</t>
   </si>
@@ -2297,6 +2297,15 @@
   </si>
   <si>
     <t>Procedure</t>
+  </si>
+  <si>
+    <t>PROCEDURE</t>
+  </si>
+  <si>
+    <t>epo:Procedure / epo:Lot</t>
+  </si>
+  <si>
+    <t>?this epo:hasProcurementScopeDividedIntoLot ?value</t>
   </si>
   <si>
     <t>IV.1</t>
@@ -5888,9 +5897,6 @@
   </si>
   <si>
     <t>Direct Award Justification Code</t>
-  </si>
-  <si>
-    <t>PROCEDURE</t>
   </si>
   <si>
     <t>epo:Procedure / epo:DirectAwardTerm / at-voc:direct-award-justification</t>
@@ -10557,15 +10563,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -10592,15 +10598,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -10627,15 +10633,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -10662,15 +10668,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -10697,15 +10703,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -10732,15 +10738,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -12973,14 +12979,20 @@
       <c r="C67" s="65"/>
       <c r="D67" s="65"/>
       <c r="E67" s="65"/>
-      <c r="F67" s="65"/>
+      <c r="F67" s="22" t="s">
+        <v>372</v>
+      </c>
       <c r="G67" s="65"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
+      <c r="H67" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="I67" s="32" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="42" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B68" s="32" t="s">
         <v>8</v>
@@ -12995,298 +13007,298 @@
     </row>
     <row r="69">
       <c r="A69" s="42" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
     </row>
     <row r="70">
       <c r="A70" s="71" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B70" s="72" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C70" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D70" s="66" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E70" s="66"/>
       <c r="F70" s="66" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="G70" s="66"/>
       <c r="H70" s="33" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I70" s="73" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="71" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B71" s="72" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C71" s="66" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D71" s="66" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="E71" s="66"/>
       <c r="F71" s="66" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="G71" s="66"/>
       <c r="H71" s="33" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I71" s="33" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="71" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B72" s="72" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C72" s="66" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D72" s="66" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E72" s="66"/>
       <c r="F72" s="66" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G72" s="66"/>
       <c r="H72" s="33" t="s">
         <v>177</v>
       </c>
       <c r="I72" s="33" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="42" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C73" s="66" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D73" s="66" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="E73" s="66"/>
       <c r="F73" s="66" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="G73" s="66"/>
       <c r="H73" s="33" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I73" s="33" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="42" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C74" s="66" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D74" s="66" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E74" s="66"/>
       <c r="F74" s="66" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G74" s="66"/>
       <c r="H74" s="33" t="s">
         <v>177</v>
       </c>
       <c r="I74" s="33" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="42" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C75" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D75" s="66" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E75" s="66"/>
       <c r="F75" s="66" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="G75" s="66"/>
       <c r="H75" s="33" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I75" s="64" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="42" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C76" s="66" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D76" s="66" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="E76" s="66"/>
       <c r="F76" s="66" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="G76" s="66"/>
       <c r="H76" s="33" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I76" s="33" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="42" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C77" s="66" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D77" s="66" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E77" s="66"/>
       <c r="F77" s="66" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="G77" s="66"/>
       <c r="H77" s="33" t="s">
         <v>177</v>
       </c>
       <c r="I77" s="33" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="42" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C78" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D78" s="66" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E78" s="66"/>
       <c r="F78" s="66" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="G78" s="66"/>
       <c r="H78" s="33" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I78" s="64" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="42" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B79" s="32" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="C79" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D79" s="66" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E79" s="66"/>
       <c r="F79" s="66" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="G79" s="66"/>
       <c r="H79" s="33" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I79" s="73" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="42" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C80" s="66" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D80" s="66" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E80" s="66"/>
       <c r="F80" s="66" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G80" s="66"/>
       <c r="H80" s="33" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I80" s="73" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="42" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B81" s="32" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C81" s="74" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D81" s="75"/>
       <c r="E81" s="75"/>
@@ -13297,63 +13309,63 @@
     </row>
     <row r="82">
       <c r="A82" s="42" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C82" s="66" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="D82" s="66" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="E82" s="66"/>
       <c r="F82" s="66" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="G82" s="66"/>
       <c r="H82" s="33" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="I82" s="73" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="42" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C83" s="66" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="D83" s="66" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="E83" s="66"/>
       <c r="F83" s="66" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="G83" s="66"/>
       <c r="H83" s="33" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="I83" s="73" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="42" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B84" s="32" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F84" s="65"/>
       <c r="G84" s="65"/>
@@ -13362,62 +13374,62 @@
     </row>
     <row r="85">
       <c r="A85" s="42" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C85" s="66" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="D85" s="66" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="E85" s="66"/>
       <c r="F85" s="66" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="G85" s="66"/>
       <c r="H85" s="33" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="I85" s="73" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="42" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="B86" s="32" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C86" s="66" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="D86" s="66" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="E86" s="66"/>
       <c r="F86" s="33" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="G86" s="62" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="H86" s="33" t="s">
         <v>353</v>
       </c>
       <c r="I86" s="33" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="42" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B87" s="32" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="F87" s="65"/>
       <c r="G87" s="65"/>
@@ -13426,74 +13438,74 @@
     </row>
     <row r="88">
       <c r="A88" s="42" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B88" s="76" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C88" s="77" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D88" s="77" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="E88" s="77"/>
       <c r="F88" s="78" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="G88" s="77"/>
       <c r="H88" s="79" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="I88" s="80" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="42" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B89" s="32" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="F89" s="65"/>
       <c r="G89" s="65"/>
       <c r="H89" s="32" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="I89" s="28"/>
     </row>
     <row r="90">
       <c r="A90" s="42" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B90" s="32" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C90" s="66" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="D90" s="33" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E90" s="33"/>
       <c r="F90" s="66" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G90" s="66"/>
       <c r="H90" s="33" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="I90" s="33" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="42" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B91" s="32" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C91" s="21"/>
       <c r="F91" s="65"/>
@@ -13503,261 +13515,261 @@
     </row>
     <row r="92">
       <c r="A92" s="42" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B92" s="32" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C92" s="66" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D92" s="66" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="E92" s="66"/>
       <c r="F92" s="66" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="G92" s="66"/>
       <c r="H92" s="33" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="I92" s="33" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="42" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B93" s="32" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="F93" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G93" s="81"/>
       <c r="H93" s="32" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="I93" s="32" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="42" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B94" s="32"/>
       <c r="C94" s="82"/>
       <c r="D94" s="82"/>
       <c r="E94" s="82"/>
       <c r="F94" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G94" s="83"/>
       <c r="H94" s="32" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="I94" s="32" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="42" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B95" s="32"/>
       <c r="C95" s="82"/>
       <c r="D95" s="82"/>
       <c r="E95" s="82"/>
       <c r="F95" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G95" s="83"/>
       <c r="H95" s="32" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="I95" s="32" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="42" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B96" s="32" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C96" s="82" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="D96" s="82" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="E96" s="82"/>
       <c r="F96" s="83" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="G96" s="83"/>
       <c r="H96" s="32" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="I96" s="32" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="42" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="B97" s="32" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C97" s="82" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="D97" s="82" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="E97" s="82"/>
       <c r="F97" s="83" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="G97" s="83"/>
       <c r="H97" s="84" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="I97" s="32" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="42" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B98" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C98" s="82" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="D98" s="82" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E98" s="82"/>
       <c r="F98" s="83" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="G98" s="83"/>
       <c r="H98" s="32" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="I98" s="32" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="42" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="B99" s="32"/>
       <c r="C99" s="82"/>
       <c r="D99" s="82"/>
       <c r="E99" s="82"/>
       <c r="F99" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G99" s="85"/>
       <c r="H99" s="33" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="I99" s="86" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="42" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B100" s="32" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C100" s="82" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="D100" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="E100" s="82"/>
       <c r="F100" s="85" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="G100" s="85" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="H100" s="33" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="I100" s="86" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="42" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B101" s="32"/>
       <c r="C101" s="82"/>
       <c r="D101" s="82"/>
       <c r="E101" s="82"/>
       <c r="F101" s="79" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="G101" s="79" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="H101" s="33" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="I101" s="86" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="42" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C102" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D102" s="82"/>
       <c r="E102" s="82"/>
       <c r="F102" s="79" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="G102" s="79" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="H102" s="33" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="I102" s="86" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="42" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C103" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D103" s="82"/>
       <c r="E103" s="82"/>
@@ -13768,86 +13780,86 @@
     </row>
     <row r="104">
       <c r="A104" s="42" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C104" s="82" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="D104" s="82" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E104" s="82"/>
       <c r="F104" s="83" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="G104" s="83"/>
       <c r="H104" s="32" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="I104" s="89" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="42" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B105" s="32" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="C105" s="82" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="D105" s="82" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E105" s="82"/>
       <c r="F105" s="83" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="G105" s="83"/>
       <c r="H105" s="32" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="I105" s="89" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="42" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B106" s="32" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="C106" s="90" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="D106" s="82"/>
       <c r="E106" s="82"/>
       <c r="F106" s="83" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="G106" s="83"/>
       <c r="H106" s="33" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="I106" s="86" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="42" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B107" s="32" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="C107" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D107" s="82"/>
       <c r="E107" s="82"/>
@@ -13858,41 +13870,41 @@
     </row>
     <row r="108">
       <c r="A108" s="42" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B108" s="32" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="C108" s="82" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="D108" s="82" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="E108" s="82"/>
       <c r="F108" s="83" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="G108" s="83"/>
       <c r="H108" s="22" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="I108" s="32" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="42" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C109" s="82"/>
       <c r="D109" s="82"/>
       <c r="E109" s="82"/>
       <c r="F109" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G109" s="91"/>
       <c r="H109" s="64" t="s">
@@ -13904,172 +13916,172 @@
     </row>
     <row r="110">
       <c r="A110" s="42" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B110" s="32" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="C110" s="82" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="D110" s="82" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="E110" s="82"/>
       <c r="F110" s="83" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="G110" s="83"/>
       <c r="H110" s="32" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="I110" s="32" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="42" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="B111" s="32" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="C111" s="82" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D111" s="82" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E111" s="82"/>
       <c r="F111" s="83" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="G111" s="83"/>
       <c r="H111" s="32" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="I111" s="32" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="42" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="B112" s="32" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="C112" s="82" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D112" s="82" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E112" s="82"/>
       <c r="F112" s="83" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="G112" s="83"/>
       <c r="H112" s="32" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="I112" s="32" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="42" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="B113" s="32" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="C113" s="82" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D113" s="82" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E113" s="82"/>
       <c r="F113" s="83" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="G113" s="83"/>
       <c r="H113" s="32" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="42" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B114" s="32" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="C114" s="82" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D114" s="82" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E114" s="82"/>
       <c r="F114" s="83" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="G114" s="83"/>
       <c r="H114" s="32" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="I114" s="32" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="42" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="B115" s="32" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C115" s="92" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="D115" s="82"/>
       <c r="E115" s="82"/>
       <c r="F115" s="83" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="G115" s="62" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="H115" s="33" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="I115" s="33" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="42" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="B116" s="32" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="C116" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D116" s="82"/>
       <c r="E116" s="82"/>
       <c r="F116" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G116" s="88"/>
       <c r="H116" s="33" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="I116" s="33" t="s">
         <v>48</v>
@@ -14077,28 +14089,28 @@
     </row>
     <row r="117">
       <c r="A117" s="42" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="B117" s="32"/>
       <c r="C117" s="88"/>
       <c r="D117" s="82"/>
       <c r="E117" s="82"/>
       <c r="F117" s="79" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="G117" s="79" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="H117" s="33" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="I117" s="86" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="42" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="B118" s="32" t="s">
         <v>50</v>
@@ -14111,19 +14123,19 @@
       </c>
       <c r="E118" s="82"/>
       <c r="F118" s="83" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="G118" s="83"/>
       <c r="H118" s="35" t="s">
         <v>54</v>
       </c>
       <c r="I118" s="35" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="42" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B119" s="32" t="s">
         <v>57</v>
@@ -14136,19 +14148,19 @@
       </c>
       <c r="E119" s="82"/>
       <c r="F119" s="83" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="G119" s="83"/>
       <c r="H119" s="36" t="s">
         <v>61</v>
       </c>
       <c r="I119" s="36" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="42" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="B120" s="32" t="s">
         <v>64</v>
@@ -14161,19 +14173,19 @@
       </c>
       <c r="E120" s="82"/>
       <c r="F120" s="83" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="G120" s="83"/>
       <c r="H120" s="32" t="s">
         <v>68</v>
       </c>
       <c r="I120" s="32" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="42" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="B121" s="32" t="s">
         <v>71</v>
@@ -14186,19 +14198,19 @@
       </c>
       <c r="E121" s="82"/>
       <c r="F121" s="83" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="G121" s="83"/>
       <c r="H121" s="32" t="s">
         <v>68</v>
       </c>
       <c r="I121" s="32" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="42" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="B122" s="32" t="s">
         <v>77</v>
@@ -14211,21 +14223,21 @@
       </c>
       <c r="E122" s="82"/>
       <c r="F122" s="83" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="G122" s="83" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="H122" s="33" t="s">
         <v>82</v>
       </c>
       <c r="I122" s="33" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="42" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="B123" s="32" t="s">
         <v>85</v>
@@ -14234,23 +14246,23 @@
         <v>86</v>
       </c>
       <c r="D123" s="82" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E123" s="82"/>
       <c r="F123" s="83" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="G123" s="83"/>
       <c r="H123" s="32" t="s">
         <v>88</v>
       </c>
       <c r="I123" s="32" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="42" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="B124" s="32" t="s">
         <v>91</v>
@@ -14263,19 +14275,19 @@
       </c>
       <c r="E124" s="82"/>
       <c r="F124" s="83" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="G124" s="83"/>
       <c r="H124" s="35" t="s">
         <v>95</v>
       </c>
       <c r="I124" s="35" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="42" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="B125" s="32" t="s">
         <v>111</v>
@@ -14288,19 +14300,19 @@
       </c>
       <c r="E125" s="82"/>
       <c r="F125" s="83" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="G125" s="83"/>
       <c r="H125" s="32" t="s">
         <v>115</v>
       </c>
       <c r="I125" s="33" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="42" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="B126" s="32" t="s">
         <v>105</v>
@@ -14313,22 +14325,22 @@
       </c>
       <c r="E126" s="82"/>
       <c r="F126" s="83" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="G126" s="83"/>
       <c r="H126" s="32" t="s">
         <v>102</v>
       </c>
       <c r="I126" s="33" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="42" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="B127" s="32" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="C127" s="88"/>
       <c r="D127" s="82"/>
@@ -14340,7 +14352,7 @@
     </row>
     <row r="128">
       <c r="A128" s="42" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="B128" s="32" t="s">
         <v>118</v>
@@ -14353,52 +14365,52 @@
       </c>
       <c r="E128" s="82"/>
       <c r="F128" s="83" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="G128" s="83"/>
       <c r="H128" s="32" t="s">
         <v>102</v>
       </c>
       <c r="I128" s="33" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="42" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="B129" s="32" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C129" s="88" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="D129" s="82" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="E129" s="82"/>
       <c r="F129" s="83" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="G129" s="83" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="H129" s="33" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="I129" s="93" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="42" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="B130" s="32" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C130" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D130" s="82"/>
       <c r="E130" s="82"/>
@@ -14409,10 +14421,10 @@
     </row>
     <row r="131">
       <c r="A131" s="42" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B131" s="32" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="C131" s="82" t="s">
         <v>225</v>
@@ -14422,44 +14434,44 @@
       </c>
       <c r="E131" s="82"/>
       <c r="F131" s="83" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="G131" s="83"/>
       <c r="H131" s="33" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="I131" s="33" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="42" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="B132" s="32" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="C132" s="82" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="D132" s="82" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="E132" s="82"/>
       <c r="F132" s="83" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="G132" s="83"/>
       <c r="H132" s="33" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="I132" s="33" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="42" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="B133" s="32" t="s">
         <v>231</v>
@@ -14472,42 +14484,42 @@
       </c>
       <c r="E133" s="82"/>
       <c r="F133" s="83" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="G133" s="83"/>
       <c r="H133" s="33" t="s">
         <v>235</v>
       </c>
       <c r="I133" s="33" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="42" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B134" s="32" t="s">
         <v>244</v>
       </c>
       <c r="C134" s="94" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D134" s="82"/>
       <c r="E134" s="82"/>
       <c r="F134" s="83" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="G134" s="83"/>
       <c r="H134" s="33" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="I134" s="33" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="42" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="B135" s="32" t="s">
         <v>238</v>
@@ -14520,48 +14532,48 @@
       </c>
       <c r="E135" s="82"/>
       <c r="F135" s="83" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="G135" s="83"/>
       <c r="H135" s="33" t="s">
         <v>235</v>
       </c>
       <c r="I135" s="33" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="42" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="B136" s="32" t="s">
         <v>244</v>
       </c>
       <c r="C136" s="94" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D136" s="82"/>
       <c r="E136" s="82"/>
       <c r="F136" s="83" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="G136" s="83"/>
       <c r="H136" s="33" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="I136" s="33" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="42" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="B137" s="32" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="C137" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D137" s="82"/>
       <c r="E137" s="82"/>
@@ -14572,60 +14584,60 @@
     </row>
     <row r="138">
       <c r="A138" s="42" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="B138" s="32" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C138" s="82" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="D138" s="82" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="E138" s="82"/>
       <c r="F138" s="83" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="G138" s="83"/>
       <c r="H138" s="33" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="I138" s="33" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="42" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="B139" s="32" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="C139" s="82" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="D139" s="82" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="E139" s="82"/>
       <c r="F139" s="83" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="G139" s="83"/>
       <c r="H139" s="33" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="I139" s="33" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="42" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="B140" s="32" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="C140" s="82"/>
       <c r="D140" s="82"/>
@@ -14636,83 +14648,83 @@
     </row>
     <row r="141">
       <c r="A141" s="42" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B141" s="32" t="s">
         <v>244</v>
       </c>
       <c r="C141" s="94" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D141" s="82"/>
       <c r="E141" s="82"/>
       <c r="F141" s="83" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="G141" s="83"/>
       <c r="H141" s="64" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="I141" s="33" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="42" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="C142" s="82" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="D142" s="82" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="E142" s="82"/>
       <c r="F142" s="83" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="G142" s="83"/>
       <c r="H142" s="64" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="I142" s="33" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="42" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="C143" s="82" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="D143" s="82" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="E143" s="82"/>
       <c r="F143" s="83" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="G143" s="83"/>
       <c r="H143" s="64" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="I143" s="33" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="42" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="C144" s="95"/>
       <c r="D144" s="96"/>
@@ -14724,7 +14736,7 @@
     </row>
     <row r="145">
       <c r="A145" s="42" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="B145" s="32" t="s">
         <v>365</v>
@@ -14735,25 +14747,25 @@
       <c r="D145" s="96"/>
       <c r="E145" s="96"/>
       <c r="F145" s="97" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="G145" s="97"/>
       <c r="H145" s="98" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="I145" s="99" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="42" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C146" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D146" s="96"/>
       <c r="E146" s="96"/>
@@ -14764,22 +14776,22 @@
     </row>
     <row r="147">
       <c r="A147" s="42" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="C147" s="101" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D147" s="96"/>
       <c r="E147" s="96"/>
       <c r="F147" s="22" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="G147" s="88"/>
       <c r="H147" s="33" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="I147" s="33" t="s">
         <v>48</v>
@@ -14787,7 +14799,7 @@
     </row>
     <row r="148">
       <c r="A148" s="42" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="B148" s="32" t="s">
         <v>50</v>
@@ -14800,19 +14812,19 @@
       </c>
       <c r="E148" s="82"/>
       <c r="F148" s="83" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="G148" s="83"/>
       <c r="H148" s="102" t="s">
         <v>54</v>
       </c>
       <c r="I148" s="103" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="42" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B149" s="32" t="s">
         <v>64</v>
@@ -14825,19 +14837,19 @@
       </c>
       <c r="E149" s="82"/>
       <c r="F149" s="83" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="G149" s="83"/>
       <c r="H149" s="102" t="s">
         <v>68</v>
       </c>
       <c r="I149" s="103" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="42" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="B150" s="32" t="s">
         <v>71</v>
@@ -14850,19 +14862,19 @@
       </c>
       <c r="E150" s="82"/>
       <c r="F150" s="83" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="G150" s="83"/>
       <c r="H150" s="102" t="s">
         <v>68</v>
       </c>
       <c r="I150" s="103" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="42" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B151" s="32" t="s">
         <v>85</v>
@@ -14871,23 +14883,23 @@
         <v>86</v>
       </c>
       <c r="D151" s="82" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E151" s="82"/>
       <c r="F151" s="83" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="G151" s="83"/>
       <c r="H151" s="104" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="I151" s="104" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="42" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B152" s="32" t="s">
         <v>91</v>
@@ -14900,19 +14912,19 @@
       </c>
       <c r="E152" s="82"/>
       <c r="F152" s="83" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="G152" s="83"/>
       <c r="H152" s="105" t="s">
         <v>82</v>
       </c>
       <c r="I152" s="106" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="42" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="B153" s="32" t="s">
         <v>111</v>
@@ -14925,19 +14937,19 @@
       </c>
       <c r="E153" s="82"/>
       <c r="F153" s="83" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="G153" s="83"/>
       <c r="H153" s="102" t="s">
         <v>115</v>
       </c>
       <c r="I153" s="105" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="42" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="B154" s="32" t="s">
         <v>105</v>
@@ -14950,22 +14962,22 @@
       </c>
       <c r="E154" s="82"/>
       <c r="F154" s="83" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="G154" s="83"/>
       <c r="H154" s="104" t="s">
         <v>102</v>
       </c>
       <c r="I154" s="83" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="42" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="B155" s="32" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="C155" s="82" t="s">
         <v>127</v>
@@ -14975,19 +14987,19 @@
       </c>
       <c r="E155" s="82"/>
       <c r="F155" s="83" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="G155" s="83"/>
       <c r="H155" s="35" t="s">
         <v>130</v>
       </c>
       <c r="I155" s="36" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="42" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="B156" s="32" t="s">
         <v>118</v>
@@ -15000,34 +15012,34 @@
       </c>
       <c r="E156" s="82"/>
       <c r="F156" s="83" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="G156" s="83"/>
       <c r="H156" s="104" t="s">
         <v>102</v>
       </c>
       <c r="I156" s="83" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="42" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="B157" s="32" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="C157" s="101" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D157" s="107"/>
       <c r="E157" s="107"/>
       <c r="F157" s="22" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="G157" s="88"/>
       <c r="H157" s="33" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="I157" s="33" t="s">
         <v>48</v>
@@ -15035,7 +15047,7 @@
     </row>
     <row r="158">
       <c r="A158" s="42" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="B158" s="32" t="s">
         <v>50</v>
@@ -15048,19 +15060,19 @@
       </c>
       <c r="E158" s="82"/>
       <c r="F158" s="83" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="G158" s="83"/>
       <c r="H158" s="102" t="s">
         <v>54</v>
       </c>
       <c r="I158" s="103" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="42" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="B159" s="32" t="s">
         <v>64</v>
@@ -15073,19 +15085,19 @@
       </c>
       <c r="E159" s="82"/>
       <c r="F159" s="83" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="G159" s="83"/>
       <c r="H159" s="102" t="s">
         <v>68</v>
       </c>
       <c r="I159" s="103" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="42" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="B160" s="32" t="s">
         <v>71</v>
@@ -15098,19 +15110,19 @@
       </c>
       <c r="E160" s="82"/>
       <c r="F160" s="83" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="G160" s="83"/>
       <c r="H160" s="102" t="s">
         <v>68</v>
       </c>
       <c r="I160" s="103" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="42" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="B161" s="32" t="s">
         <v>85</v>
@@ -15119,23 +15131,23 @@
         <v>86</v>
       </c>
       <c r="D161" s="82" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E161" s="82"/>
       <c r="F161" s="83" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="G161" s="83"/>
       <c r="H161" s="104" t="s">
         <v>88</v>
       </c>
       <c r="I161" s="104" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="42" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="B162" s="32" t="s">
         <v>91</v>
@@ -15148,19 +15160,19 @@
       </c>
       <c r="E162" s="82"/>
       <c r="F162" s="83" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="G162" s="83"/>
       <c r="H162" s="102" t="s">
         <v>82</v>
       </c>
       <c r="I162" s="103" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="42" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="B163" s="32" t="s">
         <v>111</v>
@@ -15173,19 +15185,19 @@
       </c>
       <c r="E163" s="82"/>
       <c r="F163" s="83" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="G163" s="83"/>
       <c r="H163" s="102" t="s">
         <v>115</v>
       </c>
       <c r="I163" s="105" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="42" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="B164" s="32" t="s">
         <v>105</v>
@@ -15198,22 +15210,22 @@
       </c>
       <c r="E164" s="82"/>
       <c r="F164" s="83" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="G164" s="83"/>
       <c r="H164" s="104" t="s">
         <v>102</v>
       </c>
       <c r="I164" s="83" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="42" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="B165" s="32" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="C165" s="82" t="s">
         <v>127</v>
@@ -15223,19 +15235,19 @@
       </c>
       <c r="E165" s="82"/>
       <c r="F165" s="83" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="G165" s="83"/>
       <c r="H165" s="35" t="s">
         <v>130</v>
       </c>
       <c r="I165" s="36" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="42" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B166" s="32" t="s">
         <v>118</v>
@@ -15248,57 +15260,57 @@
       </c>
       <c r="E166" s="82"/>
       <c r="F166" s="83" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="G166" s="83"/>
       <c r="H166" s="104" t="s">
         <v>102</v>
       </c>
       <c r="I166" s="83" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="42" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="B167" s="32" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C167" s="82" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="D167" s="82" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="E167" s="82"/>
       <c r="F167" s="83" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="G167" s="108"/>
       <c r="H167" s="109" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="I167" s="109" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="42" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="B168" s="32" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C168" s="95"/>
       <c r="D168" s="95"/>
       <c r="E168" s="95"/>
       <c r="F168" s="22" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="G168" s="88"/>
       <c r="H168" s="33" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="I168" s="33" t="s">
         <v>48</v>
@@ -15306,7 +15318,7 @@
     </row>
     <row r="169">
       <c r="A169" s="42" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="B169" s="32" t="s">
         <v>50</v>
@@ -15319,19 +15331,19 @@
       </c>
       <c r="E169" s="82"/>
       <c r="F169" s="83" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="G169" s="83"/>
       <c r="H169" s="102" t="s">
         <v>54</v>
       </c>
       <c r="I169" s="103" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="42" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="B170" s="32" t="s">
         <v>64</v>
@@ -15344,19 +15356,19 @@
       </c>
       <c r="E170" s="82"/>
       <c r="F170" s="83" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="G170" s="83"/>
       <c r="H170" s="102" t="s">
         <v>68</v>
       </c>
       <c r="I170" s="103" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="42" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="B171" s="32" t="s">
         <v>71</v>
@@ -15369,19 +15381,19 @@
       </c>
       <c r="E171" s="82"/>
       <c r="F171" s="83" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="G171" s="83"/>
       <c r="H171" s="102" t="s">
         <v>68</v>
       </c>
       <c r="I171" s="103" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="42" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="B172" s="32" t="s">
         <v>85</v>
@@ -15390,23 +15402,23 @@
         <v>86</v>
       </c>
       <c r="D172" s="82" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E172" s="82"/>
       <c r="F172" s="83" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="G172" s="83"/>
       <c r="H172" s="104" t="s">
         <v>88</v>
       </c>
       <c r="I172" s="104" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="42" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="B173" s="32" t="s">
         <v>91</v>
@@ -15419,19 +15431,19 @@
       </c>
       <c r="E173" s="82"/>
       <c r="F173" s="83" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="G173" s="83"/>
       <c r="H173" s="105" t="s">
         <v>82</v>
       </c>
       <c r="I173" s="106" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="42" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="B174" s="32" t="s">
         <v>111</v>
@@ -15444,19 +15456,19 @@
       </c>
       <c r="E174" s="82"/>
       <c r="F174" s="83" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="G174" s="83"/>
       <c r="H174" s="102" t="s">
         <v>115</v>
       </c>
       <c r="I174" s="105" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="42" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="B175" s="32" t="s">
         <v>105</v>
@@ -15469,22 +15481,22 @@
       </c>
       <c r="E175" s="82"/>
       <c r="F175" s="83" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="G175" s="83"/>
       <c r="H175" s="104" t="s">
         <v>102</v>
       </c>
       <c r="I175" s="83" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="42" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="B176" s="32" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="C176" s="82" t="s">
         <v>127</v>
@@ -15494,19 +15506,19 @@
       </c>
       <c r="E176" s="82"/>
       <c r="F176" s="83" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="G176" s="83"/>
       <c r="H176" s="35" t="s">
         <v>130</v>
       </c>
       <c r="I176" s="36" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="42" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="B177" s="32" t="s">
         <v>118</v>
@@ -15519,176 +15531,176 @@
       </c>
       <c r="E177" s="82"/>
       <c r="F177" s="83" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="G177" s="83"/>
       <c r="H177" s="104" t="s">
         <v>102</v>
       </c>
       <c r="I177" s="83" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="42" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="B178" s="32" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="C178" s="110" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="D178" s="110" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="E178" s="110"/>
       <c r="F178" s="111" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="G178" s="111"/>
       <c r="H178" s="99" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="I178" s="99" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="42" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="B179" s="32" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="H179" s="28"/>
       <c r="I179" s="28"/>
     </row>
     <row r="180">
       <c r="A180" s="42" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="B180" s="32" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="C180" s="112" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D180" s="88"/>
       <c r="E180" s="88"/>
       <c r="F180" s="83" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="H180" s="28"/>
       <c r="I180" s="28"/>
     </row>
     <row r="181">
       <c r="A181" s="42" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="B181" s="32" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="C181" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D181" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E181" s="82"/>
       <c r="F181" s="22" t="s">
-        <v>826</v>
+        <v>372</v>
       </c>
       <c r="H181" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I181" s="89" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="42" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="B182" s="32" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C182" s="113" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="D182" s="113" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="E182" s="113"/>
       <c r="F182" s="114" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="G182" s="57"/>
       <c r="H182" s="115" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="I182" s="51" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="42" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B183" s="32" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="C183" s="113" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="D183" s="113" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="E183" s="113"/>
       <c r="F183" s="114" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="G183" s="57"/>
       <c r="H183" s="115" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="I183" s="116" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="42" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B184" s="32" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C184" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D184" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E184" s="82"/>
       <c r="F184" s="83" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="H184" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I184" s="89" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="42" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="B185" s="32" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="C185" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D185" s="82"/>
       <c r="E185" s="82"/>
@@ -15697,205 +15709,205 @@
     </row>
     <row r="186">
       <c r="A186" s="42" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="B186" s="32" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C186" s="82" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D186" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E186" s="82"/>
       <c r="F186" s="83" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="H186" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I186" s="89" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="42" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="B187" s="32" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="C187" s="82" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D187" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E187" s="82"/>
       <c r="F187" s="83" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="H187" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I187" s="89" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="42" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="B188" s="32" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="C188" s="82" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D188" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E188" s="82"/>
       <c r="F188" s="83" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="H188" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I188" s="89" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="42" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B189" s="32" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C189" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D189" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E189" s="82"/>
       <c r="F189" s="83" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="H189" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I189" s="89" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="42" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B190" s="32" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="C190" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D190" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E190" s="82"/>
       <c r="F190" s="83" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="H190" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I190" s="89" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="42" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="B191" s="32" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C191" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D191" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E191" s="82"/>
       <c r="F191" s="83" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="H191" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I191" s="89" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="42" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="B192" s="32" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C192" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D192" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E192" s="82"/>
       <c r="F192" s="83" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="H192" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I192" s="89" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="42" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="B193" s="32" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="C193" s="87" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D193" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E193" s="82"/>
       <c r="F193" s="83" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="H193" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I193" s="89" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="42" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="B194" s="32" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C194" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D194" s="82"/>
       <c r="E194" s="82"/>
@@ -15904,61 +15916,61 @@
     </row>
     <row r="195">
       <c r="A195" s="42" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B195" s="47" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="C195" s="82" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D195" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E195" s="82"/>
       <c r="F195" s="83" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="H195" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I195" s="89" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="42" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="B196" s="47" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C196" s="82" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="D196" s="82" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="E196" s="82"/>
       <c r="F196" s="83" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="H196" s="32" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I196" s="89" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="42" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="B197" s="47" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C197" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D197" s="88"/>
       <c r="E197" s="88"/>
@@ -15967,35 +15979,35 @@
     </row>
     <row r="198">
       <c r="A198" s="42" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="B198" s="47" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="C198" s="117" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="D198" s="82"/>
       <c r="E198" s="82"/>
       <c r="F198" s="83" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="H198" s="33" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I198" s="73" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="42" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="B199" s="47" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="C199" s="87" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D199" s="88"/>
       <c r="E199" s="88"/>
@@ -16004,26 +16016,26 @@
     </row>
     <row r="200">
       <c r="A200" s="42" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="B200" s="47" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C200" s="87" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="D200" s="82" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E200" s="82"/>
       <c r="F200" s="111" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="H200" s="32" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="I200" s="63" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
     </row>
     <row r="201">
@@ -20160,36 +20172,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="119" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="120" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="121" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="122" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="8">
@@ -20200,41 +20212,41 @@
     </row>
     <row r="10">
       <c r="A10" s="122" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="122" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="123" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="31"/>
       <c r="B13" s="124" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="125" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="126" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="127" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="17">
@@ -20243,24 +20255,24 @@
     </row>
     <row r="18">
       <c r="A18" s="122" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="B19" s="128"/>
     </row>
     <row r="21">
       <c r="A21" s="122" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
     </row>
   </sheetData>
@@ -20286,52 +20298,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="122" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="66" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="66" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="66" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
     </row>
   </sheetData>
@@ -20357,48 +20369,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B1" s="129" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="130" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -20440,76 +20452,76 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
     </row>
   </sheetData>
@@ -20536,31 +20548,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -20587,15 +20599,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="131" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="122" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="B2" s="122" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
F03: handling sparql reports bugs
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -2194,7 +2194,7 @@
     <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / epo:Numeric</t>
   </si>
   <si>
-    <t>?this epo:describesResultNotice / epo:hasTotalAwardedValue / epo:hasAmountValue ?value .</t>
+    <t>?this epo:announcesNoticeAwardInformation / epo:hasTotalAwardedValue / epo:hasAmountValue ?value .</t>
   </si>
   <si>
     <t>II.1.7.2</t>
@@ -2232,7 +2232,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:describesResultNotice / epo:hasProcurementLowestReceivedTenderValue / epo:hasAmountValue ?</t>
+      <t xml:space="preserve"> epo:announcesNoticeAwardInformation / epo:hasProcurementLowestReceivedTenderValue / epo:hasAmountValue ?</t>
     </r>
     <r>
       <rPr>
@@ -2266,7 +2266,7 @@
     <t>OBJECT_CONTRACT/VAL_RANGE_TOTAL/HIGH</t>
   </si>
   <si>
-    <t>?this epo:describesResultNotice / epo:hasProcurementHighestReceivedTenderValue / epo:hasAmountValue ?value .</t>
+    <t>?this epo:announcesNoticeAwardInformation / epo:hasProcurementHighestReceivedTenderValue / epo:hasAmountValue ?value .</t>
   </si>
   <si>
     <t>II.1.7.4</t>
@@ -2294,7 +2294,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">?this epo:describesResultNotice / epo:hasTotalAwardedValue / epo:hasCurrency </t>
+      <t xml:space="preserve">?this epo:announcesNoticeAwardInformation / epo:hasTotalAwardedValue / epo:hasCurrency </t>
     </r>
     <r>
       <rPr>
@@ -2309,7 +2309,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> } UNION { ?this epo:describesResultNotice / epo:hasProcurementLowestReceivedTenderValue / epo:hasCurrency ?value } UNION  { ?this epo:describesResultNotice / epo:hasProcurementHighestReceivedTenderValue / epo:hasCurrency ?value } UNION </t>
+      <t xml:space="preserve"> } UNION { ?this epo:announcesNoticeAwardInformation / epo:hasProcurementLowestReceivedTenderValue / epo:hasCurrency ?value } UNION  { ?this epo:announcesNoticeAwardInformation / epo:hasProcurementHighestReceivedTenderValue / epo:hasCurrency ?value } UNION </t>
     </r>
   </si>
   <si>
@@ -3258,7 +3258,7 @@
     <t>epo:Procedure /  epo:FrameworkAgreementTechniqueUsage</t>
   </si>
   <si>
-    <t>?this epo:usesTechnique ?this</t>
+    <t>?this epo:usesTechnique ?value .</t>
   </si>
   <si>
     <t>IV.1.3.2</t>
@@ -4801,7 +4801,7 @@
     <t>epo:Tender / epo:SubcontractingEstimate / MonetaryValue /at-voc:currency (from currency.json)</t>
   </si>
   <si>
-    <t>?this epo:forseesSubcontracting / epo:hasSubcontractingEstimatedValue / epo:hasCurrency ?value .</t>
+    <t>?this epo:foreseesSubcontracting / epo:hasSubcontractingEstimatedValue / epo:hasCurrency ?value .</t>
   </si>
   <si>
     <t>V.2.5.5</t>
@@ -4842,7 +4842,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:forseesSubcontracting / epo:hasEstimatedPercentage ?</t>
+      <t xml:space="preserve"> epo:foreseesSubcontracting / epo:hasEstimatedPercentage ?</t>
     </r>
     <r>
       <rPr>
@@ -4892,7 +4892,7 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">this epo:forseesSubcontracting / </t>
+      <t xml:space="preserve">this epo:foreseesSubcontracting / </t>
     </r>
     <r>
       <rPr>
@@ -6630,7 +6630,7 @@
     <t>AgentInRole === section 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Winner </t>
+    <t>Winner  AND Tenderer</t>
   </si>
   <si>
     <t>AgentInRole === section 6 Review body</t>

</xml_diff>

<commit_message>
F03: Update shacl validation files & the conceptual mappings
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -106,7 +106,7 @@
 	-ibrahim dellal</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G202">
+    <comment authorId="0" ref="G201">
       <text>
         <t xml:space="preserve">Previous Procedure (It should be already created What is its identifier??? )
 	-ibrahim dellal
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="994">
   <si>
     <t>Field</t>
   </si>
@@ -184,7 +184,7 @@
     <t>EPO version</t>
   </si>
   <si>
-    <t>3.0.0.beta</t>
+    <t>3.0.1.beta</t>
   </si>
   <si>
     <r>
@@ -364,7 +364,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasName ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
     <r>
       <rPr>
@@ -1105,7 +1105,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasName ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
     <r>
       <rPr>
@@ -1700,7 +1700,7 @@
     <t>CONTRACTING_BODY/PROCUREMENT_LAW</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / epo:ProcedureTerm / rdf:langString</t>
+    <t>epo:ResultNotice / epo:Procedure / epo:ProcedureSpecificTerm / rdf:langString</t>
   </si>
   <si>
     <r>
@@ -2494,7 +2494,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:foreseesContractTerm / epo:definesSpecificPlaceOfPerformance / epo:hasNutsCode </t>
+      <t xml:space="preserve"> epo:foreseesContractSpecificTerm / epo:definesSpecificPlaceOfPerformance / epo:hasNutsCode </t>
     </r>
     <r>
       <rPr>
@@ -2524,7 +2524,7 @@
     <t>epo:Lot / epo:ContractTerm / dct:Location / locn:Address / rdf:langString</t>
   </si>
   <si>
-    <t>?this epo:foreseesContractTerm / epo:definesSpecificPlaceOfPerformance / locn:address / locn:fullAddress ?value .</t>
+    <t>?this epo:foreseesContractSpecificTerm / epo:definesSpecificPlaceOfPerformance / locn:address / locn:fullAddress ?value .</t>
   </si>
   <si>
     <t>II.2.4</t>
@@ -2811,7 +2811,7 @@
     <t>epo:Lot / epo:ContractTerm / xsd:boolean</t>
   </si>
   <si>
-    <t>?this epo:foreseesContractTerm / epo:hasOptions ?value .</t>
+    <t>?this epo:foreseesContractSpecificTerm / epo:hasOptions ?value .</t>
   </si>
   <si>
     <t>II.2.11.2</t>
@@ -2832,7 +2832,7 @@
     <t>epo:Lot / epo:ContractTerm / rdf:langString</t>
   </si>
   <si>
-    <t>?this epo:foreseesContractTerm / epo:hasOptionsDescription ?value .</t>
+    <t>?this epo:foreseesContractSpecificTerm / epo:hasOptionsDescription ?value .</t>
   </si>
   <si>
     <t>II.2.13</t>
@@ -3630,15 +3630,6 @@
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
-  </si>
-  <si>
-    <t>V.0.5</t>
-  </si>
-  <si>
-    <t>epo:Lot / epo:LotAwardOutcome</t>
-  </si>
-  <si>
-    <t>?this epo:describesLot ?value</t>
   </si>
   <si>
     <t>V.0.6</t>
@@ -3687,6 +3678,9 @@
     <t>epo:LotAwardOutcome / epo:Lot</t>
   </si>
   <si>
+    <t>?this epo:describesLot ?value</t>
+  </si>
+  <si>
     <t>V.1.1.1</t>
   </si>
   <si>
@@ -4059,7 +4053,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasName ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
     <r>
       <rPr>
@@ -5027,7 +5021,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasName ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
     <r>
       <rPr>
@@ -5337,7 +5331,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasName ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
     <r>
       <rPr>
@@ -5665,7 +5659,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / epo:hasName ?</t>
+      <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
     <r>
       <rPr>
@@ -6630,7 +6624,7 @@
     <t>AgentInRole === section 5</t>
   </si>
   <si>
-    <t>Winner  AND Tenderer</t>
+    <t xml:space="preserve">Winner </t>
   </si>
   <si>
     <t>AgentInRole === section 6 Review body</t>
@@ -14135,679 +14129,677 @@
       <c r="A119" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="B119" s="32"/>
-      <c r="C119" s="82"/>
-      <c r="D119" s="82"/>
-      <c r="E119" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="F119" s="85"/>
+      <c r="B119" s="32" t="s">
+        <v>554</v>
+      </c>
+      <c r="C119" s="82" t="s">
+        <v>555</v>
+      </c>
+      <c r="D119" s="82" t="s">
+        <v>556</v>
+      </c>
+      <c r="E119" s="85" t="s">
+        <v>557</v>
+      </c>
+      <c r="F119" s="85" t="s">
+        <v>558</v>
+      </c>
       <c r="G119" s="34" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="H119" s="48" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="42" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B120" s="32" t="s">
-        <v>557</v>
-      </c>
-      <c r="C120" s="82" t="s">
-        <v>558</v>
-      </c>
-      <c r="D120" s="82" t="s">
-        <v>559</v>
-      </c>
-      <c r="E120" s="85" t="s">
-        <v>560</v>
-      </c>
-      <c r="F120" s="85" t="s">
-        <v>561</v>
-      </c>
-      <c r="G120" s="34" t="s">
         <v>562</v>
       </c>
-      <c r="H120" s="48" t="s">
-        <v>563</v>
-      </c>
+      <c r="C120" s="86" t="s">
+        <v>462</v>
+      </c>
+      <c r="D120" s="82"/>
     </row>
     <row r="121">
       <c r="A121" s="42" t="s">
+        <v>563</v>
+      </c>
+      <c r="B121" s="32" t="s">
         <v>564</v>
-      </c>
-      <c r="B121" s="32" t="s">
-        <v>565</v>
       </c>
       <c r="C121" s="86" t="s">
         <v>462</v>
       </c>
       <c r="D121" s="82"/>
+      <c r="E121" s="87"/>
+      <c r="F121" s="87"/>
+      <c r="G121" s="34" t="s">
+        <v>565</v>
+      </c>
+      <c r="H121" s="34" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="42" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B122" s="32" t="s">
-        <v>567</v>
-      </c>
-      <c r="C122" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D122" s="82"/>
-      <c r="E122" s="87"/>
-      <c r="F122" s="87"/>
+        <v>568</v>
+      </c>
+      <c r="C122" s="82" t="s">
+        <v>569</v>
+      </c>
+      <c r="D122" s="82" t="s">
+        <v>570</v>
+      </c>
+      <c r="E122" s="83" t="s">
+        <v>571</v>
+      </c>
+      <c r="F122" s="83"/>
       <c r="G122" s="34" t="s">
-        <v>568</v>
-      </c>
-      <c r="H122" s="34" t="s">
-        <v>555</v>
+        <v>572</v>
+      </c>
+      <c r="H122" s="73" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="42" t="s">
+        <v>574</v>
+      </c>
+      <c r="B123" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="C123" s="82" t="s">
         <v>569</v>
       </c>
-      <c r="B123" s="32" t="s">
+      <c r="D123" s="82" t="s">
         <v>570</v>
       </c>
-      <c r="C123" s="82" t="s">
-        <v>571</v>
-      </c>
-      <c r="D123" s="82" t="s">
+      <c r="E123" s="83" t="s">
+        <v>576</v>
+      </c>
+      <c r="F123" s="83"/>
+      <c r="G123" s="32" t="s">
         <v>572</v>
       </c>
-      <c r="E123" s="83" t="s">
-        <v>573</v>
-      </c>
-      <c r="F123" s="83"/>
-      <c r="G123" s="34" t="s">
-        <v>574</v>
-      </c>
-      <c r="H123" s="73" t="s">
-        <v>575</v>
+      <c r="H123" s="88" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="42" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B124" s="32" t="s">
-        <v>577</v>
-      </c>
-      <c r="C124" s="82" t="s">
-        <v>571</v>
-      </c>
-      <c r="D124" s="82" t="s">
-        <v>572</v>
-      </c>
+        <v>579</v>
+      </c>
+      <c r="C124" s="89" t="s">
+        <v>580</v>
+      </c>
+      <c r="D124" s="82"/>
       <c r="E124" s="83" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="F124" s="83"/>
-      <c r="G124" s="32" t="s">
-        <v>574</v>
-      </c>
-      <c r="H124" s="88" t="s">
-        <v>579</v>
+      <c r="G124" s="34" t="s">
+        <v>582</v>
+      </c>
+      <c r="H124" s="48" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="42" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="B125" s="32" t="s">
-        <v>581</v>
-      </c>
-      <c r="C125" s="89" t="s">
-        <v>582</v>
+        <v>525</v>
+      </c>
+      <c r="C125" s="86" t="s">
+        <v>462</v>
       </c>
       <c r="D125" s="82"/>
-      <c r="E125" s="83" t="s">
-        <v>583</v>
-      </c>
-      <c r="F125" s="83"/>
-      <c r="G125" s="34" t="s">
-        <v>584</v>
-      </c>
-      <c r="H125" s="48" t="s">
-        <v>585</v>
-      </c>
+      <c r="E125" s="82"/>
+      <c r="F125" s="82"/>
+      <c r="G125" s="28"/>
+      <c r="H125" s="28"/>
     </row>
     <row r="126">
       <c r="A126" s="42" t="s">
+        <v>585</v>
+      </c>
+      <c r="B126" s="32"/>
+      <c r="C126" s="82"/>
+      <c r="E126" s="79" t="s">
         <v>586</v>
       </c>
-      <c r="B126" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="C126" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D126" s="82"/>
-      <c r="E126" s="82"/>
-      <c r="F126" s="82"/>
-      <c r="G126" s="28"/>
-      <c r="H126" s="28"/>
+      <c r="F126" s="79" t="s">
+        <v>257</v>
+      </c>
+      <c r="G126" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="H126" s="48" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="42" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B127" s="32"/>
       <c r="C127" s="82"/>
       <c r="E127" s="79" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F127" s="79" t="s">
-        <v>257</v>
+        <v>589</v>
       </c>
       <c r="G127" s="34" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H127" s="48" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="42" t="s">
-        <v>587</v>
-      </c>
-      <c r="B128" s="32"/>
-      <c r="C128" s="82"/>
-      <c r="E128" s="79" t="s">
-        <v>588</v>
-      </c>
-      <c r="F128" s="79" t="s">
-        <v>591</v>
-      </c>
-      <c r="G128" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="H128" s="48" t="s">
+      <c r="B128" s="32" t="s">
         <v>593</v>
+      </c>
+      <c r="C128" s="82" t="s">
+        <v>594</v>
+      </c>
+      <c r="D128" s="82" t="s">
+        <v>595</v>
+      </c>
+      <c r="E128" s="83" t="s">
+        <v>596</v>
+      </c>
+      <c r="F128" s="83"/>
+      <c r="G128" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="H128" s="32" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="42" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="B129" s="32" t="s">
-        <v>595</v>
-      </c>
-      <c r="C129" s="82" t="s">
-        <v>596</v>
-      </c>
-      <c r="D129" s="82" t="s">
-        <v>597</v>
-      </c>
-      <c r="E129" s="83" t="s">
-        <v>598</v>
-      </c>
-      <c r="F129" s="83"/>
-      <c r="G129" s="22" t="s">
-        <v>551</v>
-      </c>
-      <c r="H129" s="32" t="s">
         <v>599</v>
+      </c>
+      <c r="C129" s="82"/>
+      <c r="D129" s="82"/>
+      <c r="E129" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="F129" s="90"/>
+      <c r="G129" s="67" t="s">
+        <v>600</v>
+      </c>
+      <c r="H129" s="34" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="42" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B130" s="32" t="s">
-        <v>601</v>
-      </c>
-      <c r="C130" s="82"/>
-      <c r="D130" s="82"/>
-      <c r="E130" s="22" t="s">
-        <v>526</v>
-      </c>
-      <c r="F130" s="90"/>
-      <c r="G130" s="67" t="s">
-        <v>602</v>
+        <v>603</v>
+      </c>
+      <c r="C130" s="82" t="s">
+        <v>604</v>
+      </c>
+      <c r="D130" s="82" t="s">
+        <v>605</v>
+      </c>
+      <c r="E130" s="83" t="s">
+        <v>606</v>
+      </c>
+      <c r="F130" s="83"/>
+      <c r="G130" s="34" t="s">
+        <v>607</v>
       </c>
       <c r="H130" s="34" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="42" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="B131" s="32" t="s">
-        <v>605</v>
-      </c>
-      <c r="C131" s="82" t="s">
-        <v>606</v>
-      </c>
-      <c r="D131" s="82" t="s">
-        <v>607</v>
-      </c>
+        <v>610</v>
+      </c>
+      <c r="C131" s="82"/>
+      <c r="D131" s="82"/>
       <c r="E131" s="83" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="F131" s="83"/>
-      <c r="G131" s="34" t="s">
-        <v>609</v>
-      </c>
-      <c r="H131" s="34" t="s">
-        <v>610</v>
+      <c r="G131" s="32" t="s">
+        <v>612</v>
+      </c>
+      <c r="H131" s="32" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="42" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B132" s="32" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C132" s="82"/>
       <c r="D132" s="82"/>
       <c r="E132" s="83" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="F132" s="83"/>
       <c r="G132" s="32" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H132" s="32" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="42" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B133" s="32" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="C133" s="82"/>
       <c r="D133" s="82"/>
       <c r="E133" s="83" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="F133" s="83"/>
       <c r="G133" s="32" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H133" s="32" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="42" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B134" s="32" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C134" s="82"/>
       <c r="D134" s="82"/>
       <c r="E134" s="83" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="F134" s="83"/>
       <c r="G134" s="32" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H134" s="32" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="42" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B135" s="32" t="s">
-        <v>625</v>
-      </c>
-      <c r="C135" s="82"/>
+        <v>627</v>
+      </c>
+      <c r="C135" s="91" t="s">
+        <v>628</v>
+      </c>
       <c r="D135" s="82"/>
       <c r="E135" s="83" t="s">
-        <v>626</v>
-      </c>
-      <c r="F135" s="83"/>
-      <c r="G135" s="32" t="s">
-        <v>614</v>
-      </c>
-      <c r="H135" s="32" t="s">
-        <v>627</v>
+        <v>629</v>
+      </c>
+      <c r="F135" s="47"/>
+      <c r="G135" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H135" s="48" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="42" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B136" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="C136" s="91" t="s">
-        <v>630</v>
+        <v>631</v>
+      </c>
+      <c r="C136" s="86" t="s">
+        <v>462</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="83" t="s">
-        <v>631</v>
-      </c>
-      <c r="F136" s="47"/>
-      <c r="G136" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="H136" s="48" t="s">
-        <v>146</v>
-      </c>
+      <c r="E136" s="22"/>
+      <c r="F136" s="87"/>
+      <c r="G136" s="34"/>
+      <c r="H136" s="34"/>
     </row>
     <row r="137">
       <c r="A137" s="42" t="s">
         <v>632</v>
       </c>
       <c r="B137" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C137" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="D137" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="E137" s="83" t="s">
         <v>633</v>
       </c>
-      <c r="C137" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D137" s="82"/>
-      <c r="E137" s="22"/>
-      <c r="F137" s="87"/>
-      <c r="G137" s="34"/>
-      <c r="H137" s="34"/>
+      <c r="F137" s="83"/>
+      <c r="G137" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H137" s="37" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="42" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B138" s="32" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C138" s="87" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D138" s="82" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E138" s="83" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F138" s="83"/>
-      <c r="G138" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="H138" s="37" t="s">
-        <v>636</v>
+      <c r="G138" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="H138" s="40" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="42" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B139" s="32" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C139" s="87" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D139" s="82" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E139" s="83" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F139" s="83"/>
-      <c r="G139" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="H139" s="40" t="s">
-        <v>639</v>
+      <c r="G139" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H139" s="32" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="42" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B140" s="32" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C140" s="87" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D140" s="82" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E140" s="83" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F140" s="83"/>
       <c r="G140" s="32" t="s">
         <v>71</v>
       </c>
       <c r="H140" s="32" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="42" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C141" s="87" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D141" s="82" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E141" s="83" t="s">
-        <v>644</v>
-      </c>
-      <c r="F141" s="83"/>
-      <c r="G141" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="H141" s="32" t="s">
         <v>645</v>
+      </c>
+      <c r="F141" s="83" t="s">
+        <v>646</v>
+      </c>
+      <c r="G141" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="H141" s="34" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="42" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C142" s="87" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D142" s="82" t="s">
-        <v>82</v>
+        <v>649</v>
       </c>
       <c r="E142" s="83" t="s">
-        <v>647</v>
-      </c>
-      <c r="F142" s="83" t="s">
-        <v>648</v>
-      </c>
-      <c r="G142" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="H142" s="34" t="s">
-        <v>649</v>
+        <v>650</v>
+      </c>
+      <c r="F142" s="83"/>
+      <c r="G142" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="H142" s="32" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="42" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C143" s="87" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D143" s="82" t="s">
-        <v>651</v>
+        <v>97</v>
       </c>
       <c r="E143" s="83" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F143" s="83"/>
-      <c r="G143" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="H143" s="32" t="s">
-        <v>653</v>
+      <c r="G143" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="H143" s="37" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="42" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C144" s="87" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="C144" s="92" t="s">
+        <v>116</v>
       </c>
       <c r="D144" s="82" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E144" s="83" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F144" s="83"/>
-      <c r="G144" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="H144" s="37" t="s">
-        <v>656</v>
+      <c r="G144" s="93" t="s">
+        <v>657</v>
+      </c>
+      <c r="H144" s="93" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="42" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B145" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C145" s="92" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C145" s="87" t="s">
+        <v>110</v>
       </c>
       <c r="D145" s="82" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E145" s="83" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="F145" s="83"/>
       <c r="G145" s="93" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="H145" s="93" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="42" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C146" s="87" t="s">
-        <v>110</v>
+        <v>664</v>
+      </c>
+      <c r="C146" s="82" t="s">
+        <v>131</v>
       </c>
       <c r="D146" s="82" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E146" s="83" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="F146" s="83"/>
-      <c r="G146" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H146" s="93" t="s">
-        <v>664</v>
+      <c r="G146" s="40" t="s">
+        <v>657</v>
+      </c>
+      <c r="H146" s="40" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="42" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>666</v>
-      </c>
-      <c r="C147" s="82" t="s">
-        <v>131</v>
+        <v>122</v>
+      </c>
+      <c r="C147" s="87" t="s">
+        <v>123</v>
       </c>
       <c r="D147" s="82" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E147" s="83" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="F147" s="83"/>
-      <c r="G147" s="40" t="s">
-        <v>659</v>
-      </c>
-      <c r="H147" s="40" t="s">
-        <v>668</v>
+      <c r="G147" s="93" t="s">
+        <v>661</v>
+      </c>
+      <c r="H147" s="93" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="42" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B148" s="32" t="s">
-        <v>122</v>
+        <v>671</v>
       </c>
       <c r="C148" s="87" t="s">
-        <v>123</v>
+        <v>672</v>
       </c>
       <c r="D148" s="82" t="s">
-        <v>124</v>
+        <v>673</v>
       </c>
       <c r="E148" s="83" t="s">
-        <v>670</v>
-      </c>
-      <c r="F148" s="83"/>
-      <c r="G148" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H148" s="93" t="s">
-        <v>671</v>
+        <v>674</v>
+      </c>
+      <c r="F148" s="83" t="s">
+        <v>257</v>
+      </c>
+      <c r="G148" s="34" t="s">
+        <v>675</v>
+      </c>
+      <c r="H148" s="94" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="42" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="B149" s="32" t="s">
-        <v>673</v>
-      </c>
-      <c r="C149" s="87" t="s">
-        <v>674</v>
-      </c>
-      <c r="D149" s="82" t="s">
-        <v>675</v>
-      </c>
-      <c r="E149" s="83" t="s">
-        <v>676</v>
-      </c>
-      <c r="F149" s="83" t="s">
-        <v>257</v>
-      </c>
-      <c r="G149" s="34" t="s">
-        <v>677</v>
-      </c>
-      <c r="H149" s="94" t="s">
         <v>678</v>
       </c>
+      <c r="C149" s="86" t="s">
+        <v>462</v>
+      </c>
+      <c r="D149" s="82"/>
+      <c r="E149" s="87"/>
+      <c r="F149" s="87"/>
+      <c r="G149" s="32"/>
+      <c r="H149" s="32"/>
     </row>
     <row r="150">
       <c r="A150" s="42" t="s">
@@ -14816,128 +14808,134 @@
       <c r="B150" s="32" t="s">
         <v>680</v>
       </c>
-      <c r="C150" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D150" s="82"/>
-      <c r="E150" s="87"/>
-      <c r="F150" s="87"/>
-      <c r="G150" s="32"/>
-      <c r="H150" s="32"/>
+      <c r="C150" s="82" t="s">
+        <v>265</v>
+      </c>
+      <c r="D150" s="82" t="s">
+        <v>266</v>
+      </c>
+      <c r="E150" s="83" t="s">
+        <v>681</v>
+      </c>
+      <c r="F150" s="83"/>
+      <c r="G150" s="34" t="s">
+        <v>682</v>
+      </c>
+      <c r="H150" s="34" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="42" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="B151" s="32" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="C151" s="82" t="s">
-        <v>265</v>
+        <v>686</v>
       </c>
       <c r="D151" s="82" t="s">
-        <v>266</v>
+        <v>687</v>
       </c>
       <c r="E151" s="83" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="F151" s="83"/>
       <c r="G151" s="34" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
       <c r="H151" s="34" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="42" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="B152" s="32" t="s">
-        <v>687</v>
+        <v>271</v>
       </c>
       <c r="C152" s="82" t="s">
-        <v>688</v>
+        <v>272</v>
       </c>
       <c r="D152" s="82" t="s">
-        <v>689</v>
+        <v>273</v>
       </c>
       <c r="E152" s="83" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="F152" s="83"/>
       <c r="G152" s="34" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="H152" s="34" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="42" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B153" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="C153" s="82" t="s">
-        <v>272</v>
-      </c>
-      <c r="D153" s="82" t="s">
-        <v>273</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="C153" s="95" t="s">
+        <v>696</v>
+      </c>
+      <c r="D153" s="82"/>
       <c r="E153" s="83" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="F153" s="83"/>
       <c r="G153" s="34" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="H153" s="34" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="42" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="B154" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="C154" s="95" t="s">
-        <v>698</v>
-      </c>
-      <c r="D154" s="82"/>
+        <v>277</v>
+      </c>
+      <c r="C154" s="82" t="s">
+        <v>278</v>
+      </c>
+      <c r="D154" s="82" t="s">
+        <v>279</v>
+      </c>
       <c r="E154" s="83" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="F154" s="83"/>
       <c r="G154" s="34" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="H154" s="34" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="42" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B155" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="C155" s="82" t="s">
-        <v>278</v>
-      </c>
-      <c r="D155" s="82" t="s">
-        <v>279</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="C155" s="95" t="s">
+        <v>696</v>
+      </c>
+      <c r="D155" s="82"/>
       <c r="E155" s="83" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="F155" s="83"/>
       <c r="G155" s="34" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="H155" s="34" t="s">
         <v>704</v>
@@ -14948,22 +14946,16 @@
         <v>705</v>
       </c>
       <c r="B156" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="C156" s="95" t="s">
-        <v>698</v>
+        <v>706</v>
+      </c>
+      <c r="C156" s="86" t="s">
+        <v>462</v>
       </c>
       <c r="D156" s="82"/>
-      <c r="E156" s="83" t="s">
-        <v>699</v>
-      </c>
-      <c r="F156" s="83"/>
-      <c r="G156" s="34" t="s">
-        <v>700</v>
-      </c>
-      <c r="H156" s="34" t="s">
-        <v>706</v>
-      </c>
+      <c r="E156" s="87"/>
+      <c r="F156" s="87"/>
+      <c r="G156" s="28"/>
+      <c r="H156" s="28"/>
     </row>
     <row r="157">
       <c r="A157" s="42" t="s">
@@ -14972,36 +14964,28 @@
       <c r="B157" s="32" t="s">
         <v>708</v>
       </c>
-      <c r="C157" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D157" s="82"/>
-      <c r="E157" s="87"/>
-      <c r="F157" s="87"/>
-      <c r="G157" s="28"/>
-      <c r="H157" s="28"/>
+      <c r="C157" s="82" t="s">
+        <v>709</v>
+      </c>
+      <c r="D157" s="82" t="s">
+        <v>710</v>
+      </c>
+      <c r="E157" s="83" t="s">
+        <v>711</v>
+      </c>
+      <c r="F157" s="83"/>
+      <c r="G157" s="67" t="s">
+        <v>712</v>
+      </c>
+      <c r="H157" s="96" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="42" t="s">
-        <v>709</v>
+        <v>714</v>
       </c>
       <c r="B158" s="32" t="s">
-        <v>710</v>
-      </c>
-      <c r="C158" s="82" t="s">
-        <v>711</v>
-      </c>
-      <c r="D158" s="82" t="s">
-        <v>712</v>
-      </c>
-      <c r="E158" s="83" t="s">
-        <v>713</v>
-      </c>
-      <c r="F158" s="83"/>
-      <c r="G158" s="67" t="s">
-        <v>714</v>
-      </c>
-      <c r="H158" s="96" t="s">
         <v>715</v>
       </c>
     </row>
@@ -15012,138 +14996,146 @@
       <c r="B159" s="32" t="s">
         <v>717</v>
       </c>
+      <c r="C159" s="83" t="s">
+        <v>718</v>
+      </c>
+      <c r="D159" s="83" t="s">
+        <v>719</v>
+      </c>
+      <c r="E159" s="83" t="s">
+        <v>720</v>
+      </c>
+      <c r="F159" s="83"/>
+      <c r="G159" s="34" t="s">
+        <v>721</v>
+      </c>
+      <c r="H159" s="34" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="42" t="s">
-        <v>718</v>
+        <v>723</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>719</v>
-      </c>
-      <c r="C160" s="83" t="s">
-        <v>720</v>
-      </c>
-      <c r="D160" s="83" t="s">
-        <v>721</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="C160" s="95" t="s">
+        <v>696</v>
+      </c>
+      <c r="D160" s="82"/>
       <c r="E160" s="83" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="F160" s="83"/>
-      <c r="G160" s="34" t="s">
-        <v>723</v>
+      <c r="G160" s="67" t="s">
+        <v>725</v>
       </c>
       <c r="H160" s="34" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="42" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B161" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="C161" s="95" t="s">
-        <v>698</v>
-      </c>
-      <c r="D161" s="82"/>
+        <v>728</v>
+      </c>
+      <c r="C161" s="82" t="s">
+        <v>729</v>
+      </c>
+      <c r="D161" s="82" t="s">
+        <v>730</v>
+      </c>
       <c r="E161" s="83" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="F161" s="83"/>
       <c r="G161" s="67" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="H161" s="34" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="42" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="B162" s="32" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="C162" s="82" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
       <c r="D162" s="82" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="E162" s="83" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="F162" s="83"/>
       <c r="G162" s="67" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="H162" s="34" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="42" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="B163" s="32" t="s">
-        <v>737</v>
-      </c>
-      <c r="C163" s="82" t="s">
-        <v>738</v>
-      </c>
-      <c r="D163" s="82" t="s">
-        <v>739</v>
-      </c>
-      <c r="E163" s="83" t="s">
-        <v>740</v>
-      </c>
-      <c r="F163" s="83"/>
-      <c r="G163" s="67" t="s">
-        <v>741</v>
-      </c>
-      <c r="H163" s="34" t="s">
         <v>742</v>
       </c>
+      <c r="C163" s="97"/>
+      <c r="D163" s="98"/>
+      <c r="E163" s="97"/>
+      <c r="F163" s="97"/>
+      <c r="G163" s="98"/>
+      <c r="H163" s="98"/>
     </row>
     <row r="164">
       <c r="A164" s="42" t="s">
         <v>743</v>
       </c>
       <c r="B164" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="C164" s="82" t="s">
+        <v>402</v>
+      </c>
+      <c r="D164" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="E164" s="99" t="s">
         <v>744</v>
       </c>
-      <c r="C164" s="97"/>
-      <c r="D164" s="98"/>
-      <c r="E164" s="97"/>
-      <c r="F164" s="97"/>
-      <c r="G164" s="98"/>
-      <c r="H164" s="98"/>
+      <c r="F164" s="99"/>
+      <c r="G164" s="100" t="s">
+        <v>745</v>
+      </c>
+      <c r="H164" s="100" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="42" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B165" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="C165" s="82" t="s">
-        <v>402</v>
-      </c>
-      <c r="D165" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="E165" s="99" t="s">
-        <v>746</v>
-      </c>
-      <c r="F165" s="99"/>
-      <c r="G165" s="100" t="s">
-        <v>747</v>
-      </c>
-      <c r="H165" s="100" t="s">
         <v>748</v>
       </c>
+      <c r="C165" s="86" t="s">
+        <v>462</v>
+      </c>
+      <c r="D165" s="98"/>
+      <c r="E165" s="101"/>
+      <c r="F165" s="101"/>
+      <c r="G165" s="98"/>
+      <c r="H165" s="98"/>
     </row>
     <row r="166">
       <c r="A166" s="42" t="s">
@@ -15152,155 +15144,163 @@
       <c r="B166" s="32" t="s">
         <v>750</v>
       </c>
-      <c r="C166" s="86" t="s">
+      <c r="C166" s="102" t="s">
         <v>462</v>
       </c>
       <c r="D166" s="98"/>
-      <c r="E166" s="101"/>
-      <c r="F166" s="101"/>
-      <c r="G166" s="98"/>
-      <c r="H166" s="98"/>
+      <c r="E166" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="F166" s="87"/>
+      <c r="G166" s="34" t="s">
+        <v>752</v>
+      </c>
+      <c r="H166" s="34" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="42" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="B167" s="32" t="s">
-        <v>752</v>
-      </c>
-      <c r="C167" s="102" t="s">
-        <v>462</v>
-      </c>
-      <c r="D167" s="98"/>
-      <c r="E167" s="22" t="s">
-        <v>753</v>
-      </c>
-      <c r="F167" s="87"/>
-      <c r="G167" s="34" t="s">
-        <v>754</v>
-      </c>
-      <c r="H167" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C167" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="D167" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="E167" s="83" t="s">
         <v>755</v>
+      </c>
+      <c r="F167" s="83"/>
+      <c r="G167" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="H167" s="103" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="42" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B168" s="32" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C168" s="82" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D168" s="82" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E168" s="83" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F168" s="83"/>
       <c r="G168" s="103" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H168" s="104" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="42" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B169" s="32" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C169" s="82" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D169" s="82" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E169" s="83" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="F169" s="83"/>
       <c r="G169" s="103" t="s">
         <v>71</v>
       </c>
       <c r="H169" s="104" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="42" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B170" s="32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C170" s="82" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D170" s="82" t="s">
-        <v>76</v>
+        <v>649</v>
       </c>
       <c r="E170" s="83" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="F170" s="83"/>
-      <c r="G170" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="H170" s="104" t="s">
-        <v>764</v>
+      <c r="G170" s="105" t="s">
+        <v>765</v>
+      </c>
+      <c r="H170" s="105" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="42" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B171" s="32" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C171" s="82" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D171" s="82" t="s">
-        <v>651</v>
+        <v>97</v>
       </c>
       <c r="E171" s="83" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="F171" s="83"/>
-      <c r="G171" s="105" t="s">
-        <v>767</v>
-      </c>
-      <c r="H171" s="105" t="s">
-        <v>768</v>
+      <c r="G171" s="106" t="s">
+        <v>85</v>
+      </c>
+      <c r="H171" s="106" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="42" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B172" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C172" s="82" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="C172" s="83" t="s">
+        <v>116</v>
       </c>
       <c r="D172" s="82" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E172" s="83" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F172" s="83"/>
-      <c r="G172" s="106" t="s">
-        <v>85</v>
-      </c>
-      <c r="H172" s="106" t="s">
-        <v>771</v>
+      <c r="G172" s="93" t="s">
+        <v>657</v>
+      </c>
+      <c r="H172" s="93" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="173">
@@ -15308,23 +15308,23 @@
         <v>772</v>
       </c>
       <c r="B173" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C173" s="83" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C173" s="82" t="s">
+        <v>110</v>
       </c>
       <c r="D173" s="82" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E173" s="83" t="s">
         <v>773</v>
       </c>
       <c r="F173" s="83"/>
       <c r="G173" s="93" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="H173" s="93" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="174">
@@ -15332,47 +15332,47 @@
         <v>774</v>
       </c>
       <c r="B174" s="32" t="s">
-        <v>109</v>
+        <v>664</v>
       </c>
       <c r="C174" s="82" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="D174" s="82" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E174" s="83" t="s">
         <v>775</v>
       </c>
       <c r="F174" s="83"/>
-      <c r="G174" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H174" s="93" t="s">
-        <v>664</v>
+      <c r="G174" s="40" t="s">
+        <v>657</v>
+      </c>
+      <c r="H174" s="40" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="42" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B175" s="32" t="s">
-        <v>666</v>
+        <v>122</v>
       </c>
       <c r="C175" s="82" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D175" s="82" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E175" s="83" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F175" s="83"/>
-      <c r="G175" s="40" t="s">
-        <v>659</v>
-      </c>
-      <c r="H175" s="40" t="s">
-        <v>778</v>
+      <c r="G175" s="93" t="s">
+        <v>661</v>
+      </c>
+      <c r="H175" s="93" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="176">
@@ -15380,165 +15380,165 @@
         <v>779</v>
       </c>
       <c r="B176" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C176" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="D176" s="82" t="s">
-        <v>124</v>
-      </c>
-      <c r="E176" s="83" t="s">
         <v>780</v>
       </c>
-      <c r="F176" s="83"/>
-      <c r="G176" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H176" s="93" t="s">
-        <v>671</v>
+      <c r="C176" s="102" t="s">
+        <v>462</v>
+      </c>
+      <c r="D176" s="107"/>
+      <c r="E176" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="F176" s="87"/>
+      <c r="G176" s="34" t="s">
+        <v>781</v>
+      </c>
+      <c r="H176" s="34" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="42" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B177" s="32" t="s">
-        <v>782</v>
-      </c>
-      <c r="C177" s="102" t="s">
-        <v>462</v>
-      </c>
-      <c r="D177" s="107"/>
-      <c r="E177" s="22" t="s">
-        <v>753</v>
-      </c>
-      <c r="F177" s="87"/>
-      <c r="G177" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C177" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="D177" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="E177" s="83" t="s">
         <v>783</v>
       </c>
-      <c r="H177" s="34" t="s">
-        <v>755</v>
+      <c r="F177" s="83"/>
+      <c r="G177" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="H177" s="103" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="42" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B178" s="32" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C178" s="82" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D178" s="82" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E178" s="83" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F178" s="83"/>
       <c r="G178" s="103" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H178" s="104" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="42" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B179" s="32" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C179" s="82" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D179" s="82" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E179" s="83" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F179" s="83"/>
       <c r="G179" s="103" t="s">
         <v>71</v>
       </c>
       <c r="H179" s="104" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="42" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B180" s="32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C180" s="82" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D180" s="82" t="s">
-        <v>76</v>
+        <v>649</v>
       </c>
       <c r="E180" s="83" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F180" s="83"/>
-      <c r="G180" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="H180" s="104" t="s">
-        <v>792</v>
+      <c r="G180" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="H180" s="105" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="42" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B181" s="32" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C181" s="82" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D181" s="82" t="s">
-        <v>651</v>
+        <v>97</v>
       </c>
       <c r="E181" s="83" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="F181" s="83"/>
-      <c r="G181" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="H181" s="105" t="s">
-        <v>795</v>
+      <c r="G181" s="103" t="s">
+        <v>85</v>
+      </c>
+      <c r="H181" s="103" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="42" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B182" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C182" s="82" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="C182" s="83" t="s">
+        <v>116</v>
       </c>
       <c r="D182" s="82" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E182" s="83" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F182" s="83"/>
-      <c r="G182" s="103" t="s">
-        <v>85</v>
-      </c>
-      <c r="H182" s="103" t="s">
-        <v>798</v>
+      <c r="G182" s="93" t="s">
+        <v>657</v>
+      </c>
+      <c r="H182" s="93" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="183">
@@ -15546,23 +15546,23 @@
         <v>799</v>
       </c>
       <c r="B183" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C183" s="83" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C183" s="82" t="s">
+        <v>110</v>
       </c>
       <c r="D183" s="82" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E183" s="83" t="s">
         <v>800</v>
       </c>
       <c r="F183" s="83"/>
       <c r="G183" s="93" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="H183" s="93" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="184">
@@ -15570,47 +15570,47 @@
         <v>801</v>
       </c>
       <c r="B184" s="32" t="s">
-        <v>109</v>
+        <v>664</v>
       </c>
       <c r="C184" s="82" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="D184" s="82" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E184" s="83" t="s">
         <v>802</v>
       </c>
       <c r="F184" s="83"/>
-      <c r="G184" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H184" s="93" t="s">
-        <v>664</v>
+      <c r="G184" s="40" t="s">
+        <v>657</v>
+      </c>
+      <c r="H184" s="40" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="42" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B185" s="32" t="s">
-        <v>666</v>
+        <v>122</v>
       </c>
       <c r="C185" s="82" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D185" s="82" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E185" s="83" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="F185" s="83"/>
-      <c r="G185" s="40" t="s">
-        <v>659</v>
-      </c>
-      <c r="H185" s="40" t="s">
-        <v>805</v>
+      <c r="G185" s="93" t="s">
+        <v>661</v>
+      </c>
+      <c r="H185" s="93" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="186">
@@ -15618,187 +15618,187 @@
         <v>806</v>
       </c>
       <c r="B186" s="32" t="s">
-        <v>122</v>
+        <v>807</v>
       </c>
       <c r="C186" s="82" t="s">
-        <v>123</v>
+        <v>808</v>
       </c>
       <c r="D186" s="82" t="s">
-        <v>124</v>
+        <v>809</v>
       </c>
       <c r="E186" s="83" t="s">
-        <v>807</v>
-      </c>
-      <c r="F186" s="83"/>
-      <c r="G186" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H186" s="93" t="s">
-        <v>671</v>
+        <v>810</v>
+      </c>
+      <c r="F186" s="92"/>
+      <c r="G186" s="100" t="s">
+        <v>811</v>
+      </c>
+      <c r="H186" s="100" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="42" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="B187" s="32" t="s">
-        <v>809</v>
-      </c>
-      <c r="C187" s="82" t="s">
-        <v>810</v>
-      </c>
-      <c r="D187" s="82" t="s">
-        <v>811</v>
-      </c>
-      <c r="E187" s="83" t="s">
-        <v>812</v>
-      </c>
-      <c r="F187" s="92"/>
-      <c r="G187" s="100" t="s">
-        <v>813</v>
-      </c>
-      <c r="H187" s="100" t="s">
         <v>814</v>
+      </c>
+      <c r="C187" s="97"/>
+      <c r="D187" s="97"/>
+      <c r="E187" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="F187" s="87"/>
+      <c r="G187" s="34" t="s">
+        <v>815</v>
+      </c>
+      <c r="H187" s="34" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="42" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B188" s="32" t="s">
-        <v>816</v>
-      </c>
-      <c r="C188" s="97"/>
-      <c r="D188" s="97"/>
-      <c r="E188" s="22" t="s">
-        <v>753</v>
-      </c>
-      <c r="F188" s="87"/>
-      <c r="G188" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C188" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="D188" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="E188" s="83" t="s">
         <v>817</v>
       </c>
-      <c r="H188" s="34" t="s">
-        <v>755</v>
+      <c r="F188" s="83"/>
+      <c r="G188" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="H188" s="103" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="42" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B189" s="32" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C189" s="82" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D189" s="82" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E189" s="83" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="F189" s="83"/>
       <c r="G189" s="103" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H189" s="104" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="42" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B190" s="32" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C190" s="82" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D190" s="82" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E190" s="83" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="F190" s="83"/>
       <c r="G190" s="103" t="s">
         <v>71</v>
       </c>
       <c r="H190" s="104" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="42" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B191" s="32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C191" s="82" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D191" s="82" t="s">
-        <v>76</v>
+        <v>649</v>
       </c>
       <c r="E191" s="83" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="F191" s="83"/>
-      <c r="G191" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="H191" s="104" t="s">
-        <v>826</v>
+      <c r="G191" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="H191" s="105" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="42" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B192" s="32" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C192" s="82" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D192" s="82" t="s">
-        <v>651</v>
+        <v>97</v>
       </c>
       <c r="E192" s="83" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F192" s="83"/>
-      <c r="G192" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="H192" s="105" t="s">
-        <v>829</v>
+      <c r="G192" s="106" t="s">
+        <v>85</v>
+      </c>
+      <c r="H192" s="106" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="42" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B193" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C193" s="82" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="C193" s="83" t="s">
+        <v>116</v>
       </c>
       <c r="D193" s="82" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E193" s="83" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="F193" s="83"/>
-      <c r="G193" s="106" t="s">
-        <v>85</v>
-      </c>
-      <c r="H193" s="106" t="s">
-        <v>832</v>
+      <c r="G193" s="93" t="s">
+        <v>657</v>
+      </c>
+      <c r="H193" s="93" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="194">
@@ -15806,23 +15806,23 @@
         <v>833</v>
       </c>
       <c r="B194" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C194" s="83" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C194" s="82" t="s">
+        <v>110</v>
       </c>
       <c r="D194" s="82" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E194" s="83" t="s">
         <v>834</v>
       </c>
       <c r="F194" s="83"/>
       <c r="G194" s="93" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="H194" s="93" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="195">
@@ -15830,47 +15830,47 @@
         <v>835</v>
       </c>
       <c r="B195" s="32" t="s">
-        <v>109</v>
+        <v>664</v>
       </c>
       <c r="C195" s="82" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="D195" s="82" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E195" s="83" t="s">
         <v>836</v>
       </c>
       <c r="F195" s="83"/>
-      <c r="G195" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H195" s="93" t="s">
-        <v>664</v>
+      <c r="G195" s="40" t="s">
+        <v>657</v>
+      </c>
+      <c r="H195" s="40" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="42" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B196" s="32" t="s">
-        <v>666</v>
+        <v>122</v>
       </c>
       <c r="C196" s="82" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D196" s="82" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E196" s="83" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F196" s="83"/>
-      <c r="G196" s="40" t="s">
-        <v>659</v>
-      </c>
-      <c r="H196" s="40" t="s">
-        <v>839</v>
+      <c r="G196" s="93" t="s">
+        <v>661</v>
+      </c>
+      <c r="H196" s="93" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="197">
@@ -15878,48 +15878,34 @@
         <v>840</v>
       </c>
       <c r="B197" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C197" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="D197" s="82" t="s">
-        <v>124</v>
-      </c>
-      <c r="E197" s="83" t="s">
         <v>841</v>
       </c>
-      <c r="F197" s="83"/>
-      <c r="G197" s="93" t="s">
-        <v>663</v>
-      </c>
-      <c r="H197" s="93" t="s">
-        <v>671</v>
+      <c r="C197" s="108" t="s">
+        <v>842</v>
+      </c>
+      <c r="D197" s="108" t="s">
+        <v>843</v>
+      </c>
+      <c r="E197" s="109" t="s">
+        <v>844</v>
+      </c>
+      <c r="F197" s="109"/>
+      <c r="G197" s="110" t="s">
+        <v>845</v>
+      </c>
+      <c r="H197" s="110" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="42" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="B198" s="32" t="s">
-        <v>843</v>
-      </c>
-      <c r="C198" s="108" t="s">
-        <v>844</v>
-      </c>
-      <c r="D198" s="108" t="s">
-        <v>845</v>
-      </c>
-      <c r="E198" s="109" t="s">
-        <v>846</v>
-      </c>
-      <c r="F198" s="109"/>
-      <c r="G198" s="110" t="s">
-        <v>847</v>
-      </c>
-      <c r="H198" s="110" t="s">
         <v>848</v>
       </c>
+      <c r="G198" s="28"/>
+      <c r="H198" s="28"/>
     </row>
     <row r="199">
       <c r="A199" s="42" t="s">
@@ -15928,119 +15914,123 @@
       <c r="B199" s="32" t="s">
         <v>850</v>
       </c>
+      <c r="C199" s="111" t="s">
+        <v>462</v>
+      </c>
+      <c r="D199" s="87"/>
+      <c r="E199" s="83" t="s">
+        <v>851</v>
+      </c>
       <c r="G199" s="28"/>
       <c r="H199" s="28"/>
     </row>
     <row r="200">
       <c r="A200" s="42" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B200" s="32" t="s">
-        <v>852</v>
-      </c>
-      <c r="C200" s="111" t="s">
-        <v>462</v>
-      </c>
-      <c r="D200" s="87"/>
-      <c r="E200" s="83" t="s">
         <v>853</v>
       </c>
-      <c r="G200" s="28"/>
-      <c r="H200" s="28"/>
+      <c r="C200" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D200" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E200" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="G200" s="32" t="s">
+        <v>856</v>
+      </c>
+      <c r="H200" s="88" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="42" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="B201" s="32" t="s">
-        <v>855</v>
-      </c>
-      <c r="C201" s="86" t="s">
-        <v>856</v>
-      </c>
-      <c r="D201" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E201" s="22" t="s">
-        <v>408</v>
-      </c>
-      <c r="G201" s="32" t="s">
-        <v>858</v>
-      </c>
-      <c r="H201" s="88" t="s">
+        <v>415</v>
+      </c>
+      <c r="C201" s="112" t="s">
         <v>859</v>
+      </c>
+      <c r="D201" s="112" t="s">
+        <v>860</v>
+      </c>
+      <c r="E201" s="113" t="s">
+        <v>861</v>
+      </c>
+      <c r="F201" s="61"/>
+      <c r="G201" s="114" t="s">
+        <v>862</v>
+      </c>
+      <c r="H201" s="55" t="s">
+        <v>863</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="42" t="s">
+        <v>864</v>
+      </c>
+      <c r="B202" s="32" t="s">
+        <v>865</v>
+      </c>
+      <c r="C202" s="112" t="s">
+        <v>859</v>
+      </c>
+      <c r="D202" s="112" t="s">
         <v>860</v>
       </c>
-      <c r="B202" s="32" t="s">
-        <v>415</v>
-      </c>
-      <c r="C202" s="112" t="s">
-        <v>861</v>
-      </c>
-      <c r="D202" s="112" t="s">
-        <v>862</v>
-      </c>
       <c r="E202" s="113" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="F202" s="61"/>
       <c r="G202" s="114" t="s">
-        <v>864</v>
-      </c>
-      <c r="H202" s="55" t="s">
-        <v>865</v>
+        <v>862</v>
+      </c>
+      <c r="H202" s="115" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="42" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="B203" s="32" t="s">
-        <v>867</v>
-      </c>
-      <c r="C203" s="112" t="s">
-        <v>861</v>
-      </c>
-      <c r="D203" s="112" t="s">
-        <v>862</v>
-      </c>
-      <c r="E203" s="113" t="s">
-        <v>868</v>
-      </c>
-      <c r="F203" s="61"/>
-      <c r="G203" s="114" t="s">
-        <v>864</v>
-      </c>
-      <c r="H203" s="115" t="s">
         <v>869</v>
+      </c>
+      <c r="C203" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D203" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E203" s="83" t="s">
+        <v>870</v>
+      </c>
+      <c r="G203" s="32" t="s">
+        <v>856</v>
+      </c>
+      <c r="H203" s="88" t="s">
+        <v>871</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="42" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="B204" s="32" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="C204" s="86" t="s">
-        <v>856</v>
-      </c>
-      <c r="D204" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E204" s="83" t="s">
-        <v>872</v>
-      </c>
-      <c r="G204" s="32" t="s">
-        <v>858</v>
-      </c>
-      <c r="H204" s="88" t="s">
-        <v>873</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="D204" s="82"/>
+      <c r="E204" s="82"/>
+      <c r="H204" s="28"/>
     </row>
     <row r="205">
       <c r="A205" s="42" t="s">
@@ -16049,256 +16039,256 @@
       <c r="B205" s="32" t="s">
         <v>875</v>
       </c>
-      <c r="C205" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D205" s="82"/>
-      <c r="E205" s="82"/>
-      <c r="H205" s="28"/>
+      <c r="C205" s="82" t="s">
+        <v>854</v>
+      </c>
+      <c r="D205" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E205" s="83" t="s">
+        <v>876</v>
+      </c>
+      <c r="G205" s="32" t="s">
+        <v>856</v>
+      </c>
+      <c r="H205" s="88" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="42" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="B206" s="32" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="C206" s="82" t="s">
+        <v>854</v>
+      </c>
+      <c r="D206" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E206" s="83" t="s">
+        <v>880</v>
+      </c>
+      <c r="G206" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D206" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E206" s="83" t="s">
-        <v>878</v>
-      </c>
-      <c r="G206" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H206" s="88" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="42" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B207" s="32" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="C207" s="82" t="s">
+        <v>854</v>
+      </c>
+      <c r="D207" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E207" s="83" t="s">
+        <v>884</v>
+      </c>
+      <c r="G207" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D207" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E207" s="83" t="s">
-        <v>882</v>
-      </c>
-      <c r="G207" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H207" s="88" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="42" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="B208" s="32" t="s">
-        <v>885</v>
-      </c>
-      <c r="C208" s="82" t="s">
+        <v>887</v>
+      </c>
+      <c r="C208" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D208" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E208" s="83" t="s">
+        <v>888</v>
+      </c>
+      <c r="G208" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D208" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E208" s="83" t="s">
-        <v>886</v>
-      </c>
-      <c r="G208" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H208" s="88" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="42" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="B209" s="32" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C209" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D209" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E209" s="83" t="s">
+        <v>892</v>
+      </c>
+      <c r="G209" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D209" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E209" s="83" t="s">
-        <v>890</v>
-      </c>
-      <c r="G209" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H209" s="88" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="42" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="B210" s="32" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C210" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D210" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E210" s="83" t="s">
+        <v>896</v>
+      </c>
+      <c r="G210" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D210" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E210" s="83" t="s">
-        <v>894</v>
-      </c>
-      <c r="G210" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H210" s="88" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="42" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="B211" s="32" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="C211" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D211" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E211" s="83" t="s">
+        <v>900</v>
+      </c>
+      <c r="G211" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D211" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E211" s="83" t="s">
-        <v>898</v>
-      </c>
-      <c r="G211" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H211" s="88" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="42" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="B212" s="32" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C212" s="86" t="s">
+        <v>854</v>
+      </c>
+      <c r="D212" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E212" s="83" t="s">
+        <v>904</v>
+      </c>
+      <c r="G212" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D212" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E212" s="83" t="s">
-        <v>902</v>
-      </c>
-      <c r="G212" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H212" s="88" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="42" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="B213" s="32" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C213" s="86" t="s">
-        <v>856</v>
-      </c>
-      <c r="D213" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E213" s="83" t="s">
-        <v>906</v>
-      </c>
-      <c r="G213" s="32" t="s">
-        <v>858</v>
-      </c>
-      <c r="H213" s="88" t="s">
-        <v>907</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="D213" s="82"/>
+      <c r="E213" s="82"/>
+      <c r="H213" s="28"/>
     </row>
     <row r="214">
       <c r="A214" s="42" t="s">
         <v>908</v>
       </c>
-      <c r="B214" s="32" t="s">
+      <c r="B214" s="51" t="s">
         <v>909</v>
       </c>
-      <c r="C214" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D214" s="82"/>
-      <c r="E214" s="82"/>
-      <c r="H214" s="28"/>
+      <c r="C214" s="82" t="s">
+        <v>854</v>
+      </c>
+      <c r="D214" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E214" s="83" t="s">
+        <v>910</v>
+      </c>
+      <c r="G214" s="32" t="s">
+        <v>856</v>
+      </c>
+      <c r="H214" s="88" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="42" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="B215" s="51" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="C215" s="82" t="s">
+        <v>854</v>
+      </c>
+      <c r="D215" s="82" t="s">
+        <v>855</v>
+      </c>
+      <c r="E215" s="83" t="s">
+        <v>914</v>
+      </c>
+      <c r="G215" s="32" t="s">
         <v>856</v>
       </c>
-      <c r="D215" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E215" s="83" t="s">
-        <v>912</v>
-      </c>
-      <c r="G215" s="32" t="s">
-        <v>858</v>
-      </c>
       <c r="H215" s="88" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="42" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="B216" s="51" t="s">
-        <v>915</v>
-      </c>
-      <c r="C216" s="82" t="s">
-        <v>856</v>
-      </c>
-      <c r="D216" s="82" t="s">
-        <v>857</v>
-      </c>
-      <c r="E216" s="83" t="s">
-        <v>916</v>
-      </c>
-      <c r="G216" s="32" t="s">
-        <v>858</v>
-      </c>
-      <c r="H216" s="88" t="s">
         <v>917</v>
       </c>
+      <c r="C216" s="86" t="s">
+        <v>462</v>
+      </c>
+      <c r="D216" s="87"/>
+      <c r="E216" s="82"/>
+      <c r="H216" s="28"/>
     </row>
     <row r="217">
       <c r="A217" s="42" t="s">
@@ -16307,33 +16297,33 @@
       <c r="B217" s="51" t="s">
         <v>919</v>
       </c>
-      <c r="C217" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D217" s="87"/>
-      <c r="E217" s="82"/>
-      <c r="H217" s="28"/>
+      <c r="C217" s="116" t="s">
+        <v>580</v>
+      </c>
+      <c r="D217" s="82"/>
+      <c r="E217" s="83" t="s">
+        <v>920</v>
+      </c>
+      <c r="G217" s="34" t="s">
+        <v>856</v>
+      </c>
+      <c r="H217" s="73" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="42" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="B218" s="51" t="s">
-        <v>921</v>
-      </c>
-      <c r="C218" s="116" t="s">
-        <v>582</v>
-      </c>
-      <c r="D218" s="82"/>
-      <c r="E218" s="83" t="s">
-        <v>922</v>
-      </c>
-      <c r="G218" s="34" t="s">
-        <v>858</v>
-      </c>
-      <c r="H218" s="73" t="s">
         <v>923</v>
       </c>
+      <c r="C218" s="86" t="s">
+        <v>462</v>
+      </c>
+      <c r="D218" s="87"/>
+      <c r="E218" s="82"/>
+      <c r="H218" s="28"/>
     </row>
     <row r="219">
       <c r="A219" s="42" t="s">
@@ -16343,34 +16333,25 @@
         <v>925</v>
       </c>
       <c r="C219" s="86" t="s">
-        <v>462</v>
-      </c>
-      <c r="D219" s="87"/>
-      <c r="E219" s="82"/>
-      <c r="H219" s="28"/>
+        <v>926</v>
+      </c>
+      <c r="D219" s="82" t="s">
+        <v>927</v>
+      </c>
+      <c r="E219" s="109" t="s">
+        <v>928</v>
+      </c>
+      <c r="G219" s="32" t="s">
+        <v>929</v>
+      </c>
+      <c r="H219" s="66" t="s">
+        <v>930</v>
+      </c>
     </row>
     <row r="220">
-      <c r="A220" s="42" t="s">
-        <v>926</v>
-      </c>
-      <c r="B220" s="51" t="s">
-        <v>927</v>
-      </c>
-      <c r="C220" s="86" t="s">
-        <v>928</v>
-      </c>
-      <c r="D220" s="82" t="s">
-        <v>929</v>
-      </c>
-      <c r="E220" s="109" t="s">
-        <v>930</v>
-      </c>
-      <c r="G220" s="32" t="s">
-        <v>931</v>
-      </c>
-      <c r="H220" s="66" t="s">
-        <v>932</v>
-      </c>
+      <c r="A220" s="117"/>
+      <c r="G220" s="28"/>
+      <c r="H220" s="28"/>
     </row>
     <row r="221">
       <c r="A221" s="117"/>
@@ -20421,38 +20402,33 @@
       <c r="A1030" s="117"/>
       <c r="G1030" s="28"/>
       <c r="H1030" s="28"/>
-    </row>
-    <row r="1031">
-      <c r="A1031" s="117"/>
-      <c r="G1031" s="28"/>
-      <c r="H1031" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:B220">
+  <conditionalFormatting sqref="A3:B219">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>REGEXMATCH($A3,"^[^.]+$")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:B220">
+  <conditionalFormatting sqref="A3:B219">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>REGEXMATCH($A3,"^[^.]+\.[^.]+$")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:B220">
+  <conditionalFormatting sqref="A3:B219">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>REGEXMATCH($A3,"^[^.]+\.[^.]+\.[^.]+$")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:B220">
+  <conditionalFormatting sqref="A3:B219">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>REGEXMATCH($A3,"^[^.]+\.[^.]+\.[^.]+\.[^.]+$")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:B220">
+  <conditionalFormatting sqref="A3:B219">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>REGEXMATCH($A3,"^[^.]+\.[^.]+\.[^.]+\.[^.]+\.[^.]+$")</formula>
     </cfRule>
@@ -20465,23 +20441,23 @@
     <hyperlink r:id="rId6" ref="H91"/>
     <hyperlink r:id="rId7" ref="H98"/>
     <hyperlink r:id="rId8" ref="H99"/>
-    <hyperlink r:id="rId9" ref="H123"/>
-    <hyperlink r:id="rId10" ref="H124"/>
-    <hyperlink r:id="rId11" ref="H149"/>
-    <hyperlink r:id="rId12" ref="H201"/>
-    <hyperlink r:id="rId13" ref="H203"/>
-    <hyperlink r:id="rId14" ref="H204"/>
-    <hyperlink r:id="rId15" ref="H206"/>
-    <hyperlink r:id="rId16" ref="H207"/>
-    <hyperlink r:id="rId17" ref="H208"/>
-    <hyperlink r:id="rId18" ref="H209"/>
-    <hyperlink r:id="rId19" ref="H210"/>
-    <hyperlink r:id="rId20" ref="H211"/>
-    <hyperlink r:id="rId21" ref="H212"/>
-    <hyperlink r:id="rId22" ref="H213"/>
-    <hyperlink r:id="rId23" ref="H215"/>
-    <hyperlink r:id="rId24" ref="H216"/>
-    <hyperlink r:id="rId25" ref="H218"/>
+    <hyperlink r:id="rId9" ref="H122"/>
+    <hyperlink r:id="rId10" ref="H123"/>
+    <hyperlink r:id="rId11" ref="H148"/>
+    <hyperlink r:id="rId12" ref="H200"/>
+    <hyperlink r:id="rId13" ref="H202"/>
+    <hyperlink r:id="rId14" ref="H203"/>
+    <hyperlink r:id="rId15" ref="H205"/>
+    <hyperlink r:id="rId16" ref="H206"/>
+    <hyperlink r:id="rId17" ref="H207"/>
+    <hyperlink r:id="rId18" ref="H208"/>
+    <hyperlink r:id="rId19" ref="H209"/>
+    <hyperlink r:id="rId20" ref="H210"/>
+    <hyperlink r:id="rId21" ref="H211"/>
+    <hyperlink r:id="rId22" ref="H212"/>
+    <hyperlink r:id="rId23" ref="H214"/>
+    <hyperlink r:id="rId24" ref="H215"/>
+    <hyperlink r:id="rId25" ref="H217"/>
   </hyperlinks>
   <drawing r:id="rId26"/>
   <legacyDrawing r:id="rId27"/>
@@ -20504,36 +20480,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="118" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="119" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="120" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="121" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="8">
@@ -20544,41 +20520,41 @@
     </row>
     <row r="10">
       <c r="A10" s="121" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="121" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="122" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="31"/>
       <c r="B13" s="123" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="124" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="125" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="126" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="17">
@@ -20587,24 +20563,24 @@
     </row>
     <row r="18">
       <c r="A18" s="121" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B19" s="127"/>
     </row>
     <row r="21">
       <c r="A21" s="121" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
   </sheetData>
@@ -20630,57 +20606,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="121" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="69" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="69" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="69" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
   </sheetData>
@@ -20706,53 +20682,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B1" s="128" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="129" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
   </sheetData>
@@ -20794,71 +20770,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="130" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="121" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B2" s="121" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
   </sheetData>
@@ -20885,31 +20861,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="130" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="121" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B2" s="121" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
F03: adding epo:hasEUReceivedTenders & epo:hasReceivedNonEUTenders predicates
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -3944,7 +3944,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:hasEEAReceivedTenders ?</t>
+      <t xml:space="preserve"> epo:hasEUReceivedTenders  ?</t>
     </r>
     <r>
       <rPr>
@@ -3985,7 +3985,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>epo:hasReceivedNonEEATenders ?</t>
+      <t>epo:hasReceivedNonEUTenders ?</t>
     </r>
     <r>
       <rPr>

</xml_diff>

<commit_message>
Fixed minor mistake in the conceptual mapping (added Class Path for field II.2.11.1).
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="1028">
   <si>
     <t>Field</t>
   </si>
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>2.5.0</t>
+    <t>2.5.1</t>
   </si>
   <si>
     <r>
@@ -14239,7 +14239,9 @@
         <v>380</v>
       </c>
       <c r="F84" s="4"/>
-      <c r="G84" s="36"/>
+      <c r="G84" s="36" t="s">
+        <v>378</v>
+      </c>
       <c r="H84" s="52" t="s">
         <v>381</v>
       </c>

</xml_diff>

<commit_message>
Fix for issue #195.
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>2.5.1</t>
+    <t>2.6.0</t>
   </si>
   <si>
     <r>
@@ -5771,7 +5771,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasNutsCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -6053,7 +6053,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasNutsCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -6356,7 +6356,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasNutsCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -16494,7 +16494,7 @@
       </c>
       <c r="F178" s="52"/>
       <c r="G178" s="52" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="H178" s="52" t="s">
         <v>773</v>
@@ -16752,7 +16752,7 @@
       </c>
       <c r="F188" s="52"/>
       <c r="G188" s="50" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="H188" s="50" t="s">
         <v>800</v>
@@ -17034,7 +17034,7 @@
       </c>
       <c r="F199" s="52"/>
       <c r="G199" s="52" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="H199" s="52" t="s">
         <v>834</v>

</xml_diff>

<commit_message>
Updated Conceptual mapping to fix lidation issue for non-awarded lots in notices 019698-2021, 131568-2021 and 148511-2021.
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="1027">
   <si>
     <t>Field</t>
   </si>
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>2.6.1</t>
+    <t>2.6.2</t>
   </si>
   <si>
     <r>
@@ -4223,7 +4223,10 @@
     <t>AWARD_CONTRACT/NO_AWARDED_CONTRACT</t>
   </si>
   <si>
-    <t>?this epo:includesLotAwardOutcome / epo:hasAwardStatus &lt;http://publications.europa.eu/resource/authority/winner-selection-status/clos-nw&gt; .</t>
+    <t>epo:LotAwardOutcome / at-voc:winner-selection-status</t>
+  </si>
+  <si>
+    <t>?this epo:hasAwardStatus &lt;http://publications.europa.eu/resource/authority/winner-selection-status/clos-nw&gt; .</t>
   </si>
   <si>
     <t>V.1</t>
@@ -15282,20 +15285,20 @@
       </c>
       <c r="F126" s="99"/>
       <c r="G126" s="104" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="H126" s="104" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
     </row>
     <row r="127">
       <c r="A127" s="64" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B127" s="39" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C127" s="105" t="s">
         <v>467</v>
@@ -15310,10 +15313,10 @@
     </row>
     <row r="128">
       <c r="A128" s="51" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B128" s="49" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C128" s="105" t="s">
         <v>467</v>
@@ -15322,93 +15325,93 @@
       <c r="E128" s="36"/>
       <c r="F128" s="36"/>
       <c r="G128" s="36" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="H128" s="91" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
     </row>
     <row r="129">
       <c r="A129" s="80" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B129" s="58" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C129" s="62" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D129" s="62" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E129" s="52" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F129" s="52"/>
       <c r="G129" s="36" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H129" s="92" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
     </row>
     <row r="130">
       <c r="A130" s="80" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B130" s="58" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C130" s="62" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D130" s="62" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E130" s="52" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F130" s="52"/>
       <c r="G130" s="4" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H130" s="75" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
     </row>
     <row r="131">
       <c r="A131" s="80" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B131" s="58" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C131" s="106" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D131" s="62"/>
       <c r="E131" s="68" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F131" s="68"/>
       <c r="G131" s="62" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="H131" s="68" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
     </row>
     <row r="132">
       <c r="A132" s="64" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B132" s="39" t="s">
         <v>532</v>
@@ -15426,7 +15429,7 @@
     </row>
     <row r="133">
       <c r="A133" s="80" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B133" s="58"/>
       <c r="C133" s="62"/>
@@ -15435,20 +15438,20 @@
         <v>556</v>
       </c>
       <c r="F133" s="52" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="G133" s="36" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="H133" s="52" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
     </row>
     <row r="134">
       <c r="A134" s="80" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B134" s="107"/>
       <c r="C134" s="62"/>
@@ -15457,49 +15460,49 @@
         <v>556</v>
       </c>
       <c r="F134" s="52" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="G134" s="36" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="H134" s="52" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
     </row>
     <row r="135">
       <c r="A135" s="51" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B135" s="49" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C135" s="62" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D135" s="62" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E135" s="52" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F135" s="52"/>
       <c r="G135" s="4" t="s">
         <v>550</v>
       </c>
       <c r="H135" s="50" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
     </row>
     <row r="136">
       <c r="A136" s="51" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B136" s="49" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C136" s="108"/>
       <c r="D136" s="108"/>
@@ -15508,141 +15511,141 @@
       </c>
       <c r="F136" s="109"/>
       <c r="G136" s="52" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="H136" s="36" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
     </row>
     <row r="137">
       <c r="A137" s="80" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B137" s="58" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C137" s="62" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D137" s="62" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="E137" s="52" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F137" s="52"/>
       <c r="G137" s="36" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H137" s="36" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
     </row>
     <row r="138">
       <c r="A138" s="80" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B138" s="58" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C138" s="62"/>
       <c r="D138" s="62"/>
       <c r="E138" s="52" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F138" s="52"/>
       <c r="G138" s="4" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H138" s="50" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
     </row>
     <row r="139">
       <c r="A139" s="80" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B139" s="58" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C139" s="62"/>
       <c r="D139" s="62"/>
       <c r="E139" s="52" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F139" s="52"/>
       <c r="G139" s="4" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H139" s="50" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
     </row>
     <row r="140">
       <c r="A140" s="80" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B140" s="58" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C140" s="62"/>
       <c r="D140" s="62"/>
       <c r="E140" s="52" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F140" s="52"/>
       <c r="G140" s="4" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H140" s="50" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
     </row>
     <row r="141">
       <c r="A141" s="80" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B141" s="58" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C141" s="36"/>
       <c r="D141" s="62"/>
       <c r="E141" s="52" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F141" s="52"/>
       <c r="G141" s="4" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H141" s="4" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
     </row>
     <row r="142">
       <c r="A142" s="80" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B142" s="58" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C142" s="110" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D142" s="62"/>
       <c r="E142" s="52" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F142" s="81"/>
       <c r="G142" s="36" t="s">
@@ -15656,10 +15659,10 @@
     </row>
     <row r="143">
       <c r="A143" s="51" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B143" s="49" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C143" s="105" t="s">
         <v>467</v>
@@ -15674,7 +15677,7 @@
     </row>
     <row r="144">
       <c r="A144" s="80" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B144" s="58" t="s">
         <v>54</v>
@@ -15686,21 +15689,21 @@
         <v>56</v>
       </c>
       <c r="E144" s="52" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F144" s="52"/>
       <c r="G144" s="44" t="s">
         <v>58</v>
       </c>
       <c r="H144" s="44" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
     </row>
     <row r="145">
       <c r="A145" s="80" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B145" s="58" t="s">
         <v>61</v>
@@ -15712,21 +15715,21 @@
         <v>63</v>
       </c>
       <c r="E145" s="52" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F145" s="52"/>
       <c r="G145" s="46" t="s">
         <v>65</v>
       </c>
       <c r="H145" s="46" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
     </row>
     <row r="146">
       <c r="A146" s="80" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B146" s="58" t="s">
         <v>68</v>
@@ -15738,21 +15741,21 @@
         <v>70</v>
       </c>
       <c r="E146" s="52" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F146" s="52"/>
       <c r="G146" s="4" t="s">
         <v>72</v>
       </c>
       <c r="H146" s="50" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
     </row>
     <row r="147">
       <c r="A147" s="80" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B147" s="58" t="s">
         <v>75</v>
@@ -15764,21 +15767,21 @@
         <v>77</v>
       </c>
       <c r="E147" s="52" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F147" s="52"/>
       <c r="G147" s="4" t="s">
         <v>72</v>
       </c>
       <c r="H147" s="50" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
     </row>
     <row r="148">
       <c r="A148" s="80" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B148" s="58" t="s">
         <v>81</v>
@@ -15790,23 +15793,23 @@
         <v>83</v>
       </c>
       <c r="E148" s="41" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F148" s="41" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G148" s="36" t="s">
         <v>86</v>
       </c>
       <c r="H148" s="52" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
     </row>
     <row r="149">
       <c r="A149" s="80" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B149" s="58" t="s">
         <v>89</v>
@@ -15815,24 +15818,24 @@
         <v>90</v>
       </c>
       <c r="D149" s="62" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E149" s="52" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F149" s="52"/>
       <c r="G149" s="4" t="s">
         <v>93</v>
       </c>
       <c r="H149" s="50" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
     </row>
     <row r="150">
       <c r="A150" s="80" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B150" s="58" t="s">
         <v>96</v>
@@ -15844,21 +15847,21 @@
         <v>98</v>
       </c>
       <c r="E150" s="52" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F150" s="52"/>
       <c r="G150" s="44" t="s">
         <v>100</v>
       </c>
       <c r="H150" s="44" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
     </row>
     <row r="151">
       <c r="A151" s="80" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B151" s="58" t="s">
         <v>116</v>
@@ -15870,21 +15873,21 @@
         <v>118</v>
       </c>
       <c r="E151" s="52" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F151" s="52"/>
       <c r="G151" s="52" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H151" s="92" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
     </row>
     <row r="152">
       <c r="A152" s="80" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B152" s="58" t="s">
         <v>110</v>
@@ -15896,24 +15899,24 @@
         <v>112</v>
       </c>
       <c r="E152" s="52" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F152" s="52"/>
       <c r="G152" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H152" s="92" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
     </row>
     <row r="153">
       <c r="A153" s="80" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B153" s="58" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C153" s="62" t="s">
         <v>132</v>
@@ -15922,21 +15925,21 @@
         <v>133</v>
       </c>
       <c r="E153" s="52" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F153" s="52"/>
       <c r="G153" s="46" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H153" s="46" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
     </row>
     <row r="154">
       <c r="A154" s="80" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B154" s="58" t="s">
         <v>123</v>
@@ -15948,42 +15951,42 @@
         <v>125</v>
       </c>
       <c r="E154" s="52" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="F154" s="52"/>
       <c r="G154" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H154" s="92" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
     </row>
     <row r="155">
       <c r="A155" s="80" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B155" s="58" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C155" s="62" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D155" s="62" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E155" s="52" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="F155" s="41" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="G155" s="41" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="H155" s="111" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
@@ -15994,26 +15997,26 @@
       <c r="C156" s="62"/>
       <c r="D156" s="62"/>
       <c r="E156" s="68" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="F156" s="104" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="G156" s="63" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="H156" s="63" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
     </row>
     <row r="157">
       <c r="A157" s="51" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B157" s="49" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C157" s="105" t="s">
         <v>467</v>
@@ -16028,59 +16031,59 @@
     </row>
     <row r="158">
       <c r="A158" s="80" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B158" s="58" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C158" s="62" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D158" s="62" t="s">
         <v>266</v>
       </c>
       <c r="E158" s="52" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F158" s="52"/>
       <c r="G158" s="36" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="H158" s="52" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
     </row>
     <row r="159">
       <c r="A159" s="80" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B159" s="58" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C159" s="62" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D159" s="62" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="E159" s="52" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="F159" s="52"/>
       <c r="G159" s="36" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H159" s="50" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
     </row>
     <row r="160">
       <c r="A160" s="80" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B160" s="58" t="s">
         <v>271</v>
@@ -16092,45 +16095,45 @@
         <v>273</v>
       </c>
       <c r="E160" s="52" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="F160" s="52"/>
       <c r="G160" s="36" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="H160" s="52" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
     </row>
     <row r="161">
       <c r="A161" s="73" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B161" s="74" t="s">
         <v>283</v>
       </c>
       <c r="C161" s="110" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D161" s="62"/>
       <c r="E161" s="52" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F161" s="52"/>
       <c r="G161" s="36" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="H161" s="52" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
     </row>
     <row r="162">
       <c r="A162" s="80" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B162" s="58" t="s">
         <v>277</v>
@@ -16142,48 +16145,48 @@
         <v>279</v>
       </c>
       <c r="E162" s="52" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="F162" s="52"/>
       <c r="G162" s="36" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="H162" s="52" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="I162" s="7"/>
       <c r="J162" s="7"/>
     </row>
     <row r="163">
       <c r="A163" s="80" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B163" s="58" t="s">
         <v>283</v>
       </c>
       <c r="C163" s="110" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D163" s="62"/>
       <c r="E163" s="68" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F163" s="68"/>
       <c r="G163" s="62" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="H163" s="68" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="I163" s="7"/>
       <c r="J163" s="7"/>
     </row>
     <row r="164">
       <c r="A164" s="51" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B164" s="49" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C164" s="105" t="s">
         <v>467</v>
@@ -16198,36 +16201,36 @@
     </row>
     <row r="165">
       <c r="A165" s="80" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B165" s="58" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C165" s="62" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D165" s="62" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="E165" s="68" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F165" s="68"/>
       <c r="G165" s="68" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="H165" s="112" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
     </row>
     <row r="166">
       <c r="A166" s="80" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B166" s="58" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -16240,112 +16243,112 @@
     </row>
     <row r="167">
       <c r="A167" s="80" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B167" s="58" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C167" s="68" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D167" s="68" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E167" s="52" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F167" s="52"/>
       <c r="G167" s="36" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H167" s="52" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
     </row>
     <row r="168">
       <c r="A168" s="80" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B168" s="58" t="s">
         <v>283</v>
       </c>
       <c r="C168" s="110" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D168" s="62"/>
       <c r="E168" s="113" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F168" s="113"/>
       <c r="G168" s="52" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="H168" s="36" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="I168" s="7"/>
       <c r="J168" s="7"/>
     </row>
     <row r="169">
       <c r="A169" s="80" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B169" s="58" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C169" s="62" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D169" s="62" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="E169" s="113" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F169" s="113"/>
       <c r="G169" s="52" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="H169" s="52" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
     </row>
     <row r="170">
       <c r="A170" s="80" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B170" s="58" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C170" s="62" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D170" s="62" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="E170" s="113" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F170" s="113"/>
       <c r="G170" s="68" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="H170" s="68" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="I170" s="7"/>
       <c r="J170" s="7"/>
     </row>
     <row r="171">
       <c r="A171" s="88" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B171" s="34" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C171" s="7"/>
       <c r="D171" s="4"/>
@@ -16358,7 +16361,7 @@
     </row>
     <row r="172">
       <c r="A172" s="64" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B172" s="39" t="s">
         <v>408</v>
@@ -16370,24 +16373,24 @@
         <v>410</v>
       </c>
       <c r="E172" s="113" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="F172" s="113"/>
       <c r="G172" s="114" t="s">
         <v>221</v>
       </c>
       <c r="H172" s="115" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="I172" s="7"/>
       <c r="J172" s="7"/>
     </row>
     <row r="173">
       <c r="A173" s="64" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B173" s="39" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C173" s="105" t="s">
         <v>467</v>
@@ -16402,31 +16405,31 @@
     </row>
     <row r="174">
       <c r="A174" s="51" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B174" s="49" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C174" s="117" t="s">
         <v>467</v>
       </c>
       <c r="D174" s="7"/>
       <c r="E174" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F174" s="36"/>
       <c r="G174" s="36" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H174" s="36" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="I174" s="7"/>
       <c r="J174" s="7"/>
     </row>
     <row r="175">
       <c r="A175" s="80" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B175" s="58" t="s">
         <v>54</v>
@@ -16438,21 +16441,21 @@
         <v>56</v>
       </c>
       <c r="E175" s="52" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F175" s="52"/>
       <c r="G175" s="50" t="s">
         <v>58</v>
       </c>
       <c r="H175" s="50" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="I175" s="7"/>
       <c r="J175" s="7"/>
     </row>
     <row r="176">
       <c r="A176" s="80" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B176" s="58" t="s">
         <v>68</v>
@@ -16464,21 +16467,21 @@
         <v>70</v>
       </c>
       <c r="E176" s="52" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="F176" s="52"/>
       <c r="G176" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H176" s="50" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="I176" s="7"/>
       <c r="J176" s="7"/>
     </row>
     <row r="177">
       <c r="A177" s="80" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B177" s="58" t="s">
         <v>75</v>
@@ -16490,21 +16493,21 @@
         <v>77</v>
       </c>
       <c r="E177" s="52" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F177" s="52"/>
       <c r="G177" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H177" s="50" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="I177" s="7"/>
       <c r="J177" s="7"/>
     </row>
     <row r="178">
       <c r="A178" s="80" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B178" s="58" t="s">
         <v>89</v>
@@ -16513,24 +16516,24 @@
         <v>90</v>
       </c>
       <c r="D178" s="62" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E178" s="52" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F178" s="52"/>
       <c r="G178" s="50" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="H178" s="50" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="I178" s="7"/>
       <c r="J178" s="7"/>
     </row>
     <row r="179">
       <c r="A179" s="80" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B179" s="58" t="s">
         <v>96</v>
@@ -16542,21 +16545,21 @@
         <v>98</v>
       </c>
       <c r="E179" s="52" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="F179" s="52"/>
       <c r="G179" s="52" t="s">
         <v>100</v>
       </c>
       <c r="H179" s="52" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="I179" s="7"/>
       <c r="J179" s="7"/>
     </row>
     <row r="180">
       <c r="A180" s="80" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B180" s="58" t="s">
         <v>116</v>
@@ -16568,21 +16571,21 @@
         <v>118</v>
       </c>
       <c r="E180" s="52" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="F180" s="52"/>
       <c r="G180" s="52" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H180" s="52" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I180" s="7"/>
       <c r="J180" s="7"/>
     </row>
     <row r="181">
       <c r="A181" s="80" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B181" s="58" t="s">
         <v>110</v>
@@ -16594,24 +16597,24 @@
         <v>112</v>
       </c>
       <c r="E181" s="52" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F181" s="52"/>
       <c r="G181" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H181" s="52" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="I181" s="7"/>
       <c r="J181" s="7"/>
     </row>
     <row r="182">
       <c r="A182" s="80" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B182" s="58" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C182" s="62" t="s">
         <v>132</v>
@@ -16620,21 +16623,21 @@
         <v>133</v>
       </c>
       <c r="E182" s="52" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="F182" s="52"/>
       <c r="G182" s="46" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H182" s="46" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="I182" s="7"/>
       <c r="J182" s="7"/>
     </row>
     <row r="183">
       <c r="A183" s="80" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B183" s="58" t="s">
         <v>123</v>
@@ -16646,45 +16649,45 @@
         <v>125</v>
       </c>
       <c r="E183" s="52" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F183" s="68"/>
       <c r="G183" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H183" s="52" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I183" s="7"/>
       <c r="J183" s="7"/>
     </row>
     <row r="184">
       <c r="A184" s="51" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B184" s="49" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C184" s="117" t="s">
         <v>467</v>
       </c>
       <c r="D184" s="118"/>
       <c r="E184" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F184" s="36"/>
       <c r="G184" s="36" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="H184" s="36" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="I184" s="7"/>
       <c r="J184" s="7"/>
     </row>
     <row r="185">
       <c r="A185" s="80" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B185" s="58" t="s">
         <v>54</v>
@@ -16696,21 +16699,21 @@
         <v>56</v>
       </c>
       <c r="E185" s="52" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F185" s="52"/>
       <c r="G185" s="50" t="s">
         <v>58</v>
       </c>
       <c r="H185" s="50" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="I185" s="7"/>
       <c r="J185" s="7"/>
     </row>
     <row r="186">
       <c r="A186" s="80" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B186" s="58" t="s">
         <v>68</v>
@@ -16722,21 +16725,21 @@
         <v>70</v>
       </c>
       <c r="E186" s="52" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="F186" s="52"/>
       <c r="G186" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H186" s="50" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="I186" s="7"/>
       <c r="J186" s="7"/>
     </row>
     <row r="187">
       <c r="A187" s="80" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B187" s="58" t="s">
         <v>75</v>
@@ -16748,21 +16751,21 @@
         <v>77</v>
       </c>
       <c r="E187" s="52" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F187" s="52"/>
       <c r="G187" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H187" s="50" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="I187" s="7"/>
       <c r="J187" s="7"/>
     </row>
     <row r="188">
       <c r="A188" s="80" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B188" s="58" t="s">
         <v>89</v>
@@ -16771,24 +16774,24 @@
         <v>90</v>
       </c>
       <c r="D188" s="62" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E188" s="52" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F188" s="52"/>
       <c r="G188" s="50" t="s">
         <v>93</v>
       </c>
       <c r="H188" s="50" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="I188" s="7"/>
       <c r="J188" s="7"/>
     </row>
     <row r="189">
       <c r="A189" s="80" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B189" s="58" t="s">
         <v>96</v>
@@ -16800,21 +16803,21 @@
         <v>98</v>
       </c>
       <c r="E189" s="52" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="F189" s="52"/>
       <c r="G189" s="50" t="s">
         <v>100</v>
       </c>
       <c r="H189" s="50" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="I189" s="7"/>
       <c r="J189" s="7"/>
     </row>
     <row r="190">
       <c r="A190" s="80" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B190" s="58" t="s">
         <v>116</v>
@@ -16826,21 +16829,21 @@
         <v>118</v>
       </c>
       <c r="E190" s="52" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="F190" s="52"/>
       <c r="G190" s="52" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H190" s="52" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I190" s="7"/>
       <c r="J190" s="7"/>
     </row>
     <row r="191">
       <c r="A191" s="80" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B191" s="58" t="s">
         <v>110</v>
@@ -16852,24 +16855,24 @@
         <v>112</v>
       </c>
       <c r="E191" s="52" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="F191" s="52"/>
       <c r="G191" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H191" s="52" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
     </row>
     <row r="192">
       <c r="A192" s="80" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B192" s="58" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C192" s="62" t="s">
         <v>132</v>
@@ -16878,21 +16881,21 @@
         <v>133</v>
       </c>
       <c r="E192" s="52" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="F192" s="52"/>
       <c r="G192" s="46" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H192" s="46" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="I192" s="7"/>
       <c r="J192" s="7"/>
     </row>
     <row r="193">
       <c r="A193" s="80" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B193" s="58" t="s">
         <v>123</v>
@@ -16904,69 +16907,69 @@
         <v>125</v>
       </c>
       <c r="E193" s="52" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="F193" s="52"/>
       <c r="G193" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H193" s="52" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I193" s="7"/>
       <c r="J193" s="7"/>
     </row>
     <row r="194">
       <c r="A194" s="51" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B194" s="49" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C194" s="62" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="D194" s="62" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E194" s="52" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="F194" s="62"/>
       <c r="G194" s="119" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="H194" s="120" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
     </row>
     <row r="195">
       <c r="A195" s="51" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B195" s="49" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C195" s="7"/>
       <c r="D195" s="7"/>
       <c r="E195" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F195" s="36"/>
       <c r="G195" s="36" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="H195" s="36" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="I195" s="7"/>
       <c r="J195" s="7"/>
     </row>
     <row r="196">
       <c r="A196" s="80" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B196" s="58" t="s">
         <v>54</v>
@@ -16978,21 +16981,21 @@
         <v>56</v>
       </c>
       <c r="E196" s="52" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="F196" s="52"/>
       <c r="G196" s="50" t="s">
         <v>58</v>
       </c>
       <c r="H196" s="50" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
     </row>
     <row r="197">
       <c r="A197" s="80" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B197" s="58" t="s">
         <v>68</v>
@@ -17004,21 +17007,21 @@
         <v>70</v>
       </c>
       <c r="E197" s="52" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="F197" s="52"/>
       <c r="G197" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H197" s="50" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
     </row>
     <row r="198">
       <c r="A198" s="80" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B198" s="58" t="s">
         <v>75</v>
@@ -17030,21 +17033,21 @@
         <v>77</v>
       </c>
       <c r="E198" s="52" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F198" s="52"/>
       <c r="G198" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H198" s="50" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="I198" s="7"/>
       <c r="J198" s="7"/>
     </row>
     <row r="199">
       <c r="A199" s="80" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B199" s="58" t="s">
         <v>89</v>
@@ -17053,24 +17056,24 @@
         <v>90</v>
       </c>
       <c r="D199" s="62" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E199" s="52" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="F199" s="52"/>
       <c r="G199" s="50" t="s">
         <v>93</v>
       </c>
       <c r="H199" s="50" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
     </row>
     <row r="200">
       <c r="A200" s="80" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B200" s="58" t="s">
         <v>96</v>
@@ -17082,21 +17085,21 @@
         <v>98</v>
       </c>
       <c r="E200" s="52" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="F200" s="52"/>
       <c r="G200" s="52" t="s">
         <v>100</v>
       </c>
       <c r="H200" s="52" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="I200" s="7"/>
       <c r="J200" s="7"/>
     </row>
     <row r="201">
       <c r="A201" s="80" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B201" s="58" t="s">
         <v>116</v>
@@ -17108,21 +17111,21 @@
         <v>118</v>
       </c>
       <c r="E201" s="52" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F201" s="52"/>
       <c r="G201" s="52" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H201" s="52" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I201" s="7"/>
       <c r="J201" s="7"/>
     </row>
     <row r="202">
       <c r="A202" s="80" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B202" s="58" t="s">
         <v>110</v>
@@ -17134,24 +17137,24 @@
         <v>112</v>
       </c>
       <c r="E202" s="52" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F202" s="52"/>
       <c r="G202" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H202" s="52" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="I202" s="7"/>
       <c r="J202" s="7"/>
     </row>
     <row r="203">
       <c r="A203" s="80" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B203" s="58" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C203" s="62" t="s">
         <v>132</v>
@@ -17160,21 +17163,21 @@
         <v>133</v>
       </c>
       <c r="E203" s="52" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="F203" s="52"/>
       <c r="G203" s="46" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H203" s="46" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="I203" s="7"/>
       <c r="J203" s="7"/>
     </row>
     <row r="204">
       <c r="A204" s="80" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B204" s="58" t="s">
         <v>123</v>
@@ -17186,50 +17189,50 @@
         <v>125</v>
       </c>
       <c r="E204" s="52" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F204" s="52"/>
       <c r="G204" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H204" s="52" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I204" s="7"/>
       <c r="J204" s="7"/>
     </row>
     <row r="205">
       <c r="A205" s="64" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B205" s="39" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C205" s="122" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D205" s="122" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E205" s="123" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="F205" s="123"/>
       <c r="G205" s="124" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="H205" s="124" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
     </row>
     <row r="206">
       <c r="A206" s="88" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B206" s="34" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C206" s="125"/>
       <c r="D206" s="7"/>
@@ -17242,17 +17245,17 @@
     </row>
     <row r="207">
       <c r="A207" s="64" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B207" s="126" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C207" s="127" t="s">
         <v>467</v>
       </c>
       <c r="D207" s="62"/>
       <c r="E207" s="52" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="F207" s="4"/>
       <c r="G207" s="4"/>
@@ -17262,16 +17265,16 @@
     </row>
     <row r="208">
       <c r="A208" s="51" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B208" s="49" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C208" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D208" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E208" s="4"/>
       <c r="F208" s="7"/>
@@ -17282,144 +17285,144 @@
     </row>
     <row r="209">
       <c r="A209" s="80" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B209" s="58" t="s">
         <v>420</v>
       </c>
       <c r="C209" s="62" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D209" s="62" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E209" s="52" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="F209" s="62" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="G209" s="50" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H209" s="75" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="I209" s="7"/>
       <c r="J209" s="7"/>
     </row>
     <row r="210">
       <c r="A210" s="128" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B210" s="78" t="s">
         <v>420</v>
       </c>
       <c r="C210" s="129" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D210" s="129" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E210" s="52" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="F210" s="62"/>
       <c r="G210" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H210" s="75" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="I210" s="7"/>
       <c r="J210" s="7"/>
     </row>
     <row r="211">
       <c r="A211" s="80" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B211" s="58" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C211" s="62" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D211" s="62" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E211" s="68" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="F211" s="62" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="G211" s="81" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H211" s="130" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="I211" s="7"/>
       <c r="J211" s="7"/>
     </row>
     <row r="212">
       <c r="A212" s="128" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B212" s="78" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C212" s="129" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D212" s="129" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E212" s="52" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="F212" s="62"/>
       <c r="G212" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H212" s="75" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
     </row>
     <row r="213">
       <c r="A213" s="51" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B213" s="49" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C213" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D213" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E213" s="52" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="F213" s="7"/>
       <c r="G213" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H213" s="75" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
     </row>
     <row r="214">
       <c r="A214" s="51" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B214" s="49" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C214" s="105" t="s">
         <v>467</v>
@@ -17434,218 +17437,218 @@
     </row>
     <row r="215">
       <c r="A215" s="80" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B215" s="58" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C215" s="62" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D215" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E215" s="52" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="F215" s="7"/>
       <c r="G215" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H215" s="75" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I215" s="7"/>
       <c r="J215" s="7"/>
     </row>
     <row r="216">
       <c r="A216" s="80" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B216" s="58" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C216" s="62" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D216" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E216" s="52" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="F216" s="7"/>
       <c r="G216" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H216" s="75" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="I216" s="7"/>
       <c r="J216" s="7"/>
     </row>
     <row r="217">
       <c r="A217" s="80" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B217" s="58" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C217" s="62" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D217" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E217" s="52" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="F217" s="7"/>
       <c r="G217" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H217" s="75" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="I217" s="7"/>
       <c r="J217" s="7"/>
     </row>
     <row r="218">
       <c r="A218" s="51" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B218" s="49" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C218" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D218" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E218" s="52" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F218" s="7"/>
       <c r="G218" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H218" s="75" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="I218" s="7"/>
       <c r="J218" s="7"/>
     </row>
     <row r="219">
       <c r="A219" s="51" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B219" s="49" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C219" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D219" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E219" s="52" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="F219" s="7"/>
       <c r="G219" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H219" s="75" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="I219" s="7"/>
       <c r="J219" s="7"/>
     </row>
     <row r="220">
       <c r="A220" s="51" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B220" s="49" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C220" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D220" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E220" s="68" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="F220" s="7"/>
       <c r="G220" s="7" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H220" s="130" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
     </row>
     <row r="221">
       <c r="A221" s="51" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B221" s="131" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C221" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D221" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E221" s="52" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="F221" s="7"/>
       <c r="G221" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H221" s="75" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
     </row>
     <row r="222">
       <c r="A222" s="51" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B222" s="131" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C222" s="105" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D222" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E222" s="52" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="F222" s="7"/>
       <c r="G222" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H222" s="75" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="I222" s="7"/>
       <c r="J222" s="7"/>
     </row>
     <row r="223">
       <c r="A223" s="51" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B223" s="131" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C223" s="105" t="s">
         <v>467</v>
@@ -17660,62 +17663,62 @@
     </row>
     <row r="224">
       <c r="A224" s="80" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B224" s="132" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C224" s="62" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D224" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E224" s="52" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="F224" s="7"/>
       <c r="G224" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H224" s="75" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
     </row>
     <row r="225">
       <c r="A225" s="80" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B225" s="132" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C225" s="62" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D225" s="62" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E225" s="68" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="F225" s="7"/>
       <c r="G225" s="7" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H225" s="130" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="I225" s="7"/>
       <c r="J225" s="7"/>
     </row>
     <row r="226">
       <c r="A226" s="64" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B226" s="61" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C226" s="105" t="s">
         <v>467</v>
@@ -17730,34 +17733,34 @@
     </row>
     <row r="227">
       <c r="A227" s="51" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B227" s="131" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C227" s="133" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D227" s="62"/>
       <c r="E227" s="68" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="F227" s="7"/>
       <c r="G227" s="62" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H227" s="134" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I227" s="7"/>
       <c r="J227" s="7"/>
     </row>
     <row r="228">
       <c r="A228" s="64" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B228" s="61" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C228" s="105" t="s">
         <v>467</v>
@@ -17772,26 +17775,26 @@
     </row>
     <row r="229">
       <c r="A229" s="51" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B229" s="131" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C229" s="105" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="D229" s="62" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E229" s="123" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="F229" s="7"/>
       <c r="G229" s="7" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="H229" s="81" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
@@ -18291,38 +18294,38 @@
     </row>
     <row r="2">
       <c r="A2" s="65" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C2" s="68" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="D2" s="68"/>
       <c r="E2" s="50" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="65" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="50" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="4">
@@ -18330,24 +18333,24 @@
         <v>546</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C4" s="68" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D4" s="68" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B5" s="81" t="s">
         <v>553</v>
@@ -18362,7 +18365,7 @@
         <v>559</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="G5" s="137"/>
       <c r="H5" s="137"/>
@@ -18387,20 +18390,20 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C6" s="138" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="50" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="G6" s="137"/>
       <c r="H6" s="137"/>
@@ -18425,22 +18428,22 @@
     </row>
     <row r="7">
       <c r="A7" s="65" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="8">
@@ -22445,36 +22448,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="139" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="140" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="141" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="142" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="8">
@@ -22485,41 +22488,41 @@
     </row>
     <row r="10">
       <c r="A10" s="142" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="142" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B11" s="143" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="144" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="145"/>
       <c r="B13" s="146" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="147" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="148" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="149" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="17">
@@ -22528,24 +22531,24 @@
     </row>
     <row r="18">
       <c r="A18" s="142" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B18" s="150" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B19" s="151"/>
     </row>
     <row r="21">
       <c r="A21" s="142" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B21" s="152" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -22571,57 +22574,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="142" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="153" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="153" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="153" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
   </sheetData>
@@ -22647,53 +22650,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B1" s="154" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="155" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
   </sheetData>
@@ -22737,35 +22740,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="156" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C1" s="156" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="142" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B2" s="142" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="142" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="D2" s="142" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="157" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B3" s="157" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="D3" s="158" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -22774,13 +22777,13 @@
     </row>
     <row r="4">
       <c r="A4" s="157" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B4" s="157" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>1005</v>
-      </c>
-      <c r="B4" s="157" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>1004</v>
       </c>
       <c r="D4" s="21" t="str">
         <f t="shared" si="1"/>
@@ -22789,66 +22792,66 @@
     </row>
     <row r="5">
       <c r="A5" s="143" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B5" s="143" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="143" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B6" s="143" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="D7" s="159" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="D8" s="160" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
     </row>
   </sheetData>
@@ -22878,51 +22881,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="156" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="142" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B2" s="142" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="142" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="D2" s="142" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C5" s="160" t="s">
         <v>1023</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>1024</v>
-      </c>
-      <c r="C5" s="160" t="s">
-        <v>1022</v>
-      </c>
       <c r="D5" s="21" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated output and validation reports for form F03.
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>4.2.1</t>
+    <t>5.1.0</t>
   </si>
   <si>
     <r>
@@ -570,7 +570,7 @@
     <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:AgentInRole (from CL1)</t>
+    <t>epo:Notice / epo:AgentInRole (from CL1)</t>
   </si>
   <si>
     <t>?this epo:refersToRole ?value</t>
@@ -1893,7 +1893,7 @@
     <t>CONTRACTING_BODY/JOINT_PROCUREMENT_INVOLVED</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / xsd:boolean</t>
+    <t>epo:Notice / epo:Procedure / xsd:boolean</t>
   </si>
   <si>
     <r>
@@ -1950,7 +1950,7 @@
     <t>CONTRACTING_BODY/PROCUREMENT_LAW</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / epo:ProcedureSpecificTerm / rdf:langString</t>
+    <t>epo:Notice / epo:Procedure / epo:ProcedureSpecificTerm / rdf:langString</t>
   </si>
   <si>
     <r>
@@ -2001,7 +2001,7 @@
     <t>CONTRACTING_BODY/CENTRAL_PURCHASING</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / epo:ProcedureSpecificTerm / xsd:boolean</t>
+    <t>epo:Notice / epo:Procedure / epo:ProcedureSpecificTerm / xsd:boolean</t>
   </si>
   <si>
     <r>
@@ -2492,7 +2492,7 @@
     <t>OBJECT_CONTRACT</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation</t>
+    <t>epo:Notice / epo:NoticeAwardInformation</t>
   </si>
   <si>
     <t>?this epo:announcesNoticeAwardInformation ?value .</t>
@@ -2513,7 +2513,7 @@
     <t>OBJECT_CONTRACT/VAL_TOTAL</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / xsd:decimal</t>
+    <t>epo:Notice / epo:NoticeAwardInformation / epo:MonetaryValue / xsd:decimal</t>
   </si>
   <si>
     <t>?this epo:announcesNoticeAwardInformation / epo:hasTotalAwardedValue / epo:hasAmountValue ?value .</t>
@@ -2600,7 +2600,7 @@
     <t>OBJECT_CONTRACT/VAL_TOTAL/@CURRENCY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
+    <t>epo:Notice / epo:NoticeAwardInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
   </si>
   <si>
     <r>
@@ -2640,7 +2640,7 @@
     <t>II.2</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Lot</t>
+    <t>epo:Notice / epo:Lot</t>
   </si>
   <si>
     <t>?this epo:refersToLot ?value .</t>
@@ -3972,7 +3972,7 @@
     <t>PROCEDURE/NOTICE_NUMBER_OJ</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Notice /  epo:Identifier / xsd:string</t>
+    <t>epo:Notice / epo:Notice /  epo:Identifier / xsd:string</t>
   </si>
   <si>
     <r>
@@ -4087,7 +4087,7 @@
     <t>if(exists(AWARDED_CONTRACT))</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Contract</t>
+    <t>epo:Notice / epo:Contract</t>
   </si>
   <si>
     <t>?this epo:announcesContract ?value</t>
@@ -5966,7 +5966,7 @@
     <t>COMPLEMENTARY_INFO/ADDRESS_MEDIATION_BODY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Mediator</t>
+    <t>epo:Notice / epo:Mediator</t>
   </si>
   <si>
     <t>VI.4.2.1</t>
@@ -6560,7 +6560,7 @@
     <t>COMPLEMENTARY_INFO/DATE_DISPATCH_NOTICE</t>
   </si>
   <si>
-    <t>epo:ResultNotice</t>
+    <t>epo:Notice</t>
   </si>
   <si>
     <r>
@@ -7368,7 +7368,7 @@
     <t>annex_d1.rml.ttl</t>
   </si>
   <si>
-    <t>result_notice.rml.ttl</t>
+    <t>notice.rml.ttl</t>
   </si>
   <si>
     <t>Informal (if possible to become formal)</t>

</xml_diff>

<commit_message>
Updated CM to version 5.6.0 according to temporary fix for issue #237
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>5.5.0</t>
+    <t>5.6.0</t>
   </si>
   <si>
     <r>
@@ -4442,10 +4442,10 @@
     <t>Information about tenders</t>
   </si>
   <si>
-    <t>epo:SubmissionStatisticalInformation / epo:Lot</t>
-  </si>
-  <si>
-    <t>?this epo:concernsSubmissionsForLot ?value .</t>
+    <t>epo:SubmissionStatisticalInformation / epo:LotAwardOutcome</t>
+  </si>
+  <si>
+    <t>?this epo:summarisesInformationForLotAwardOutcome ?value .</t>
   </si>
   <si>
     <t>V.2.2.1</t>
@@ -17259,7 +17259,7 @@
         <v>820</v>
       </c>
       <c r="F196" s="50"/>
-      <c r="G196" s="118" t="s">
+      <c r="G196" s="40" t="s">
         <v>821</v>
       </c>
       <c r="H196" s="119" t="s">

</xml_diff>

<commit_message>
Updated CMs for all forms (v 6.1.0), to work with previous XSD versions .
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.0.0</t>
+    <t>6.1.0</t>
   </si>
   <si>
     <r>
@@ -2905,7 +2905,8 @@
     <t>Award criteria</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_QUALITY</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_QUALITY
+OBJECT_CONTRACT/OBJECT_DESCR/AC_QUALITY</t>
   </si>
   <si>
     <t xml:space="preserve">epo:Lot / epo:AwardCriterion </t>
@@ -3003,7 +3004,8 @@
     <t>Award Criterion name</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_QUALITY/AC_CRITERION</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_QUALITY/AC_CRITERION
+OBJECT_CONTRACT/OBJECT_DESCR/AC_QUALITY/AC_CRITERION</t>
   </si>
   <si>
     <t>epo:AwardCriterion / rdf:langString</t>
@@ -3024,13 +3026,15 @@
     <t>Award Criterion complicated</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_QUALITY/AC_WEIGHTING</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_QUALITY/AC_WEIGHTING
+OBJECT_CONTRACT/OBJECT_DESCR/AC_QUALITY/AC_WEIGHTING</t>
   </si>
   <si>
     <t>?this cccev:weight ?value .</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_COST</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_COST
+OBJECT_CONTRACT/OBJECT_DESCR/AC_COST</t>
   </si>
   <si>
     <r>
@@ -3107,16 +3111,19 @@
     <t>II.2.5.2.1</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_COST/AC_CRITERION</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_COST/AC_CRITERION
+OBJECT_CONTRACT/OBJECT_DESCR/AC_COST/AC_CRITERION</t>
   </si>
   <si>
     <t>II.2.5.2.2</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_COST/AC_WEIGHTING</t>
-  </si>
-  <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_PRICE</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_COST/AC_WEIGHTING
+OBJECT_CONTRACT/OBJECT_DESCR/AC_COST/AC_WEIGHTING</t>
+  </si>
+  <si>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_PRICE
+OBJECT_CONTRACT/OBJECT_DESCR/AC_PRICE</t>
   </si>
   <si>
     <r>
@@ -3193,7 +3200,8 @@
     <t>II.2.5.3.1</t>
   </si>
   <si>
-    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_PRICE/AC_WEIGHTING</t>
+    <t>OBJECT_CONTRACT/OBJECT_DESCR/AC/AC_PRICE/AC_WEIGHTING
+OBJECT_CONTRACT/OBJECT_DESCR/AC_PRICE/AC_WEIGHTING</t>
   </si>
   <si>
     <t>II.2.11</t>
@@ -4459,7 +4467,7 @@
     <t>?this epo:comprisesTenderAwardOutcome / epo:indicatesAwardOfLotToWinner ?value</t>
   </si>
   <si>
-    <t>Winner is created only if there is a contractor identified through the `AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTORS/CONTRACTOR` or (in earlier versions of XML) `AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR` XPath</t>
+    <t>Winner is created only if there is a contractor identified by the `AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTORS/CONTRACTOR` (or in earlier versions of XML by the `AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTOR`) XPath</t>
   </si>
   <si>
     <t>V.2.1</t>
@@ -4546,7 +4554,8 @@
     <t>Received Submissions Count</t>
   </si>
   <si>
-    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED</t>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED
+AWARD_CONTRACT/AWARDED_CONTRACT/NB_TENDERS_RECEIVED</t>
   </si>
   <si>
     <t xml:space="preserve"> epo:SubmissionStatisticalInformation / xsd:integer</t>
@@ -4561,7 +4570,8 @@
     <t>Number of tenders received from SMEs</t>
   </si>
   <si>
-    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_SME</t>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_SME
+AWARD_CONTRACT/AWARDED_CONTRACT/NB_TENDERS_RECEIVED_SME</t>
   </si>
   <si>
     <t>epo:SubmissionStatisticalInformation / xsd:integer</t>
@@ -4605,7 +4615,8 @@
     <t>Number of tenders received from tenderers from other EU Member States</t>
   </si>
   <si>
-    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_OTHER_EU</t>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_OTHER_EU
+AWARD_CONTRACT/AWARDED_CONTRACT/NB_TENDERS_RECEIVED_OTHER_EU</t>
   </si>
   <si>
     <r>
@@ -4646,7 +4657,8 @@
     <t>Number of tenders received from tenderers from non-EU Member States</t>
   </si>
   <si>
-    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_NON_EU</t>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_NON_EU
+AWARD_CONTRACT/AWARDED_CONTRACT/NB_TENDERS_RECEIVED_NON_EU</t>
   </si>
   <si>
     <r>
@@ -4687,7 +4699,8 @@
     <t>Number of tenders received by electronic means</t>
   </si>
   <si>
-    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_EMEANS</t>
+    <t>AWARD_CONTRACT/AWARDED_CONTRACT/TENDERS/NB_TENDERS_RECEIVED_EMEANS
+AWARD_CONTRACT/AWARDED_CONTRACT/NB_TENDERS_RECEIVED_EMEANS</t>
   </si>
   <si>
     <t>?this epo:hasElectronicTenders ?value .</t>

</xml_diff>

<commit_message>
Updating CM to v.6.2.0, to address issues #200, #327, #328, #329, and various typos (JIRA issue TED-1201).
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="1046">
   <si>
     <t>Field</t>
   </si>
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.1.0</t>
+    <t>6.2.0</t>
   </si>
   <si>
     <r>
@@ -1281,7 +1281,7 @@
     <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY/URL_BUYER</t>
   </si>
   <si>
-    <t>epo:AgentInRole (from CL1) / epo:BuyerProfile / xsd:anyURI</t>
+    <t>epo:AgentInRole (from CL1) / xsd:anyURI</t>
   </si>
   <si>
     <r>
@@ -1304,7 +1304,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:hasBuyerProfile / epo:hasURL ?</t>
+      <t xml:space="preserve"> epo:hasBuyerProfile ?</t>
     </r>
     <r>
       <rPr>
@@ -1868,7 +1868,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:hasBuyerProfile / epo:hasURL ?</t>
+      <t xml:space="preserve"> epo:hasBuyerProfile ?</t>
     </r>
     <r>
       <rPr>
@@ -2198,7 +2198,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:hasMainActivityType ?</t>
+      <t xml:space="preserve"> epo:hasMainActivity ?</t>
     </r>
     <r>
       <rPr>
@@ -2364,7 +2364,7 @@
     <t>epo:Procedure / epo:Purpose / at-voc:cpv (from cpv.json)</t>
   </si>
   <si>
-    <t>?this epo:hasOverallPurpose / epo:hasMainClassification ?value .</t>
+    <t>?this epo:hasPurpose / epo:hasMainClassification ?value .</t>
   </si>
   <si>
     <t>II.1.2.1</t>
@@ -2403,43 +2403,7 @@
     <t>epo:Procedure / epo:Purpose / at-voc:contract-nature (from contract_nature.json)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>?</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>this</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> epo:hasOverallPurpose / epo:hasContractNatureType ?</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> .</t>
-    </r>
+    <t>?this epo:hasPurpose / epo:hasContractNatureType ?value .</t>
   </si>
   <si>
     <t>II.1.4</t>
@@ -4312,31 +4276,7 @@
     <t>epo:Contract / epo:LotAwardOutcome / at-voc:winner-selection-status</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>?this</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> epo:includesLotAwardOutcome / epo:hasAwardStatus   </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>&lt;http://publications.europa.eu/resource/authority/winner-selection-status/selec-w&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> .
-</t>
-    </r>
+    <t>?this epo:resultsFromLotAwardOutcome / epo:hasAwardStatus   &lt;http://publications.europa.eu/resource/authority/winner-selection-status/selec-w&gt; .</t>
   </si>
   <si>
     <t>AWARD_CONTRACT/NO_AWARDED_CONTRACT</t>
@@ -5393,7 +5333,7 @@
 AWARD_CONTRACT/AWARDED_CONTRACT/VAL_RANGE_TOTAL/LOW</t>
   </si>
   <si>
-    <t>epo:SubmissionStatisticalInformation / MonetaryValue / xsd:decimal</t>
+    <t>epo:SubmissionStatisticalInformation / epo:MonetaryValue / xsd:decimal</t>
   </si>
   <si>
     <r>
@@ -5443,7 +5383,7 @@
 AWARD_CONTRACT/AWARDED_CONTRACT/VAL_RANGE_TOTAL/@CURRENCY</t>
   </si>
   <si>
-    <t>epo:SubmissionStatisticalInformation / MonetaryValue / at-voc:currency (from currency.json)</t>
+    <t>epo:SubmissionStatisticalInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
   </si>
   <si>
     <r>
@@ -5625,7 +5565,7 @@
     <t>AWARD_CONTRACT/AWARDED_CONTRACT/VAL_SUBCONTRACTING/@CURRENCY</t>
   </si>
   <si>
-    <t>epo:Tender / epo:SubcontractingEstimate / MonetaryValue /at-voc:currency (from currency.json)</t>
+    <t>epo:Tender / epo:SubcontractingEstimate / epo:MonetaryValue /at-voc:currency (from currency.json)</t>
   </si>
   <si>
     <t>?this epo:foreseesSubcontracting / epo:hasSubcontractingEstimatedValue / epo:hasCurrency ?value .</t>
@@ -5953,9 +5893,6 @@
   </si>
   <si>
     <t>COMPLEMENTARY_INFO/ADDRESS_REVIEW_BODY/POSTAL_CODE</t>
-  </si>
-  <si>
-    <t>epo:AgentInRole (from CL1)  / org:Organizationn (from CL2) / locn:Address / rdf:langString</t>
   </si>
   <si>
     <r>
@@ -7466,9 +7403,6 @@
   </si>
   <si>
     <t>buyer_legal_type.csv</t>
-  </si>
-  <si>
-    <t>award_criterion_type.json</t>
   </si>
   <si>
     <t>legal_basis.json</t>
@@ -13553,7 +13487,7 @@
       <c r="G51" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="H51" s="40" t="s">
+      <c r="H51" s="4" t="s">
         <v>255</v>
       </c>
       <c r="I51" s="7"/>
@@ -17026,10 +16960,10 @@
       </c>
       <c r="F180" s="50"/>
       <c r="G180" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="H180" s="40" t="s">
         <v>778</v>
-      </c>
-      <c r="H180" s="40" t="s">
-        <v>779</v>
       </c>
       <c r="I180" s="7"/>
       <c r="J180" s="7"/>
@@ -17037,7 +16971,7 @@
     </row>
     <row r="181">
       <c r="A181" s="80" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B181" s="56" t="s">
         <v>100</v>
@@ -17049,14 +16983,14 @@
         <v>102</v>
       </c>
       <c r="E181" s="50" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F181" s="50"/>
       <c r="G181" s="50" t="s">
         <v>104</v>
       </c>
       <c r="H181" s="50" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I181" s="7"/>
       <c r="J181" s="7"/>
@@ -17064,7 +16998,7 @@
     </row>
     <row r="182">
       <c r="A182" s="80" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B182" s="56" t="s">
         <v>120</v>
@@ -17076,7 +17010,7 @@
         <v>122</v>
       </c>
       <c r="E182" s="50" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F182" s="50"/>
       <c r="G182" s="50" t="s">
@@ -17091,7 +17025,7 @@
     </row>
     <row r="183">
       <c r="A183" s="80" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B183" s="56" t="s">
         <v>114</v>
@@ -17103,7 +17037,7 @@
         <v>116</v>
       </c>
       <c r="E183" s="50" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F183" s="70"/>
       <c r="G183" s="50" t="s">
@@ -17118,7 +17052,7 @@
     </row>
     <row r="184">
       <c r="A184" s="80" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B184" s="56" t="s">
         <v>668</v>
@@ -17130,14 +17064,14 @@
         <v>137</v>
       </c>
       <c r="E184" s="50" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F184" s="50"/>
       <c r="G184" s="46" t="s">
         <v>661</v>
       </c>
       <c r="H184" s="46" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="I184" s="7"/>
       <c r="J184" s="7"/>
@@ -17145,7 +17079,7 @@
     </row>
     <row r="185">
       <c r="A185" s="80" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B185" s="56" t="s">
         <v>127</v>
@@ -17157,7 +17091,7 @@
         <v>129</v>
       </c>
       <c r="E185" s="50" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F185" s="50"/>
       <c r="G185" s="50" t="s">
@@ -17172,21 +17106,21 @@
     </row>
     <row r="186">
       <c r="A186" s="49" t="s">
+        <v>791</v>
+      </c>
+      <c r="B186" s="48" t="s">
         <v>792</v>
-      </c>
-      <c r="B186" s="48" t="s">
-        <v>793</v>
       </c>
       <c r="C186" s="121" t="s">
         <v>472</v>
       </c>
       <c r="D186" s="123"/>
       <c r="E186" s="40" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F186" s="37"/>
       <c r="G186" s="37" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H186" s="37" t="s">
         <v>766</v>
@@ -17197,7 +17131,7 @@
     </row>
     <row r="187">
       <c r="A187" s="80" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B187" s="56" t="s">
         <v>56</v>
@@ -17209,14 +17143,14 @@
         <v>58</v>
       </c>
       <c r="E187" s="50" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F187" s="50"/>
       <c r="G187" s="40" t="s">
         <v>60</v>
       </c>
       <c r="H187" s="40" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="I187" s="7" t="s">
         <v>62</v>
@@ -17226,7 +17160,7 @@
     </row>
     <row r="188">
       <c r="A188" s="80" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B188" s="56" t="s">
         <v>72</v>
@@ -17238,14 +17172,14 @@
         <v>74</v>
       </c>
       <c r="E188" s="50" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F188" s="50"/>
       <c r="G188" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H188" s="40" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="I188" s="7"/>
       <c r="J188" s="7"/>
@@ -17253,7 +17187,7 @@
     </row>
     <row r="189">
       <c r="A189" s="80" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B189" s="56" t="s">
         <v>79</v>
@@ -17265,14 +17199,14 @@
         <v>81</v>
       </c>
       <c r="E189" s="50" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F189" s="50"/>
       <c r="G189" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H189" s="40" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="I189" s="7"/>
       <c r="J189" s="7"/>
@@ -17280,7 +17214,7 @@
     </row>
     <row r="190">
       <c r="A190" s="80" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B190" s="56" t="s">
         <v>93</v>
@@ -17292,14 +17226,14 @@
         <v>653</v>
       </c>
       <c r="E190" s="50" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F190" s="50"/>
       <c r="G190" s="40" t="s">
         <v>97</v>
       </c>
       <c r="H190" s="40" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I190" s="7"/>
       <c r="J190" s="7"/>
@@ -17307,7 +17241,7 @@
     </row>
     <row r="191">
       <c r="A191" s="80" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B191" s="56" t="s">
         <v>100</v>
@@ -17319,14 +17253,14 @@
         <v>102</v>
       </c>
       <c r="E191" s="50" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F191" s="50"/>
       <c r="G191" s="40" t="s">
         <v>104</v>
       </c>
       <c r="H191" s="40" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
@@ -17334,7 +17268,7 @@
     </row>
     <row r="192">
       <c r="A192" s="80" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B192" s="56" t="s">
         <v>120</v>
@@ -17346,7 +17280,7 @@
         <v>122</v>
       </c>
       <c r="E192" s="50" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F192" s="50"/>
       <c r="G192" s="50" t="s">
@@ -17361,7 +17295,7 @@
     </row>
     <row r="193">
       <c r="A193" s="80" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B193" s="56" t="s">
         <v>114</v>
@@ -17373,7 +17307,7 @@
         <v>116</v>
       </c>
       <c r="E193" s="50" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F193" s="50"/>
       <c r="G193" s="50" t="s">
@@ -17388,7 +17322,7 @@
     </row>
     <row r="194">
       <c r="A194" s="80" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B194" s="56" t="s">
         <v>668</v>
@@ -17400,14 +17334,14 @@
         <v>137</v>
       </c>
       <c r="E194" s="50" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F194" s="70"/>
       <c r="G194" s="46" t="s">
         <v>661</v>
       </c>
       <c r="H194" s="46" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
@@ -17415,7 +17349,7 @@
     </row>
     <row r="195">
       <c r="A195" s="80" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B195" s="56" t="s">
         <v>127</v>
@@ -17427,7 +17361,7 @@
         <v>129</v>
       </c>
       <c r="E195" s="50" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F195" s="50"/>
       <c r="G195" s="50" t="s">
@@ -17442,26 +17376,26 @@
     </row>
     <row r="196">
       <c r="A196" s="49" t="s">
+        <v>819</v>
+      </c>
+      <c r="B196" s="48" t="s">
         <v>820</v>
       </c>
-      <c r="B196" s="48" t="s">
+      <c r="C196" s="63" t="s">
         <v>821</v>
       </c>
-      <c r="C196" s="63" t="s">
+      <c r="D196" s="63" t="s">
         <v>822</v>
       </c>
-      <c r="D196" s="63" t="s">
+      <c r="E196" s="50" t="s">
         <v>823</v>
-      </c>
-      <c r="E196" s="50" t="s">
-        <v>824</v>
       </c>
       <c r="F196" s="50"/>
       <c r="G196" s="40" t="s">
+        <v>824</v>
+      </c>
+      <c r="H196" s="119" t="s">
         <v>825</v>
-      </c>
-      <c r="H196" s="119" t="s">
-        <v>826</v>
       </c>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
@@ -17469,15 +17403,15 @@
     </row>
     <row r="197">
       <c r="A197" s="49" t="s">
+        <v>826</v>
+      </c>
+      <c r="B197" s="48" t="s">
         <v>827</v>
-      </c>
-      <c r="B197" s="48" t="s">
-        <v>828</v>
       </c>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="40" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="F197" s="37"/>
       <c r="G197" s="37" t="s">
@@ -17492,7 +17426,7 @@
     </row>
     <row r="198">
       <c r="A198" s="80" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B198" s="56" t="s">
         <v>56</v>
@@ -17504,14 +17438,14 @@
         <v>58</v>
       </c>
       <c r="E198" s="50" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F198" s="50"/>
       <c r="G198" s="40" t="s">
         <v>60</v>
       </c>
       <c r="H198" s="40" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="I198" s="7" t="s">
         <v>62</v>
@@ -17521,7 +17455,7 @@
     </row>
     <row r="199">
       <c r="A199" s="80" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B199" s="56" t="s">
         <v>72</v>
@@ -17533,14 +17467,14 @@
         <v>74</v>
       </c>
       <c r="E199" s="50" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F199" s="50"/>
       <c r="G199" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H199" s="40" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
@@ -17548,7 +17482,7 @@
     </row>
     <row r="200">
       <c r="A200" s="80" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B200" s="56" t="s">
         <v>79</v>
@@ -17560,14 +17494,14 @@
         <v>81</v>
       </c>
       <c r="E200" s="50" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F200" s="50"/>
       <c r="G200" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H200" s="40" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="I200" s="7"/>
       <c r="J200" s="7"/>
@@ -17575,7 +17509,7 @@
     </row>
     <row r="201">
       <c r="A201" s="80" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B201" s="56" t="s">
         <v>93</v>
@@ -17587,14 +17521,14 @@
         <v>653</v>
       </c>
       <c r="E201" s="50" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F201" s="50"/>
       <c r="G201" s="40" t="s">
         <v>97</v>
       </c>
       <c r="H201" s="40" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="I201" s="7"/>
       <c r="J201" s="7"/>
@@ -17602,7 +17536,7 @@
     </row>
     <row r="202">
       <c r="A202" s="80" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B202" s="56" t="s">
         <v>100</v>
@@ -17614,14 +17548,14 @@
         <v>102</v>
       </c>
       <c r="E202" s="50" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F202" s="50"/>
       <c r="G202" s="50" t="s">
         <v>104</v>
       </c>
       <c r="H202" s="50" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="I202" s="7"/>
       <c r="J202" s="7"/>
@@ -17629,7 +17563,7 @@
     </row>
     <row r="203">
       <c r="A203" s="80" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B203" s="56" t="s">
         <v>120</v>
@@ -17641,7 +17575,7 @@
         <v>122</v>
       </c>
       <c r="E203" s="50" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F203" s="50"/>
       <c r="G203" s="50" t="s">
@@ -17656,7 +17590,7 @@
     </row>
     <row r="204">
       <c r="A204" s="80" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B204" s="56" t="s">
         <v>114</v>
@@ -17668,7 +17602,7 @@
         <v>116</v>
       </c>
       <c r="E204" s="50" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F204" s="50"/>
       <c r="G204" s="50" t="s">
@@ -17683,7 +17617,7 @@
     </row>
     <row r="205">
       <c r="A205" s="80" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B205" s="56" t="s">
         <v>668</v>
@@ -17695,14 +17629,14 @@
         <v>137</v>
       </c>
       <c r="E205" s="70" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F205" s="70"/>
       <c r="G205" s="61" t="s">
         <v>661</v>
       </c>
       <c r="H205" s="61" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
@@ -17710,7 +17644,7 @@
     </row>
     <row r="206">
       <c r="A206" s="80" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B206" s="56" t="s">
         <v>127</v>
@@ -17722,7 +17656,7 @@
         <v>129</v>
       </c>
       <c r="E206" s="50" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F206" s="70"/>
       <c r="G206" s="70" t="s">
@@ -17737,26 +17671,26 @@
     </row>
     <row r="207">
       <c r="A207" s="64" t="s">
+        <v>853</v>
+      </c>
+      <c r="B207" s="39" t="s">
         <v>854</v>
       </c>
-      <c r="B207" s="39" t="s">
+      <c r="C207" s="125" t="s">
         <v>855</v>
       </c>
-      <c r="C207" s="125" t="s">
+      <c r="D207" s="125" t="s">
         <v>856</v>
       </c>
-      <c r="D207" s="125" t="s">
+      <c r="E207" s="126" t="s">
         <v>857</v>
-      </c>
-      <c r="E207" s="126" t="s">
-        <v>858</v>
       </c>
       <c r="F207" s="126"/>
       <c r="G207" s="40" t="s">
+        <v>858</v>
+      </c>
+      <c r="H207" s="127" t="s">
         <v>859</v>
-      </c>
-      <c r="H207" s="127" t="s">
-        <v>860</v>
       </c>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
@@ -17764,10 +17698,10 @@
     </row>
     <row r="208">
       <c r="A208" s="88" t="s">
+        <v>860</v>
+      </c>
+      <c r="B208" s="35" t="s">
         <v>861</v>
-      </c>
-      <c r="B208" s="35" t="s">
-        <v>862</v>
       </c>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
@@ -17781,17 +17715,17 @@
     </row>
     <row r="209">
       <c r="A209" s="64" t="s">
+        <v>862</v>
+      </c>
+      <c r="B209" s="39" t="s">
         <v>863</v>
-      </c>
-      <c r="B209" s="39" t="s">
-        <v>864</v>
       </c>
       <c r="C209" s="104" t="s">
         <v>472</v>
       </c>
       <c r="D209" s="63"/>
       <c r="E209" s="50" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="F209" s="7"/>
       <c r="G209" s="4"/>
@@ -17802,16 +17736,16 @@
     </row>
     <row r="210">
       <c r="A210" s="49" t="s">
+        <v>865</v>
+      </c>
+      <c r="B210" s="48" t="s">
         <v>866</v>
       </c>
-      <c r="B210" s="48" t="s">
+      <c r="C210" s="104" t="s">
         <v>867</v>
       </c>
-      <c r="C210" s="104" t="s">
+      <c r="D210" s="63" t="s">
         <v>868</v>
-      </c>
-      <c r="D210" s="63" t="s">
-        <v>869</v>
       </c>
       <c r="E210" s="40"/>
       <c r="F210" s="7"/>
@@ -17823,26 +17757,26 @@
     </row>
     <row r="211">
       <c r="A211" s="80" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B211" s="56" t="s">
         <v>424</v>
       </c>
       <c r="C211" s="63" t="s">
+        <v>870</v>
+      </c>
+      <c r="D211" s="63" t="s">
         <v>871</v>
       </c>
-      <c r="D211" s="63" t="s">
+      <c r="E211" s="70" t="s">
         <v>872</v>
-      </c>
-      <c r="E211" s="70" t="s">
-        <v>873</v>
       </c>
       <c r="F211" s="63"/>
       <c r="G211" s="66" t="s">
+        <v>873</v>
+      </c>
+      <c r="H211" s="128" t="s">
         <v>874</v>
-      </c>
-      <c r="H211" s="128" t="s">
-        <v>875</v>
       </c>
       <c r="I211" s="7"/>
       <c r="J211" s="7"/>
@@ -17850,26 +17784,26 @@
     </row>
     <row r="212">
       <c r="A212" s="129" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B212" s="78" t="s">
         <v>424</v>
       </c>
       <c r="C212" s="130" t="s">
+        <v>870</v>
+      </c>
+      <c r="D212" s="130" t="s">
         <v>871</v>
       </c>
-      <c r="D212" s="130" t="s">
+      <c r="E212" s="57" t="s">
         <v>872</v>
-      </c>
-      <c r="E212" s="57" t="s">
-        <v>873</v>
       </c>
       <c r="F212" s="63"/>
       <c r="G212" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="H212" s="76" t="s">
         <v>876</v>
-      </c>
-      <c r="H212" s="76" t="s">
-        <v>877</v>
       </c>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
@@ -17877,26 +17811,26 @@
     </row>
     <row r="213">
       <c r="A213" s="80" t="s">
+        <v>877</v>
+      </c>
+      <c r="B213" s="56" t="s">
         <v>878</v>
       </c>
-      <c r="B213" s="56" t="s">
+      <c r="C213" s="63" t="s">
+        <v>870</v>
+      </c>
+      <c r="D213" s="63" t="s">
+        <v>871</v>
+      </c>
+      <c r="E213" s="50" t="s">
         <v>879</v>
-      </c>
-      <c r="C213" s="63" t="s">
-        <v>871</v>
-      </c>
-      <c r="D213" s="63" t="s">
-        <v>872</v>
-      </c>
-      <c r="E213" s="50" t="s">
-        <v>880</v>
       </c>
       <c r="F213" s="63"/>
       <c r="G213" s="40" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H213" s="76" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
@@ -17904,26 +17838,26 @@
     </row>
     <row r="214">
       <c r="A214" s="129" t="s">
+        <v>877</v>
+      </c>
+      <c r="B214" s="78" t="s">
         <v>878</v>
       </c>
-      <c r="B214" s="78" t="s">
+      <c r="C214" s="130" t="s">
+        <v>870</v>
+      </c>
+      <c r="D214" s="130" t="s">
+        <v>871</v>
+      </c>
+      <c r="E214" s="57" t="s">
         <v>879</v>
-      </c>
-      <c r="C214" s="130" t="s">
-        <v>871</v>
-      </c>
-      <c r="D214" s="130" t="s">
-        <v>872</v>
-      </c>
-      <c r="E214" s="57" t="s">
-        <v>880</v>
       </c>
       <c r="F214" s="63"/>
       <c r="G214" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H214" s="76" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
@@ -17931,26 +17865,26 @@
     </row>
     <row r="215">
       <c r="A215" s="49" t="s">
+        <v>882</v>
+      </c>
+      <c r="B215" s="48" t="s">
         <v>883</v>
       </c>
-      <c r="B215" s="48" t="s">
+      <c r="C215" s="104" t="s">
+        <v>867</v>
+      </c>
+      <c r="D215" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E215" s="50" t="s">
         <v>884</v>
-      </c>
-      <c r="C215" s="104" t="s">
-        <v>868</v>
-      </c>
-      <c r="D215" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E215" s="50" t="s">
-        <v>885</v>
       </c>
       <c r="F215" s="7"/>
       <c r="G215" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H215" s="76" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I215" s="7"/>
       <c r="J215" s="7"/>
@@ -17958,10 +17892,10 @@
     </row>
     <row r="216">
       <c r="A216" s="49" t="s">
+        <v>886</v>
+      </c>
+      <c r="B216" s="48" t="s">
         <v>887</v>
-      </c>
-      <c r="B216" s="48" t="s">
-        <v>888</v>
       </c>
       <c r="C216" s="104" t="s">
         <v>472</v>
@@ -17977,26 +17911,26 @@
     </row>
     <row r="217">
       <c r="A217" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="B217" s="56" t="s">
         <v>889</v>
       </c>
-      <c r="B217" s="56" t="s">
+      <c r="C217" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="D217" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E217" s="50" t="s">
         <v>890</v>
-      </c>
-      <c r="C217" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="D217" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E217" s="50" t="s">
-        <v>891</v>
       </c>
       <c r="F217" s="7"/>
       <c r="G217" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H217" s="76" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I217" s="7"/>
       <c r="J217" s="7"/>
@@ -18004,26 +17938,26 @@
     </row>
     <row r="218">
       <c r="A218" s="80" t="s">
+        <v>892</v>
+      </c>
+      <c r="B218" s="56" t="s">
         <v>893</v>
       </c>
-      <c r="B218" s="56" t="s">
+      <c r="C218" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="D218" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E218" s="50" t="s">
         <v>894</v>
-      </c>
-      <c r="C218" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="D218" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E218" s="50" t="s">
-        <v>895</v>
       </c>
       <c r="F218" s="7"/>
       <c r="G218" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H218" s="76" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I218" s="7"/>
       <c r="J218" s="7"/>
@@ -18031,26 +17965,26 @@
     </row>
     <row r="219">
       <c r="A219" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="B219" s="56" t="s">
         <v>897</v>
       </c>
-      <c r="B219" s="56" t="s">
+      <c r="C219" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="D219" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E219" s="50" t="s">
         <v>898</v>
-      </c>
-      <c r="C219" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="D219" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E219" s="50" t="s">
-        <v>899</v>
       </c>
       <c r="F219" s="7"/>
       <c r="G219" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H219" s="76" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I219" s="7"/>
       <c r="J219" s="7"/>
@@ -18058,26 +17992,26 @@
     </row>
     <row r="220">
       <c r="A220" s="49" t="s">
+        <v>900</v>
+      </c>
+      <c r="B220" s="48" t="s">
         <v>901</v>
       </c>
-      <c r="B220" s="48" t="s">
+      <c r="C220" s="104" t="s">
+        <v>867</v>
+      </c>
+      <c r="D220" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E220" s="70" t="s">
         <v>902</v>
-      </c>
-      <c r="C220" s="104" t="s">
-        <v>868</v>
-      </c>
-      <c r="D220" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E220" s="70" t="s">
-        <v>903</v>
       </c>
       <c r="F220" s="7"/>
       <c r="G220" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H220" s="128" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
@@ -18085,26 +18019,26 @@
     </row>
     <row r="221">
       <c r="A221" s="49" t="s">
+        <v>904</v>
+      </c>
+      <c r="B221" s="131" t="s">
         <v>905</v>
       </c>
-      <c r="B221" s="131" t="s">
+      <c r="C221" s="104" t="s">
+        <v>867</v>
+      </c>
+      <c r="D221" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E221" s="50" t="s">
         <v>906</v>
-      </c>
-      <c r="C221" s="104" t="s">
-        <v>868</v>
-      </c>
-      <c r="D221" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E221" s="50" t="s">
-        <v>907</v>
       </c>
       <c r="F221" s="7"/>
       <c r="G221" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H221" s="76" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
@@ -18112,26 +18046,26 @@
     </row>
     <row r="222">
       <c r="A222" s="49" t="s">
+        <v>908</v>
+      </c>
+      <c r="B222" s="131" t="s">
         <v>909</v>
       </c>
-      <c r="B222" s="131" t="s">
+      <c r="C222" s="104" t="s">
+        <v>867</v>
+      </c>
+      <c r="D222" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E222" s="50" t="s">
         <v>910</v>
-      </c>
-      <c r="C222" s="104" t="s">
-        <v>868</v>
-      </c>
-      <c r="D222" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E222" s="50" t="s">
-        <v>911</v>
       </c>
       <c r="F222" s="7"/>
       <c r="G222" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H222" s="76" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I222" s="7"/>
       <c r="J222" s="7"/>
@@ -18139,26 +18073,26 @@
     </row>
     <row r="223">
       <c r="A223" s="49" t="s">
+        <v>912</v>
+      </c>
+      <c r="B223" s="131" t="s">
         <v>913</v>
       </c>
-      <c r="B223" s="131" t="s">
+      <c r="C223" s="104" t="s">
+        <v>867</v>
+      </c>
+      <c r="D223" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E223" s="70" t="s">
         <v>914</v>
-      </c>
-      <c r="C223" s="104" t="s">
-        <v>868</v>
-      </c>
-      <c r="D223" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E223" s="70" t="s">
-        <v>915</v>
       </c>
       <c r="F223" s="7"/>
       <c r="G223" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H223" s="128" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I223" s="7"/>
       <c r="J223" s="7"/>
@@ -18166,26 +18100,26 @@
     </row>
     <row r="224">
       <c r="A224" s="49" t="s">
+        <v>916</v>
+      </c>
+      <c r="B224" s="131" t="s">
         <v>917</v>
       </c>
-      <c r="B224" s="131" t="s">
+      <c r="C224" s="104" t="s">
+        <v>867</v>
+      </c>
+      <c r="D224" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E224" s="50" t="s">
         <v>918</v>
-      </c>
-      <c r="C224" s="104" t="s">
-        <v>868</v>
-      </c>
-      <c r="D224" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E224" s="50" t="s">
-        <v>919</v>
       </c>
       <c r="F224" s="7"/>
       <c r="G224" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H224" s="76" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
@@ -18193,10 +18127,10 @@
     </row>
     <row r="225">
       <c r="A225" s="49" t="s">
+        <v>920</v>
+      </c>
+      <c r="B225" s="131" t="s">
         <v>921</v>
-      </c>
-      <c r="B225" s="131" t="s">
-        <v>922</v>
       </c>
       <c r="C225" s="104" t="s">
         <v>472</v>
@@ -18212,26 +18146,26 @@
     </row>
     <row r="226">
       <c r="A226" s="80" t="s">
+        <v>922</v>
+      </c>
+      <c r="B226" s="132" t="s">
         <v>923</v>
       </c>
-      <c r="B226" s="132" t="s">
+      <c r="C226" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="D226" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E226" s="70" t="s">
         <v>924</v>
-      </c>
-      <c r="C226" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="D226" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E226" s="70" t="s">
-        <v>925</v>
       </c>
       <c r="F226" s="7"/>
       <c r="G226" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H226" s="128" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="I226" s="7"/>
       <c r="J226" s="7"/>
@@ -18239,26 +18173,26 @@
     </row>
     <row r="227">
       <c r="A227" s="80" t="s">
+        <v>926</v>
+      </c>
+      <c r="B227" s="132" t="s">
         <v>927</v>
       </c>
-      <c r="B227" s="132" t="s">
+      <c r="C227" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="D227" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="E227" s="70" t="s">
         <v>928</v>
-      </c>
-      <c r="C227" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="D227" s="63" t="s">
-        <v>869</v>
-      </c>
-      <c r="E227" s="70" t="s">
-        <v>929</v>
       </c>
       <c r="F227" s="7"/>
       <c r="G227" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H227" s="128" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="I227" s="7"/>
       <c r="J227" s="7"/>
@@ -18266,10 +18200,10 @@
     </row>
     <row r="228">
       <c r="A228" s="64" t="s">
+        <v>930</v>
+      </c>
+      <c r="B228" s="62" t="s">
         <v>931</v>
-      </c>
-      <c r="B228" s="62" t="s">
-        <v>932</v>
       </c>
       <c r="C228" s="104" t="s">
         <v>472</v>
@@ -18285,24 +18219,24 @@
     </row>
     <row r="229">
       <c r="A229" s="49" t="s">
+        <v>932</v>
+      </c>
+      <c r="B229" s="131" t="s">
         <v>933</v>
-      </c>
-      <c r="B229" s="131" t="s">
-        <v>934</v>
       </c>
       <c r="C229" s="133" t="s">
         <v>583</v>
       </c>
       <c r="D229" s="63"/>
       <c r="E229" s="70" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F229" s="7"/>
       <c r="G229" s="63" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H229" s="134" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
@@ -18310,10 +18244,10 @@
     </row>
     <row r="230">
       <c r="A230" s="64" t="s">
+        <v>936</v>
+      </c>
+      <c r="B230" s="62" t="s">
         <v>937</v>
-      </c>
-      <c r="B230" s="62" t="s">
-        <v>938</v>
       </c>
       <c r="C230" s="104" t="s">
         <v>472</v>
@@ -18329,29 +18263,29 @@
     </row>
     <row r="231">
       <c r="A231" s="49" t="s">
+        <v>938</v>
+      </c>
+      <c r="B231" s="135" t="s">
         <v>939</v>
       </c>
-      <c r="B231" s="135" t="s">
+      <c r="C231" s="104" t="s">
         <v>940</v>
       </c>
-      <c r="C231" s="104" t="s">
+      <c r="D231" s="63" t="s">
         <v>941</v>
       </c>
-      <c r="D231" s="63" t="s">
+      <c r="E231" s="136" t="s">
         <v>942</v>
-      </c>
-      <c r="E231" s="136" t="s">
-        <v>943</v>
       </c>
       <c r="F231" s="7"/>
       <c r="G231" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="H231" s="66" t="s">
         <v>944</v>
       </c>
-      <c r="H231" s="66" t="s">
+      <c r="I231" s="7" t="s">
         <v>945</v>
-      </c>
-      <c r="I231" s="7" t="s">
-        <v>946</v>
       </c>
       <c r="J231" s="7"/>
       <c r="K231" s="7"/>
@@ -18472,38 +18406,38 @@
     </row>
     <row r="2">
       <c r="A2" s="72" t="s">
+        <v>946</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>947</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="C2" s="70" t="s">
         <v>948</v>
-      </c>
-      <c r="C2" s="70" t="s">
-        <v>949</v>
       </c>
       <c r="D2" s="70"/>
       <c r="E2" s="40" t="s">
+        <v>949</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>950</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="72" t="s">
+        <v>946</v>
+      </c>
+      <c r="B3" s="66" t="s">
         <v>947</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="C3" s="70" t="s">
         <v>948</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>949</v>
       </c>
       <c r="D3" s="70"/>
       <c r="E3" s="40" t="s">
+        <v>951</v>
+      </c>
+      <c r="F3" s="40" t="s">
         <v>952</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="4">
@@ -18511,19 +18445,19 @@
         <v>550</v>
       </c>
       <c r="B4" s="66" t="s">
+        <v>953</v>
+      </c>
+      <c r="C4" s="70" t="s">
         <v>954</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="D4" s="70" t="s">
         <v>955</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="E4" s="40" t="s">
         <v>956</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="F4" s="40" t="s">
         <v>957</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="5">
@@ -18543,7 +18477,7 @@
         <v>563</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G5" s="139"/>
       <c r="H5" s="139"/>
@@ -18578,10 +18512,10 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="40" t="s">
+        <v>959</v>
+      </c>
+      <c r="F6" s="40" t="s">
         <v>960</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>961</v>
       </c>
       <c r="G6" s="139"/>
       <c r="H6" s="139"/>
@@ -18618,10 +18552,10 @@
         <v>677</v>
       </c>
       <c r="E7" s="40" t="s">
+        <v>961</v>
+      </c>
+      <c r="F7" s="40" t="s">
         <v>962</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="8">
@@ -22626,36 +22560,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="141" t="s">
+        <v>963</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>964</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="142" t="s">
+        <v>965</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>966</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="143" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="144" t="s">
+        <v>968</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>969</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="8">
@@ -22666,41 +22600,41 @@
     </row>
     <row r="10">
       <c r="A10" s="144" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="144" t="s">
+        <v>972</v>
+      </c>
+      <c r="B11" s="145" t="s">
         <v>973</v>
-      </c>
-      <c r="B11" s="145" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="146" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="147"/>
       <c r="B13" s="148" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="149" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="150" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="151" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="17">
@@ -22709,24 +22643,24 @@
     </row>
     <row r="18">
       <c r="A18" s="144" t="s">
+        <v>979</v>
+      </c>
+      <c r="B18" s="152" t="s">
         <v>980</v>
-      </c>
-      <c r="B18" s="152" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B19" s="153"/>
     </row>
     <row r="21">
       <c r="A21" s="144" t="s">
+        <v>982</v>
+      </c>
+      <c r="B21" s="154" t="s">
         <v>983</v>
-      </c>
-      <c r="B21" s="154" t="s">
-        <v>984</v>
       </c>
     </row>
   </sheetData>
@@ -22752,57 +22686,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="144" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="155" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="155" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="155" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="21" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
   </sheetData>
@@ -22828,53 +22757,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B1" s="156" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="138" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
   </sheetData>
@@ -22918,35 +22847,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="157" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C1" s="157" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1009</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>1012</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1014</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -22955,13 +22884,13 @@
     </row>
     <row r="4">
       <c r="A4" s="40" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D4" s="158" t="str">
         <f t="shared" si="1"/>
@@ -22970,70 +22899,70 @@
     </row>
     <row r="5">
       <c r="A5" s="40" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>1018</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D7" s="159" t="s">
         <v>1021</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D7" s="159" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>1024</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1025</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="160" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B9" s="161" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C9" s="161" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D9" s="161" t="s">
         <v>1027</v>
-      </c>
-      <c r="B9" s="161" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C9" s="161" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D9" s="161" t="s">
-        <v>1029</v>
       </c>
       <c r="E9" s="161"/>
       <c r="F9" s="161"/>
@@ -23060,16 +22989,16 @@
     </row>
     <row r="10">
       <c r="A10" s="160" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B10" s="161" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C10" s="161" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D10" s="161" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E10" s="162"/>
       <c r="F10" s="162"/>
@@ -23096,16 +23025,16 @@
     </row>
     <row r="11">
       <c r="A11" s="160" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B11" s="161" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C11" s="161" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D11" s="161" t="s">
         <v>1032</v>
-      </c>
-      <c r="B11" s="161" t="s">
-        <v>1033</v>
-      </c>
-      <c r="C11" s="161" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D11" s="161" t="s">
-        <v>1034</v>
       </c>
       <c r="E11" s="162"/>
       <c r="F11" s="162"/>
@@ -23132,16 +23061,16 @@
     </row>
     <row r="12">
       <c r="A12" s="160" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B12" s="161" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C12" s="161" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D12" s="161" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="E12" s="162"/>
       <c r="F12" s="162"/>
@@ -23168,16 +23097,16 @@
     </row>
     <row r="13">
       <c r="A13" s="160" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B13" s="160" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C13" s="161" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D13" s="161" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E13" s="162"/>
       <c r="F13" s="162"/>
@@ -23204,16 +23133,16 @@
     </row>
     <row r="14">
       <c r="A14" s="160" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B14" s="160" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C14" s="161" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D14" s="161" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="E14" s="162"/>
       <c r="F14" s="162"/>
@@ -23265,51 +23194,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="163" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="144" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B2" s="144" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C2" s="144" t="s">
         <v>1008</v>
       </c>
-      <c r="B2" s="144" t="s">
+      <c r="D2" s="144" t="s">
         <v>1009</v>
-      </c>
-      <c r="C2" s="144" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D2" s="144" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C5" s="164" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>1045</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C5" s="164" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>1047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated conceptual mappings of all forms (v6.4.0) to fix issue #334.
</commit_message>
<xml_diff>
--- a/mappings/package_F03/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F03/transformation/conceptual_mappings.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="1044">
   <si>
     <t>Field</t>
   </si>
@@ -404,7 +404,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.2.0</t>
+    <t>6.4.0</t>
   </si>
   <si>
     <r>
@@ -737,7 +737,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:thoroughfare ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:thoroughfare ?</t>
     </r>
     <r>
       <rPr>
@@ -791,7 +791,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postName ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postName ?</t>
     </r>
     <r>
       <rPr>
@@ -851,7 +851,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasNutsCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasNutsCode ?</t>
     </r>
     <r>
       <rPr>
@@ -908,7 +908,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postCode ?</t>
     </r>
     <r>
       <rPr>
@@ -965,7 +965,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -1445,7 +1445,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:thoroughfare ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:thoroughfare ?</t>
     </r>
     <r>
       <rPr>
@@ -1487,7 +1487,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postName ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postName ?</t>
     </r>
     <r>
       <rPr>
@@ -1532,7 +1532,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasNutsCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasNutsCode ?</t>
     </r>
     <r>
       <rPr>
@@ -1574,7 +1574,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postCode ?</t>
     </r>
     <r>
       <rPr>
@@ -1616,7 +1616,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -3891,27 +3891,6 @@
   </si>
   <si>
     <t>PROCEDURE/EAUCTION_USED</t>
-  </si>
-  <si>
-    <t>epo:Procedure / epo:EAuctionTechniqueUsage</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>?this</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> epo:usesTechnique ?value .</t>
-    </r>
   </si>
   <si>
     <t>IV.1.8</t>
@@ -4784,7 +4763,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:thoroughfare ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:thoroughfare ?</t>
     </r>
     <r>
       <rPr>
@@ -4830,7 +4809,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postName ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postName ?</t>
     </r>
     <r>
       <rPr>
@@ -4880,7 +4859,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasNutsCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasNutsCode ?</t>
     </r>
     <r>
       <rPr>
@@ -4929,7 +4908,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postCode ?</t>
     </r>
     <r>
       <rPr>
@@ -4975,7 +4954,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -5825,7 +5804,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:thoroughfare ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:thoroughfare ?</t>
     </r>
     <r>
       <rPr>
@@ -5870,7 +5849,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postName ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postName ?</t>
     </r>
     <r>
       <rPr>
@@ -5915,7 +5894,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postCode ?</t>
     </r>
     <r>
       <rPr>
@@ -5960,7 +5939,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -6110,7 +6089,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:thoroughfare ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:thoroughfare ?</t>
     </r>
     <r>
       <rPr>
@@ -6155,7 +6134,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postName ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postName ?</t>
     </r>
     <r>
       <rPr>
@@ -6200,7 +6179,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postCode ?</t>
     </r>
     <r>
       <rPr>
@@ -6245,7 +6224,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -6413,7 +6392,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:thoroughfare ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:thoroughfare ?</t>
     </r>
     <r>
       <rPr>
@@ -6458,7 +6437,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postName ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postName ?</t>
     </r>
     <r>
       <rPr>
@@ -6503,7 +6482,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / locn:postCode ?</t>
     </r>
     <r>
       <rPr>
@@ -6548,7 +6527,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / epo:hasCountryCode ?</t>
+      <t xml:space="preserve"> epo:playedBy / cv:registeredAddress / epo:hasCountryCode ?</t>
     </r>
     <r>
       <rPr>
@@ -15219,38 +15198,34 @@
         <v>493</v>
       </c>
       <c r="F110" s="50"/>
-      <c r="G110" s="37" t="s">
-        <v>494</v>
-      </c>
-      <c r="H110" s="67" t="s">
-        <v>495</v>
-      </c>
+      <c r="G110" s="37"/>
+      <c r="H110" s="50"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
     </row>
     <row r="111">
       <c r="A111" s="49" t="s">
+        <v>494</v>
+      </c>
+      <c r="B111" s="48" t="s">
+        <v>495</v>
+      </c>
+      <c r="C111" s="37" t="s">
         <v>496</v>
       </c>
-      <c r="B111" s="48" t="s">
+      <c r="D111" s="37" t="s">
         <v>497</v>
       </c>
-      <c r="C111" s="37" t="s">
+      <c r="E111" s="50" t="s">
         <v>498</v>
-      </c>
-      <c r="D111" s="37" t="s">
-        <v>499</v>
-      </c>
-      <c r="E111" s="50" t="s">
-        <v>500</v>
       </c>
       <c r="F111" s="50"/>
       <c r="G111" s="37" t="s">
         <v>435</v>
       </c>
       <c r="H111" s="67" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
@@ -15258,26 +15233,26 @@
     </row>
     <row r="112">
       <c r="A112" s="93" t="s">
+        <v>494</v>
+      </c>
+      <c r="B112" s="94" t="s">
+        <v>495</v>
+      </c>
+      <c r="C112" s="95" t="s">
         <v>496</v>
       </c>
-      <c r="B112" s="94" t="s">
+      <c r="D112" s="96" t="s">
         <v>497</v>
       </c>
-      <c r="C112" s="95" t="s">
-        <v>498</v>
-      </c>
-      <c r="D112" s="96" t="s">
-        <v>499</v>
-      </c>
       <c r="E112" s="70" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F112" s="70"/>
       <c r="G112" s="63" t="s">
         <v>435</v>
       </c>
       <c r="H112" s="97" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
@@ -15285,10 +15260,10 @@
     </row>
     <row r="113">
       <c r="A113" s="64" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B113" s="39" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -15302,7 +15277,7 @@
     </row>
     <row r="114">
       <c r="A114" s="49" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B114" s="98"/>
       <c r="C114" s="4"/>
@@ -15311,13 +15286,13 @@
         <v>419</v>
       </c>
       <c r="F114" s="40" t="s">
+        <v>505</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="H114" s="37" t="s">
         <v>507</v>
-      </c>
-      <c r="G114" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="H114" s="37" t="s">
-        <v>509</v>
       </c>
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
@@ -15325,22 +15300,22 @@
     </row>
     <row r="115">
       <c r="A115" s="49" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B115" s="98" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C115" s="37"/>
       <c r="D115" s="37"/>
       <c r="E115" s="50" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F115" s="37"/>
       <c r="G115" s="50" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H115" s="67" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I115" s="7" t="s">
         <v>70</v>
@@ -15350,10 +15325,10 @@
     </row>
     <row r="116">
       <c r="A116" s="49" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B116" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -15367,26 +15342,26 @@
     </row>
     <row r="117">
       <c r="A117" s="80" t="s">
+        <v>515</v>
+      </c>
+      <c r="B117" s="56" t="s">
+        <v>516</v>
+      </c>
+      <c r="C117" s="37" t="s">
         <v>517</v>
       </c>
-      <c r="B117" s="56" t="s">
+      <c r="D117" s="37" t="s">
         <v>518</v>
       </c>
-      <c r="C117" s="37" t="s">
+      <c r="E117" s="50" t="s">
         <v>519</v>
-      </c>
-      <c r="D117" s="37" t="s">
-        <v>520</v>
-      </c>
-      <c r="E117" s="50" t="s">
-        <v>521</v>
       </c>
       <c r="F117" s="50"/>
       <c r="G117" s="37" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H117" s="67" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
@@ -15394,10 +15369,10 @@
     </row>
     <row r="118">
       <c r="A118" s="49" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B118" s="48" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="7"/>
@@ -15411,26 +15386,26 @@
     </row>
     <row r="119">
       <c r="A119" s="80" t="s">
+        <v>524</v>
+      </c>
+      <c r="B119" s="56" t="s">
+        <v>525</v>
+      </c>
+      <c r="C119" s="37" t="s">
         <v>526</v>
       </c>
-      <c r="B119" s="56" t="s">
+      <c r="D119" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="C119" s="37" t="s">
+      <c r="E119" s="50" t="s">
         <v>528</v>
-      </c>
-      <c r="D119" s="37" t="s">
-        <v>529</v>
-      </c>
-      <c r="E119" s="50" t="s">
-        <v>530</v>
       </c>
       <c r="F119" s="50"/>
       <c r="G119" s="37" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H119" s="37" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
@@ -15438,24 +15413,24 @@
     </row>
     <row r="120">
       <c r="A120" s="88" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B120" s="35" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="F120" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="G120" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="F120" s="50" t="s">
+      <c r="H120" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="H120" s="4" t="s">
-        <v>537</v>
       </c>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
@@ -15463,49 +15438,49 @@
     </row>
     <row r="121">
       <c r="A121" s="99" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B121" s="100" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
       <c r="E121" s="57" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F121" s="41" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G121" s="41" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H121" s="102" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
       <c r="K121" s="7" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="99" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B122" s="100" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C122" s="63"/>
       <c r="D122" s="63"/>
       <c r="E122" s="103" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F122" s="37"/>
       <c r="G122" s="37" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H122" s="37" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
@@ -15513,28 +15488,28 @@
     </row>
     <row r="123">
       <c r="A123" s="49" t="s">
+        <v>541</v>
+      </c>
+      <c r="B123" s="48" t="s">
+        <v>542</v>
+      </c>
+      <c r="C123" s="63" t="s">
         <v>543</v>
       </c>
-      <c r="B123" s="48" t="s">
+      <c r="D123" s="63" t="s">
         <v>544</v>
       </c>
-      <c r="C123" s="63" t="s">
+      <c r="E123" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="D123" s="63" t="s">
+      <c r="F123" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="G123" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="E123" s="50" t="s">
+      <c r="H123" s="4" t="s">
         <v>547</v>
-      </c>
-      <c r="F123" s="50" t="s">
-        <v>535</v>
-      </c>
-      <c r="G123" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="H123" s="4" t="s">
-        <v>549</v>
       </c>
       <c r="I123" s="7" t="s">
         <v>70</v>
@@ -15544,28 +15519,28 @@
     </row>
     <row r="124">
       <c r="A124" s="49" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B124" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C124" s="63" t="s">
+        <v>549</v>
+      </c>
+      <c r="D124" s="63" t="s">
+        <v>550</v>
+      </c>
+      <c r="E124" s="50" t="s">
         <v>551</v>
       </c>
-      <c r="D124" s="63" t="s">
+      <c r="F124" s="50" t="s">
+        <v>533</v>
+      </c>
+      <c r="G124" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="E124" s="50" t="s">
+      <c r="H124" s="71" t="s">
         <v>553</v>
-      </c>
-      <c r="F124" s="50" t="s">
-        <v>535</v>
-      </c>
-      <c r="G124" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="H124" s="71" t="s">
-        <v>555</v>
       </c>
       <c r="I124" s="7" t="s">
         <v>62</v>
@@ -15575,26 +15550,26 @@
     </row>
     <row r="125">
       <c r="A125" s="49" t="s">
+        <v>554</v>
+      </c>
+      <c r="B125" s="48" t="s">
+        <v>555</v>
+      </c>
+      <c r="C125" s="63" t="s">
         <v>556</v>
       </c>
-      <c r="B125" s="48" t="s">
+      <c r="D125" s="63" t="s">
         <v>557</v>
       </c>
-      <c r="C125" s="63" t="s">
+      <c r="E125" s="40" t="s">
         <v>558</v>
-      </c>
-      <c r="D125" s="63" t="s">
-        <v>559</v>
-      </c>
-      <c r="E125" s="40" t="s">
-        <v>560</v>
       </c>
       <c r="F125" s="4"/>
       <c r="G125" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H125" s="76" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
@@ -15602,26 +15577,26 @@
     </row>
     <row r="126">
       <c r="A126" s="93" t="s">
+        <v>554</v>
+      </c>
+      <c r="B126" s="94" t="s">
+        <v>555</v>
+      </c>
+      <c r="C126" s="96" t="s">
         <v>556</v>
       </c>
-      <c r="B126" s="94" t="s">
+      <c r="D126" s="96" t="s">
         <v>557</v>
       </c>
-      <c r="C126" s="96" t="s">
-        <v>558</v>
-      </c>
-      <c r="D126" s="96" t="s">
-        <v>559</v>
-      </c>
       <c r="E126" s="66" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F126" s="7"/>
       <c r="G126" s="7" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="H126" s="66" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
@@ -15629,10 +15604,10 @@
     </row>
     <row r="127">
       <c r="A127" s="64" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B127" s="39" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C127" s="104" t="s">
         <v>472</v>
@@ -15648,10 +15623,10 @@
     </row>
     <row r="128">
       <c r="A128" s="49" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B128" s="48" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C128" s="104" t="s">
         <v>472</v>
@@ -15667,26 +15642,26 @@
     </row>
     <row r="129">
       <c r="A129" s="80" t="s">
+        <v>568</v>
+      </c>
+      <c r="B129" s="56" t="s">
+        <v>569</v>
+      </c>
+      <c r="C129" s="63" t="s">
         <v>570</v>
       </c>
-      <c r="B129" s="56" t="s">
+      <c r="D129" s="63" t="s">
         <v>571</v>
       </c>
-      <c r="C129" s="63" t="s">
+      <c r="E129" s="50" t="s">
         <v>572</v>
-      </c>
-      <c r="D129" s="63" t="s">
-        <v>573</v>
-      </c>
-      <c r="E129" s="50" t="s">
-        <v>574</v>
       </c>
       <c r="F129" s="50"/>
       <c r="G129" s="37" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H129" s="91" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
@@ -15694,26 +15669,26 @@
     </row>
     <row r="130">
       <c r="A130" s="80" t="s">
+        <v>575</v>
+      </c>
+      <c r="B130" s="56" t="s">
+        <v>576</v>
+      </c>
+      <c r="C130" s="63" t="s">
+        <v>570</v>
+      </c>
+      <c r="D130" s="63" t="s">
+        <v>571</v>
+      </c>
+      <c r="E130" s="50" t="s">
         <v>577</v>
-      </c>
-      <c r="B130" s="56" t="s">
-        <v>578</v>
-      </c>
-      <c r="C130" s="63" t="s">
-        <v>572</v>
-      </c>
-      <c r="D130" s="63" t="s">
-        <v>573</v>
-      </c>
-      <c r="E130" s="50" t="s">
-        <v>579</v>
       </c>
       <c r="F130" s="50"/>
       <c r="G130" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H130" s="76" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
@@ -15721,24 +15696,24 @@
     </row>
     <row r="131">
       <c r="A131" s="80" t="s">
+        <v>579</v>
+      </c>
+      <c r="B131" s="56" t="s">
+        <v>580</v>
+      </c>
+      <c r="C131" s="105" t="s">
         <v>581</v>
-      </c>
-      <c r="B131" s="56" t="s">
-        <v>582</v>
-      </c>
-      <c r="C131" s="105" t="s">
-        <v>583</v>
       </c>
       <c r="D131" s="63"/>
       <c r="E131" s="106" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F131" s="106"/>
       <c r="G131" s="106" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H131" s="107" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
@@ -15746,10 +15721,10 @@
     </row>
     <row r="132">
       <c r="A132" s="64" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B132" s="39" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C132" s="104" t="s">
         <v>472</v>
@@ -15765,20 +15740,20 @@
     </row>
     <row r="133">
       <c r="A133" s="80" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B133" s="56"/>
       <c r="C133" s="63"/>
       <c r="D133" s="7"/>
       <c r="E133" s="57" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F133" s="50"/>
       <c r="G133" s="37" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H133" s="50" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
@@ -15786,49 +15761,49 @@
     </row>
     <row r="134">
       <c r="A134" s="80" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B134" s="108"/>
       <c r="C134" s="63"/>
       <c r="D134" s="7"/>
       <c r="E134" s="57" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F134" s="50"/>
       <c r="G134" s="37" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H134" s="50" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
       <c r="K134" s="7" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="49" t="s">
+        <v>592</v>
+      </c>
+      <c r="B135" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="C135" s="63" t="s">
         <v>594</v>
       </c>
-      <c r="B135" s="48" t="s">
+      <c r="D135" s="63" t="s">
         <v>595</v>
       </c>
-      <c r="C135" s="63" t="s">
+      <c r="E135" s="50" t="s">
         <v>596</v>
-      </c>
-      <c r="D135" s="63" t="s">
-        <v>597</v>
-      </c>
-      <c r="E135" s="50" t="s">
-        <v>598</v>
       </c>
       <c r="F135" s="50"/>
       <c r="G135" s="40" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H135" s="40" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
@@ -15836,51 +15811,51 @@
     </row>
     <row r="136">
       <c r="A136" s="49" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B136" s="48" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C136" s="109"/>
       <c r="D136" s="109"/>
       <c r="E136" s="57" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F136" s="110"/>
       <c r="G136" s="50" t="s">
+        <v>601</v>
+      </c>
+      <c r="H136" s="37" t="s">
+        <v>602</v>
+      </c>
+      <c r="I136" s="7" t="s">
         <v>603</v>
-      </c>
-      <c r="H136" s="37" t="s">
-        <v>604</v>
-      </c>
-      <c r="I136" s="7" t="s">
-        <v>605</v>
       </c>
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
     </row>
     <row r="137">
       <c r="A137" s="80" t="s">
+        <v>604</v>
+      </c>
+      <c r="B137" s="56" t="s">
+        <v>605</v>
+      </c>
+      <c r="C137" s="63" t="s">
         <v>606</v>
       </c>
-      <c r="B137" s="56" t="s">
+      <c r="D137" s="63" t="s">
         <v>607</v>
       </c>
-      <c r="C137" s="63" t="s">
+      <c r="E137" s="50" t="s">
         <v>608</v>
-      </c>
-      <c r="D137" s="63" t="s">
-        <v>609</v>
-      </c>
-      <c r="E137" s="50" t="s">
-        <v>610</v>
       </c>
       <c r="F137" s="50"/>
       <c r="G137" s="37" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H137" s="37" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
@@ -15888,22 +15863,22 @@
     </row>
     <row r="138">
       <c r="A138" s="80" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B138" s="56" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C138" s="63"/>
       <c r="D138" s="63"/>
       <c r="E138" s="50" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F138" s="50"/>
       <c r="G138" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H138" s="40" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
@@ -15911,22 +15886,22 @@
     </row>
     <row r="139">
       <c r="A139" s="80" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B139" s="56" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C139" s="63"/>
       <c r="D139" s="63"/>
       <c r="E139" s="50" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F139" s="50"/>
       <c r="G139" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H139" s="40" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -15934,22 +15909,22 @@
     </row>
     <row r="140">
       <c r="A140" s="80" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B140" s="56" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C140" s="63"/>
       <c r="D140" s="63"/>
       <c r="E140" s="50" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F140" s="50"/>
       <c r="G140" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H140" s="40" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
@@ -15957,22 +15932,22 @@
     </row>
     <row r="141">
       <c r="A141" s="80" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B141" s="56" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C141" s="37"/>
       <c r="D141" s="63"/>
       <c r="E141" s="50" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F141" s="50"/>
       <c r="G141" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H141" s="4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
@@ -15980,17 +15955,17 @@
     </row>
     <row r="142">
       <c r="A142" s="80" t="s">
+        <v>628</v>
+      </c>
+      <c r="B142" s="56" t="s">
+        <v>629</v>
+      </c>
+      <c r="C142" s="111" t="s">
         <v>630</v>
-      </c>
-      <c r="B142" s="56" t="s">
-        <v>631</v>
-      </c>
-      <c r="C142" s="111" t="s">
-        <v>632</v>
       </c>
       <c r="D142" s="63"/>
       <c r="E142" s="50" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F142" s="66"/>
       <c r="G142" s="37" t="s">
@@ -16005,10 +15980,10 @@
     </row>
     <row r="143">
       <c r="A143" s="49" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B143" s="48" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C143" s="104" t="s">
         <v>472</v>
@@ -16024,7 +15999,7 @@
     </row>
     <row r="144">
       <c r="A144" s="80" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B144" s="56" t="s">
         <v>56</v>
@@ -16036,14 +16011,14 @@
         <v>58</v>
       </c>
       <c r="E144" s="50" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F144" s="50"/>
       <c r="G144" s="44" t="s">
         <v>60</v>
       </c>
       <c r="H144" s="44" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="I144" s="7" t="s">
         <v>62</v>
@@ -16053,7 +16028,7 @@
     </row>
     <row r="145">
       <c r="A145" s="80" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B145" s="56" t="s">
         <v>64</v>
@@ -16065,14 +16040,14 @@
         <v>66</v>
       </c>
       <c r="E145" s="50" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F145" s="50"/>
       <c r="G145" s="46" t="s">
         <v>68</v>
       </c>
       <c r="H145" s="46" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="I145" s="7" t="s">
         <v>70</v>
@@ -16082,7 +16057,7 @@
     </row>
     <row r="146">
       <c r="A146" s="80" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B146" s="56" t="s">
         <v>72</v>
@@ -16094,14 +16069,14 @@
         <v>74</v>
       </c>
       <c r="E146" s="50" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="F146" s="50"/>
       <c r="G146" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H146" s="40" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
@@ -16109,7 +16084,7 @@
     </row>
     <row r="147">
       <c r="A147" s="80" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B147" s="56" t="s">
         <v>79</v>
@@ -16121,14 +16096,14 @@
         <v>81</v>
       </c>
       <c r="E147" s="50" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="F147" s="50"/>
       <c r="G147" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H147" s="40" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
@@ -16136,7 +16111,7 @@
     </row>
     <row r="148">
       <c r="A148" s="80" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B148" s="56" t="s">
         <v>85</v>
@@ -16148,16 +16123,16 @@
         <v>87</v>
       </c>
       <c r="E148" s="40" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F148" s="40" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G148" s="37" t="s">
         <v>90</v>
       </c>
       <c r="H148" s="50" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
@@ -16165,7 +16140,7 @@
     </row>
     <row r="149">
       <c r="A149" s="80" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B149" s="56" t="s">
         <v>93</v>
@@ -16174,17 +16149,17 @@
         <v>94</v>
       </c>
       <c r="D149" s="63" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E149" s="50" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="F149" s="50"/>
       <c r="G149" s="4" t="s">
         <v>97</v>
       </c>
       <c r="H149" s="40" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
@@ -16192,7 +16167,7 @@
     </row>
     <row r="150">
       <c r="A150" s="80" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B150" s="56" t="s">
         <v>100</v>
@@ -16204,14 +16179,14 @@
         <v>102</v>
       </c>
       <c r="E150" s="50" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F150" s="50"/>
       <c r="G150" s="44" t="s">
         <v>104</v>
       </c>
       <c r="H150" s="44" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
@@ -16219,7 +16194,7 @@
     </row>
     <row r="151">
       <c r="A151" s="80" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B151" s="56" t="s">
         <v>120</v>
@@ -16231,14 +16206,14 @@
         <v>122</v>
       </c>
       <c r="E151" s="50" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="F151" s="50"/>
       <c r="G151" s="50" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H151" s="91" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
@@ -16246,7 +16221,7 @@
     </row>
     <row r="152">
       <c r="A152" s="80" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B152" s="56" t="s">
         <v>114</v>
@@ -16258,14 +16233,14 @@
         <v>116</v>
       </c>
       <c r="E152" s="50" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F152" s="50"/>
       <c r="G152" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H152" s="91" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
@@ -16273,10 +16248,10 @@
     </row>
     <row r="153">
       <c r="A153" s="80" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B153" s="56" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C153" s="63" t="s">
         <v>136</v>
@@ -16285,14 +16260,14 @@
         <v>137</v>
       </c>
       <c r="E153" s="50" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F153" s="50"/>
       <c r="G153" s="46" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H153" s="46" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
@@ -16300,7 +16275,7 @@
     </row>
     <row r="154">
       <c r="A154" s="80" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B154" s="56" t="s">
         <v>127</v>
@@ -16312,14 +16287,14 @@
         <v>129</v>
       </c>
       <c r="E154" s="50" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="F154" s="50"/>
       <c r="G154" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H154" s="91" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
@@ -16327,26 +16302,26 @@
     </row>
     <row r="155">
       <c r="A155" s="80" t="s">
+        <v>672</v>
+      </c>
+      <c r="B155" s="56" t="s">
+        <v>673</v>
+      </c>
+      <c r="C155" s="63" t="s">
         <v>674</v>
       </c>
-      <c r="B155" s="56" t="s">
+      <c r="D155" s="63" t="s">
         <v>675</v>
       </c>
-      <c r="C155" s="63" t="s">
+      <c r="E155" s="50" t="s">
         <v>676</v>
-      </c>
-      <c r="D155" s="63" t="s">
-        <v>677</v>
-      </c>
-      <c r="E155" s="50" t="s">
-        <v>678</v>
       </c>
       <c r="F155" s="40"/>
       <c r="G155" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H155" s="112" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
@@ -16358,14 +16333,14 @@
       <c r="C156" s="63"/>
       <c r="D156" s="63"/>
       <c r="E156" s="113" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F156" s="66"/>
       <c r="G156" s="44" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="H156" s="114" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
@@ -16373,10 +16348,10 @@
     </row>
     <row r="157">
       <c r="A157" s="49" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B157" s="48" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C157" s="104" t="s">
         <v>472</v>
@@ -16392,26 +16367,26 @@
     </row>
     <row r="158">
       <c r="A158" s="80" t="s">
+        <v>683</v>
+      </c>
+      <c r="B158" s="56" t="s">
+        <v>684</v>
+      </c>
+      <c r="C158" s="63" t="s">
         <v>685</v>
-      </c>
-      <c r="B158" s="56" t="s">
-        <v>686</v>
-      </c>
-      <c r="C158" s="63" t="s">
-        <v>687</v>
       </c>
       <c r="D158" s="63" t="s">
         <v>271</v>
       </c>
       <c r="E158" s="50" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F158" s="50"/>
       <c r="G158" s="37" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="H158" s="50" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
@@ -16419,24 +16394,24 @@
     </row>
     <row r="159">
       <c r="A159" s="74" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B159" s="75" t="s">
         <v>288</v>
       </c>
       <c r="C159" s="115" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D159" s="63"/>
       <c r="E159" s="50" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F159" s="50"/>
       <c r="G159" s="37" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H159" s="50" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
@@ -16444,26 +16419,26 @@
     </row>
     <row r="160">
       <c r="A160" s="80" t="s">
+        <v>694</v>
+      </c>
+      <c r="B160" s="56" t="s">
+        <v>695</v>
+      </c>
+      <c r="C160" s="63" t="s">
         <v>696</v>
       </c>
-      <c r="B160" s="56" t="s">
+      <c r="D160" s="63" t="s">
         <v>697</v>
       </c>
-      <c r="C160" s="63" t="s">
+      <c r="E160" s="50" t="s">
         <v>698</v>
-      </c>
-      <c r="D160" s="63" t="s">
-        <v>699</v>
-      </c>
-      <c r="E160" s="50" t="s">
-        <v>700</v>
       </c>
       <c r="F160" s="50"/>
       <c r="G160" s="4" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H160" s="40" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
@@ -16471,24 +16446,24 @@
     </row>
     <row r="161">
       <c r="A161" s="74" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B161" s="75" t="s">
         <v>288</v>
       </c>
       <c r="C161" s="115" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D161" s="63"/>
       <c r="E161" s="50" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="F161" s="50"/>
       <c r="G161" s="4" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="H161" s="40" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
@@ -16496,7 +16471,7 @@
     </row>
     <row r="162">
       <c r="A162" s="80" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B162" s="56" t="s">
         <v>276</v>
@@ -16508,14 +16483,14 @@
         <v>278</v>
       </c>
       <c r="E162" s="50" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F162" s="50"/>
       <c r="G162" s="37" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="H162" s="50" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="I162" s="7"/>
       <c r="J162" s="7"/>
@@ -16523,24 +16498,24 @@
     </row>
     <row r="163">
       <c r="A163" s="74" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B163" s="75" t="s">
         <v>288</v>
       </c>
       <c r="C163" s="115" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D163" s="63"/>
       <c r="E163" s="70" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F163" s="70"/>
       <c r="G163" s="63" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H163" s="70" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="I163" s="7"/>
       <c r="J163" s="7"/>
@@ -16548,7 +16523,7 @@
     </row>
     <row r="164">
       <c r="A164" s="80" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B164" s="56" t="s">
         <v>282</v>
@@ -16560,14 +16535,14 @@
         <v>284</v>
       </c>
       <c r="E164" s="50" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F164" s="50"/>
       <c r="G164" s="37" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="H164" s="50" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="I164" s="7"/>
       <c r="J164" s="7"/>
@@ -16575,24 +16550,24 @@
     </row>
     <row r="165">
       <c r="A165" s="74" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B165" s="75" t="s">
         <v>288</v>
       </c>
       <c r="C165" s="115" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D165" s="63"/>
       <c r="E165" s="113" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F165" s="70"/>
       <c r="G165" s="63" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H165" s="70" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
@@ -16600,10 +16575,10 @@
     </row>
     <row r="166">
       <c r="A166" s="49" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B166" s="48" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C166" s="116" t="s">
         <v>472</v>
@@ -16619,26 +16594,26 @@
     </row>
     <row r="167">
       <c r="A167" s="80" t="s">
+        <v>720</v>
+      </c>
+      <c r="B167" s="56" t="s">
+        <v>721</v>
+      </c>
+      <c r="C167" s="63" t="s">
         <v>722</v>
       </c>
-      <c r="B167" s="56" t="s">
+      <c r="D167" s="63" t="s">
         <v>723</v>
       </c>
-      <c r="C167" s="63" t="s">
+      <c r="E167" s="50" t="s">
         <v>724</v>
-      </c>
-      <c r="D167" s="63" t="s">
-        <v>725</v>
-      </c>
-      <c r="E167" s="50" t="s">
-        <v>726</v>
       </c>
       <c r="F167" s="50"/>
       <c r="G167" s="50" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="H167" s="67" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
@@ -16646,10 +16621,10 @@
     </row>
     <row r="168">
       <c r="A168" s="80" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B168" s="56" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
@@ -16663,26 +16638,26 @@
     </row>
     <row r="169">
       <c r="A169" s="80" t="s">
+        <v>729</v>
+      </c>
+      <c r="B169" s="56" t="s">
+        <v>730</v>
+      </c>
+      <c r="C169" s="70" t="s">
         <v>731</v>
       </c>
-      <c r="B169" s="56" t="s">
+      <c r="D169" s="70" t="s">
         <v>732</v>
       </c>
-      <c r="C169" s="70" t="s">
+      <c r="E169" s="117" t="s">
         <v>733</v>
-      </c>
-      <c r="D169" s="70" t="s">
-        <v>734</v>
-      </c>
-      <c r="E169" s="117" t="s">
-        <v>735</v>
       </c>
       <c r="F169" s="117"/>
       <c r="G169" s="37" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H169" s="50" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
@@ -16690,24 +16665,24 @@
     </row>
     <row r="170">
       <c r="A170" s="80" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B170" s="56" t="s">
         <v>288</v>
       </c>
       <c r="C170" s="115" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D170" s="63"/>
       <c r="E170" s="117" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="F170" s="117"/>
       <c r="G170" s="70" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="H170" s="63" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I170" s="7"/>
       <c r="J170" s="7"/>
@@ -16715,26 +16690,26 @@
     </row>
     <row r="171">
       <c r="A171" s="80" t="s">
+        <v>740</v>
+      </c>
+      <c r="B171" s="56" t="s">
+        <v>741</v>
+      </c>
+      <c r="C171" s="63" t="s">
         <v>742</v>
       </c>
-      <c r="B171" s="56" t="s">
+      <c r="D171" s="37" t="s">
         <v>743</v>
       </c>
-      <c r="C171" s="63" t="s">
+      <c r="E171" s="117" t="s">
         <v>744</v>
-      </c>
-      <c r="D171" s="37" t="s">
-        <v>745</v>
-      </c>
-      <c r="E171" s="117" t="s">
-        <v>746</v>
       </c>
       <c r="F171" s="117"/>
       <c r="G171" s="50" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="H171" s="50" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="I171" s="7"/>
       <c r="J171" s="7"/>
@@ -16742,26 +16717,26 @@
     </row>
     <row r="172">
       <c r="A172" s="80" t="s">
+        <v>747</v>
+      </c>
+      <c r="B172" s="56" t="s">
+        <v>748</v>
+      </c>
+      <c r="C172" s="63" t="s">
         <v>749</v>
       </c>
-      <c r="B172" s="56" t="s">
+      <c r="D172" s="63" t="s">
         <v>750</v>
       </c>
-      <c r="C172" s="63" t="s">
+      <c r="E172" s="117" t="s">
         <v>751</v>
-      </c>
-      <c r="D172" s="63" t="s">
-        <v>752</v>
-      </c>
-      <c r="E172" s="117" t="s">
-        <v>753</v>
       </c>
       <c r="F172" s="117"/>
       <c r="G172" s="70" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="H172" s="70" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="I172" s="7" t="s">
         <v>62</v>
@@ -16771,10 +16746,10 @@
     </row>
     <row r="173">
       <c r="A173" s="88" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B173" s="35" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
@@ -16788,7 +16763,7 @@
     </row>
     <row r="174">
       <c r="A174" s="64" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B174" s="39" t="s">
         <v>412</v>
@@ -16800,14 +16775,14 @@
         <v>414</v>
       </c>
       <c r="E174" s="117" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="F174" s="117"/>
       <c r="G174" s="118" t="s">
         <v>227</v>
       </c>
       <c r="H174" s="119" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="I174" s="7" t="s">
         <v>62</v>
@@ -16817,10 +16792,10 @@
     </row>
     <row r="175">
       <c r="A175" s="64" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B175" s="39" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C175" s="104" t="s">
         <v>472</v>
@@ -16836,24 +16811,24 @@
     </row>
     <row r="176">
       <c r="A176" s="49" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B176" s="48" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C176" s="121" t="s">
         <v>472</v>
       </c>
       <c r="D176" s="7"/>
       <c r="E176" s="122" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F176" s="117"/>
       <c r="G176" s="37" t="s">
         <v>53</v>
       </c>
       <c r="H176" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I176" s="7"/>
       <c r="J176" s="7"/>
@@ -16861,7 +16836,7 @@
     </row>
     <row r="177">
       <c r="A177" s="80" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B177" s="56" t="s">
         <v>56</v>
@@ -16873,14 +16848,14 @@
         <v>58</v>
       </c>
       <c r="E177" s="50" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="F177" s="50"/>
       <c r="G177" s="40" t="s">
         <v>60</v>
       </c>
       <c r="H177" s="40" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="I177" s="7" t="s">
         <v>62</v>
@@ -16890,7 +16865,7 @@
     </row>
     <row r="178">
       <c r="A178" s="80" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B178" s="56" t="s">
         <v>72</v>
@@ -16902,14 +16877,14 @@
         <v>74</v>
       </c>
       <c r="E178" s="50" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F178" s="50"/>
       <c r="G178" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H178" s="40" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="I178" s="7"/>
       <c r="J178" s="7"/>
@@ -16917,7 +16892,7 @@
     </row>
     <row r="179">
       <c r="A179" s="80" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B179" s="56" t="s">
         <v>79</v>
@@ -16929,14 +16904,14 @@
         <v>81</v>
       </c>
       <c r="E179" s="50" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F179" s="50"/>
       <c r="G179" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H179" s="40" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="I179" s="7"/>
       <c r="J179" s="7"/>
@@ -16944,7 +16919,7 @@
     </row>
     <row r="180">
       <c r="A180" s="80" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B180" s="56" t="s">
         <v>93</v>
@@ -16953,17 +16928,17 @@
         <v>94</v>
       </c>
       <c r="D180" s="63" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E180" s="50" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F180" s="50"/>
       <c r="G180" s="40" t="s">
         <v>97</v>
       </c>
       <c r="H180" s="40" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="I180" s="7"/>
       <c r="J180" s="7"/>
@@ -16971,7 +16946,7 @@
     </row>
     <row r="181">
       <c r="A181" s="80" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B181" s="56" t="s">
         <v>100</v>
@@ -16983,14 +16958,14 @@
         <v>102</v>
       </c>
       <c r="E181" s="50" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F181" s="50"/>
       <c r="G181" s="50" t="s">
         <v>104</v>
       </c>
       <c r="H181" s="50" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I181" s="7"/>
       <c r="J181" s="7"/>
@@ -16998,7 +16973,7 @@
     </row>
     <row r="182">
       <c r="A182" s="80" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B182" s="56" t="s">
         <v>120</v>
@@ -17010,14 +16985,14 @@
         <v>122</v>
       </c>
       <c r="E182" s="50" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F182" s="50"/>
       <c r="G182" s="50" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H182" s="50" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I182" s="7"/>
       <c r="J182" s="7"/>
@@ -17025,7 +17000,7 @@
     </row>
     <row r="183">
       <c r="A183" s="80" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B183" s="56" t="s">
         <v>114</v>
@@ -17037,14 +17012,14 @@
         <v>116</v>
       </c>
       <c r="E183" s="50" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F183" s="70"/>
       <c r="G183" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H183" s="50" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I183" s="7"/>
       <c r="J183" s="7"/>
@@ -17052,10 +17027,10 @@
     </row>
     <row r="184">
       <c r="A184" s="80" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B184" s="56" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C184" s="63" t="s">
         <v>136</v>
@@ -17064,14 +17039,14 @@
         <v>137</v>
       </c>
       <c r="E184" s="50" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F184" s="50"/>
       <c r="G184" s="46" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H184" s="46" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="I184" s="7"/>
       <c r="J184" s="7"/>
@@ -17079,7 +17054,7 @@
     </row>
     <row r="185">
       <c r="A185" s="80" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B185" s="56" t="s">
         <v>127</v>
@@ -17091,14 +17066,14 @@
         <v>129</v>
       </c>
       <c r="E185" s="50" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="F185" s="50"/>
       <c r="G185" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H185" s="50" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I185" s="7"/>
       <c r="J185" s="7"/>
@@ -17106,24 +17081,24 @@
     </row>
     <row r="186">
       <c r="A186" s="49" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B186" s="48" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C186" s="121" t="s">
         <v>472</v>
       </c>
       <c r="D186" s="123"/>
       <c r="E186" s="40" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F186" s="37"/>
       <c r="G186" s="37" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="H186" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I186" s="7"/>
       <c r="J186" s="7"/>
@@ -17131,7 +17106,7 @@
     </row>
     <row r="187">
       <c r="A187" s="80" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B187" s="56" t="s">
         <v>56</v>
@@ -17143,14 +17118,14 @@
         <v>58</v>
       </c>
       <c r="E187" s="50" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="F187" s="50"/>
       <c r="G187" s="40" t="s">
         <v>60</v>
       </c>
       <c r="H187" s="40" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="I187" s="7" t="s">
         <v>62</v>
@@ -17160,7 +17135,7 @@
     </row>
     <row r="188">
       <c r="A188" s="80" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B188" s="56" t="s">
         <v>72</v>
@@ -17172,14 +17147,14 @@
         <v>74</v>
       </c>
       <c r="E188" s="50" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F188" s="50"/>
       <c r="G188" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H188" s="40" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="I188" s="7"/>
       <c r="J188" s="7"/>
@@ -17187,7 +17162,7 @@
     </row>
     <row r="189">
       <c r="A189" s="80" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B189" s="56" t="s">
         <v>79</v>
@@ -17199,14 +17174,14 @@
         <v>81</v>
       </c>
       <c r="E189" s="50" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F189" s="50"/>
       <c r="G189" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H189" s="40" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="I189" s="7"/>
       <c r="J189" s="7"/>
@@ -17214,7 +17189,7 @@
     </row>
     <row r="190">
       <c r="A190" s="80" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B190" s="56" t="s">
         <v>93</v>
@@ -17223,17 +17198,17 @@
         <v>94</v>
       </c>
       <c r="D190" s="63" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E190" s="50" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F190" s="50"/>
       <c r="G190" s="40" t="s">
         <v>97</v>
       </c>
       <c r="H190" s="40" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="I190" s="7"/>
       <c r="J190" s="7"/>
@@ -17241,7 +17216,7 @@
     </row>
     <row r="191">
       <c r="A191" s="80" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B191" s="56" t="s">
         <v>100</v>
@@ -17253,14 +17228,14 @@
         <v>102</v>
       </c>
       <c r="E191" s="50" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F191" s="50"/>
       <c r="G191" s="40" t="s">
         <v>104</v>
       </c>
       <c r="H191" s="40" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
@@ -17268,7 +17243,7 @@
     </row>
     <row r="192">
       <c r="A192" s="80" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B192" s="56" t="s">
         <v>120</v>
@@ -17280,14 +17255,14 @@
         <v>122</v>
       </c>
       <c r="E192" s="50" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="F192" s="50"/>
       <c r="G192" s="50" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H192" s="50" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I192" s="7"/>
       <c r="J192" s="7"/>
@@ -17295,7 +17270,7 @@
     </row>
     <row r="193">
       <c r="A193" s="80" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B193" s="56" t="s">
         <v>114</v>
@@ -17307,14 +17282,14 @@
         <v>116</v>
       </c>
       <c r="E193" s="50" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F193" s="50"/>
       <c r="G193" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H193" s="50" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I193" s="7"/>
       <c r="J193" s="7"/>
@@ -17322,10 +17297,10 @@
     </row>
     <row r="194">
       <c r="A194" s="80" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B194" s="56" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C194" s="63" t="s">
         <v>136</v>
@@ -17334,14 +17309,14 @@
         <v>137</v>
       </c>
       <c r="E194" s="50" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F194" s="70"/>
       <c r="G194" s="46" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H194" s="46" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
@@ -17349,7 +17324,7 @@
     </row>
     <row r="195">
       <c r="A195" s="80" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B195" s="56" t="s">
         <v>127</v>
@@ -17361,14 +17336,14 @@
         <v>129</v>
       </c>
       <c r="E195" s="50" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F195" s="50"/>
       <c r="G195" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H195" s="50" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I195" s="7"/>
       <c r="J195" s="7"/>
@@ -17376,26 +17351,26 @@
     </row>
     <row r="196">
       <c r="A196" s="49" t="s">
+        <v>817</v>
+      </c>
+      <c r="B196" s="48" t="s">
+        <v>818</v>
+      </c>
+      <c r="C196" s="63" t="s">
         <v>819</v>
       </c>
-      <c r="B196" s="48" t="s">
+      <c r="D196" s="63" t="s">
         <v>820</v>
       </c>
-      <c r="C196" s="63" t="s">
+      <c r="E196" s="50" t="s">
         <v>821</v>
-      </c>
-      <c r="D196" s="63" t="s">
-        <v>822</v>
-      </c>
-      <c r="E196" s="50" t="s">
-        <v>823</v>
       </c>
       <c r="F196" s="50"/>
       <c r="G196" s="40" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H196" s="119" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
@@ -17403,22 +17378,22 @@
     </row>
     <row r="197">
       <c r="A197" s="49" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B197" s="48" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="40" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F197" s="37"/>
       <c r="G197" s="37" t="s">
         <v>53</v>
       </c>
       <c r="H197" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
@@ -17426,7 +17401,7 @@
     </row>
     <row r="198">
       <c r="A198" s="80" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B198" s="56" t="s">
         <v>56</v>
@@ -17438,14 +17413,14 @@
         <v>58</v>
       </c>
       <c r="E198" s="50" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F198" s="50"/>
       <c r="G198" s="40" t="s">
         <v>60</v>
       </c>
       <c r="H198" s="40" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I198" s="7" t="s">
         <v>62</v>
@@ -17455,7 +17430,7 @@
     </row>
     <row r="199">
       <c r="A199" s="80" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B199" s="56" t="s">
         <v>72</v>
@@ -17467,14 +17442,14 @@
         <v>74</v>
       </c>
       <c r="E199" s="50" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F199" s="50"/>
       <c r="G199" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H199" s="40" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
@@ -17482,7 +17457,7 @@
     </row>
     <row r="200">
       <c r="A200" s="80" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B200" s="56" t="s">
         <v>79</v>
@@ -17494,14 +17469,14 @@
         <v>81</v>
       </c>
       <c r="E200" s="50" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F200" s="50"/>
       <c r="G200" s="40" t="s">
         <v>76</v>
       </c>
       <c r="H200" s="40" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="I200" s="7"/>
       <c r="J200" s="7"/>
@@ -17509,7 +17484,7 @@
     </row>
     <row r="201">
       <c r="A201" s="80" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B201" s="56" t="s">
         <v>93</v>
@@ -17518,17 +17493,17 @@
         <v>94</v>
       </c>
       <c r="D201" s="63" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E201" s="50" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F201" s="50"/>
       <c r="G201" s="40" t="s">
         <v>97</v>
       </c>
       <c r="H201" s="40" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="I201" s="7"/>
       <c r="J201" s="7"/>
@@ -17536,7 +17511,7 @@
     </row>
     <row r="202">
       <c r="A202" s="80" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B202" s="56" t="s">
         <v>100</v>
@@ -17548,14 +17523,14 @@
         <v>102</v>
       </c>
       <c r="E202" s="50" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="F202" s="50"/>
       <c r="G202" s="50" t="s">
         <v>104</v>
       </c>
       <c r="H202" s="50" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="I202" s="7"/>
       <c r="J202" s="7"/>
@@ -17563,7 +17538,7 @@
     </row>
     <row r="203">
       <c r="A203" s="80" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B203" s="56" t="s">
         <v>120</v>
@@ -17575,14 +17550,14 @@
         <v>122</v>
       </c>
       <c r="E203" s="50" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="F203" s="50"/>
       <c r="G203" s="50" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H203" s="50" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I203" s="7"/>
       <c r="J203" s="7"/>
@@ -17590,7 +17565,7 @@
     </row>
     <row r="204">
       <c r="A204" s="80" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B204" s="56" t="s">
         <v>114</v>
@@ -17602,14 +17577,14 @@
         <v>116</v>
       </c>
       <c r="E204" s="50" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="F204" s="50"/>
       <c r="G204" s="50" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H204" s="50" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I204" s="7"/>
       <c r="J204" s="7"/>
@@ -17617,10 +17592,10 @@
     </row>
     <row r="205">
       <c r="A205" s="80" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B205" s="56" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C205" s="63" t="s">
         <v>136</v>
@@ -17629,14 +17604,14 @@
         <v>137</v>
       </c>
       <c r="E205" s="70" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="F205" s="70"/>
       <c r="G205" s="61" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H205" s="61" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
@@ -17644,7 +17619,7 @@
     </row>
     <row r="206">
       <c r="A206" s="80" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B206" s="56" t="s">
         <v>127</v>
@@ -17656,14 +17631,14 @@
         <v>129</v>
       </c>
       <c r="E206" s="50" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="F206" s="70"/>
       <c r="G206" s="70" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H206" s="70" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I206" s="7"/>
       <c r="J206" s="7"/>
@@ -17671,26 +17646,26 @@
     </row>
     <row r="207">
       <c r="A207" s="64" t="s">
+        <v>851</v>
+      </c>
+      <c r="B207" s="39" t="s">
+        <v>852</v>
+      </c>
+      <c r="C207" s="125" t="s">
         <v>853</v>
       </c>
-      <c r="B207" s="39" t="s">
+      <c r="D207" s="125" t="s">
         <v>854</v>
       </c>
-      <c r="C207" s="125" t="s">
+      <c r="E207" s="126" t="s">
         <v>855</v>
-      </c>
-      <c r="D207" s="125" t="s">
-        <v>856</v>
-      </c>
-      <c r="E207" s="126" t="s">
-        <v>857</v>
       </c>
       <c r="F207" s="126"/>
       <c r="G207" s="40" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="H207" s="127" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
@@ -17698,10 +17673,10 @@
     </row>
     <row r="208">
       <c r="A208" s="88" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B208" s="35" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
@@ -17715,17 +17690,17 @@
     </row>
     <row r="209">
       <c r="A209" s="64" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B209" s="39" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C209" s="104" t="s">
         <v>472</v>
       </c>
       <c r="D209" s="63"/>
       <c r="E209" s="50" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="F209" s="7"/>
       <c r="G209" s="4"/>
@@ -17736,16 +17711,16 @@
     </row>
     <row r="210">
       <c r="A210" s="49" t="s">
+        <v>863</v>
+      </c>
+      <c r="B210" s="48" t="s">
+        <v>864</v>
+      </c>
+      <c r="C210" s="104" t="s">
         <v>865</v>
       </c>
-      <c r="B210" s="48" t="s">
+      <c r="D210" s="63" t="s">
         <v>866</v>
-      </c>
-      <c r="C210" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D210" s="63" t="s">
-        <v>868</v>
       </c>
       <c r="E210" s="40"/>
       <c r="F210" s="7"/>
@@ -17757,26 +17732,26 @@
     </row>
     <row r="211">
       <c r="A211" s="80" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B211" s="56" t="s">
         <v>424</v>
       </c>
       <c r="C211" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="D211" s="63" t="s">
+        <v>869</v>
+      </c>
+      <c r="E211" s="70" t="s">
         <v>870</v>
-      </c>
-      <c r="D211" s="63" t="s">
-        <v>871</v>
-      </c>
-      <c r="E211" s="70" t="s">
-        <v>872</v>
       </c>
       <c r="F211" s="63"/>
       <c r="G211" s="66" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="H211" s="128" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="I211" s="7"/>
       <c r="J211" s="7"/>
@@ -17784,26 +17759,26 @@
     </row>
     <row r="212">
       <c r="A212" s="129" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B212" s="78" t="s">
         <v>424</v>
       </c>
       <c r="C212" s="130" t="s">
+        <v>868</v>
+      </c>
+      <c r="D212" s="130" t="s">
+        <v>869</v>
+      </c>
+      <c r="E212" s="57" t="s">
         <v>870</v>
-      </c>
-      <c r="D212" s="130" t="s">
-        <v>871</v>
-      </c>
-      <c r="E212" s="57" t="s">
-        <v>872</v>
       </c>
       <c r="F212" s="63"/>
       <c r="G212" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H212" s="76" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
@@ -17811,26 +17786,26 @@
     </row>
     <row r="213">
       <c r="A213" s="80" t="s">
+        <v>875</v>
+      </c>
+      <c r="B213" s="56" t="s">
+        <v>876</v>
+      </c>
+      <c r="C213" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="D213" s="63" t="s">
+        <v>869</v>
+      </c>
+      <c r="E213" s="50" t="s">
         <v>877</v>
-      </c>
-      <c r="B213" s="56" t="s">
-        <v>878</v>
-      </c>
-      <c r="C213" s="63" t="s">
-        <v>870</v>
-      </c>
-      <c r="D213" s="63" t="s">
-        <v>871</v>
-      </c>
-      <c r="E213" s="50" t="s">
-        <v>879</v>
       </c>
       <c r="F213" s="63"/>
       <c r="G213" s="40" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="H213" s="76" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
@@ -17838,26 +17813,26 @@
     </row>
     <row r="214">
       <c r="A214" s="129" t="s">
+        <v>875</v>
+      </c>
+      <c r="B214" s="78" t="s">
+        <v>876</v>
+      </c>
+      <c r="C214" s="130" t="s">
+        <v>868</v>
+      </c>
+      <c r="D214" s="130" t="s">
+        <v>869</v>
+      </c>
+      <c r="E214" s="57" t="s">
         <v>877</v>
-      </c>
-      <c r="B214" s="78" t="s">
-        <v>878</v>
-      </c>
-      <c r="C214" s="130" t="s">
-        <v>870</v>
-      </c>
-      <c r="D214" s="130" t="s">
-        <v>871</v>
-      </c>
-      <c r="E214" s="57" t="s">
-        <v>879</v>
       </c>
       <c r="F214" s="63"/>
       <c r="G214" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H214" s="76" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
@@ -17865,26 +17840,26 @@
     </row>
     <row r="215">
       <c r="A215" s="49" t="s">
+        <v>880</v>
+      </c>
+      <c r="B215" s="48" t="s">
+        <v>881</v>
+      </c>
+      <c r="C215" s="104" t="s">
+        <v>865</v>
+      </c>
+      <c r="D215" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E215" s="50" t="s">
         <v>882</v>
-      </c>
-      <c r="B215" s="48" t="s">
-        <v>883</v>
-      </c>
-      <c r="C215" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D215" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E215" s="50" t="s">
-        <v>884</v>
       </c>
       <c r="F215" s="7"/>
       <c r="G215" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H215" s="76" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="I215" s="7"/>
       <c r="J215" s="7"/>
@@ -17892,10 +17867,10 @@
     </row>
     <row r="216">
       <c r="A216" s="49" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B216" s="48" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C216" s="104" t="s">
         <v>472</v>
@@ -17911,26 +17886,26 @@
     </row>
     <row r="217">
       <c r="A217" s="80" t="s">
+        <v>886</v>
+      </c>
+      <c r="B217" s="56" t="s">
+        <v>887</v>
+      </c>
+      <c r="C217" s="63" t="s">
+        <v>865</v>
+      </c>
+      <c r="D217" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E217" s="50" t="s">
         <v>888</v>
-      </c>
-      <c r="B217" s="56" t="s">
-        <v>889</v>
-      </c>
-      <c r="C217" s="63" t="s">
-        <v>867</v>
-      </c>
-      <c r="D217" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E217" s="50" t="s">
-        <v>890</v>
       </c>
       <c r="F217" s="7"/>
       <c r="G217" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H217" s="76" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="I217" s="7"/>
       <c r="J217" s="7"/>
@@ -17938,26 +17913,26 @@
     </row>
     <row r="218">
       <c r="A218" s="80" t="s">
+        <v>890</v>
+      </c>
+      <c r="B218" s="56" t="s">
+        <v>891</v>
+      </c>
+      <c r="C218" s="63" t="s">
+        <v>865</v>
+      </c>
+      <c r="D218" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E218" s="50" t="s">
         <v>892</v>
-      </c>
-      <c r="B218" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="C218" s="63" t="s">
-        <v>867</v>
-      </c>
-      <c r="D218" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E218" s="50" t="s">
-        <v>894</v>
       </c>
       <c r="F218" s="7"/>
       <c r="G218" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H218" s="76" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="I218" s="7"/>
       <c r="J218" s="7"/>
@@ -17965,26 +17940,26 @@
     </row>
     <row r="219">
       <c r="A219" s="80" t="s">
+        <v>894</v>
+      </c>
+      <c r="B219" s="56" t="s">
+        <v>895</v>
+      </c>
+      <c r="C219" s="63" t="s">
+        <v>865</v>
+      </c>
+      <c r="D219" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E219" s="50" t="s">
         <v>896</v>
-      </c>
-      <c r="B219" s="56" t="s">
-        <v>897</v>
-      </c>
-      <c r="C219" s="63" t="s">
-        <v>867</v>
-      </c>
-      <c r="D219" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E219" s="50" t="s">
-        <v>898</v>
       </c>
       <c r="F219" s="7"/>
       <c r="G219" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H219" s="76" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="I219" s="7"/>
       <c r="J219" s="7"/>
@@ -17992,26 +17967,26 @@
     </row>
     <row r="220">
       <c r="A220" s="49" t="s">
+        <v>898</v>
+      </c>
+      <c r="B220" s="48" t="s">
+        <v>899</v>
+      </c>
+      <c r="C220" s="104" t="s">
+        <v>865</v>
+      </c>
+      <c r="D220" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E220" s="70" t="s">
         <v>900</v>
-      </c>
-      <c r="B220" s="48" t="s">
-        <v>901</v>
-      </c>
-      <c r="C220" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D220" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E220" s="70" t="s">
-        <v>902</v>
       </c>
       <c r="F220" s="7"/>
       <c r="G220" s="7" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H220" s="128" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
@@ -18019,26 +17994,26 @@
     </row>
     <row r="221">
       <c r="A221" s="49" t="s">
+        <v>902</v>
+      </c>
+      <c r="B221" s="131" t="s">
+        <v>903</v>
+      </c>
+      <c r="C221" s="104" t="s">
+        <v>865</v>
+      </c>
+      <c r="D221" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E221" s="50" t="s">
         <v>904</v>
-      </c>
-      <c r="B221" s="131" t="s">
-        <v>905</v>
-      </c>
-      <c r="C221" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D221" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E221" s="50" t="s">
-        <v>906</v>
       </c>
       <c r="F221" s="7"/>
       <c r="G221" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H221" s="76" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
@@ -18046,26 +18021,26 @@
     </row>
     <row r="222">
       <c r="A222" s="49" t="s">
+        <v>906</v>
+      </c>
+      <c r="B222" s="131" t="s">
+        <v>907</v>
+      </c>
+      <c r="C222" s="104" t="s">
+        <v>865</v>
+      </c>
+      <c r="D222" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E222" s="50" t="s">
         <v>908</v>
-      </c>
-      <c r="B222" s="131" t="s">
-        <v>909</v>
-      </c>
-      <c r="C222" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D222" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E222" s="50" t="s">
-        <v>910</v>
       </c>
       <c r="F222" s="7"/>
       <c r="G222" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H222" s="76" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="I222" s="7"/>
       <c r="J222" s="7"/>
@@ -18073,26 +18048,26 @@
     </row>
     <row r="223">
       <c r="A223" s="49" t="s">
+        <v>910</v>
+      </c>
+      <c r="B223" s="131" t="s">
+        <v>911</v>
+      </c>
+      <c r="C223" s="104" t="s">
+        <v>865</v>
+      </c>
+      <c r="D223" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E223" s="70" t="s">
         <v>912</v>
-      </c>
-      <c r="B223" s="131" t="s">
-        <v>913</v>
-      </c>
-      <c r="C223" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D223" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E223" s="70" t="s">
-        <v>914</v>
       </c>
       <c r="F223" s="7"/>
       <c r="G223" s="7" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H223" s="128" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="I223" s="7"/>
       <c r="J223" s="7"/>
@@ -18100,26 +18075,26 @@
     </row>
     <row r="224">
       <c r="A224" s="49" t="s">
+        <v>914</v>
+      </c>
+      <c r="B224" s="131" t="s">
+        <v>915</v>
+      </c>
+      <c r="C224" s="104" t="s">
+        <v>865</v>
+      </c>
+      <c r="D224" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E224" s="50" t="s">
         <v>916</v>
-      </c>
-      <c r="B224" s="131" t="s">
-        <v>917</v>
-      </c>
-      <c r="C224" s="104" t="s">
-        <v>867</v>
-      </c>
-      <c r="D224" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E224" s="50" t="s">
-        <v>918</v>
       </c>
       <c r="F224" s="7"/>
       <c r="G224" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H224" s="76" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
@@ -18127,10 +18102,10 @@
     </row>
     <row r="225">
       <c r="A225" s="49" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B225" s="131" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C225" s="104" t="s">
         <v>472</v>
@@ -18146,26 +18121,26 @@
     </row>
     <row r="226">
       <c r="A226" s="80" t="s">
+        <v>920</v>
+      </c>
+      <c r="B226" s="132" t="s">
+        <v>921</v>
+      </c>
+      <c r="C226" s="63" t="s">
+        <v>865</v>
+      </c>
+      <c r="D226" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E226" s="70" t="s">
         <v>922</v>
-      </c>
-      <c r="B226" s="132" t="s">
-        <v>923</v>
-      </c>
-      <c r="C226" s="63" t="s">
-        <v>867</v>
-      </c>
-      <c r="D226" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E226" s="70" t="s">
-        <v>924</v>
       </c>
       <c r="F226" s="7"/>
       <c r="G226" s="7" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H226" s="128" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="I226" s="7"/>
       <c r="J226" s="7"/>
@@ -18173,26 +18148,26 @@
     </row>
     <row r="227">
       <c r="A227" s="80" t="s">
+        <v>924</v>
+      </c>
+      <c r="B227" s="132" t="s">
+        <v>925</v>
+      </c>
+      <c r="C227" s="63" t="s">
+        <v>865</v>
+      </c>
+      <c r="D227" s="63" t="s">
+        <v>866</v>
+      </c>
+      <c r="E227" s="70" t="s">
         <v>926</v>
-      </c>
-      <c r="B227" s="132" t="s">
-        <v>927</v>
-      </c>
-      <c r="C227" s="63" t="s">
-        <v>867</v>
-      </c>
-      <c r="D227" s="63" t="s">
-        <v>868</v>
-      </c>
-      <c r="E227" s="70" t="s">
-        <v>928</v>
       </c>
       <c r="F227" s="7"/>
       <c r="G227" s="7" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H227" s="128" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="I227" s="7"/>
       <c r="J227" s="7"/>
@@ -18200,10 +18175,10 @@
     </row>
     <row r="228">
       <c r="A228" s="64" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B228" s="62" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C228" s="104" t="s">
         <v>472</v>
@@ -18219,24 +18194,24 @@
     </row>
     <row r="229">
       <c r="A229" s="49" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B229" s="131" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C229" s="133" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D229" s="63"/>
       <c r="E229" s="70" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="F229" s="7"/>
       <c r="G229" s="63" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H229" s="134" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
@@ -18244,10 +18219,10 @@
     </row>
     <row r="230">
       <c r="A230" s="64" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B230" s="62" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C230" s="104" t="s">
         <v>472</v>
@@ -18263,29 +18238,29 @@
     </row>
     <row r="231">
       <c r="A231" s="49" t="s">
+        <v>936</v>
+      </c>
+      <c r="B231" s="135" t="s">
+        <v>937</v>
+      </c>
+      <c r="C231" s="104" t="s">
         <v>938</v>
       </c>
-      <c r="B231" s="135" t="s">
+      <c r="D231" s="63" t="s">
         <v>939</v>
       </c>
-      <c r="C231" s="104" t="s">
+      <c r="E231" s="136" t="s">
         <v>940</v>
-      </c>
-      <c r="D231" s="63" t="s">
-        <v>941</v>
-      </c>
-      <c r="E231" s="136" t="s">
-        <v>942</v>
       </c>
       <c r="F231" s="7"/>
       <c r="G231" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="H231" s="66" t="s">
+        <v>942</v>
+      </c>
+      <c r="I231" s="7" t="s">
         <v>943</v>
-      </c>
-      <c r="H231" s="66" t="s">
-        <v>944</v>
-      </c>
-      <c r="I231" s="7" t="s">
-        <v>945</v>
       </c>
       <c r="J231" s="7"/>
       <c r="K231" s="7"/>
@@ -18406,78 +18381,78 @@
     </row>
     <row r="2">
       <c r="A2" s="72" t="s">
+        <v>944</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>945</v>
+      </c>
+      <c r="C2" s="70" t="s">
         <v>946</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>947</v>
-      </c>
-      <c r="C2" s="70" t="s">
-        <v>948</v>
       </c>
       <c r="D2" s="70"/>
       <c r="E2" s="40" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="72" t="s">
+        <v>944</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>945</v>
+      </c>
+      <c r="C3" s="70" t="s">
         <v>946</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>947</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>948</v>
       </c>
       <c r="D3" s="70"/>
       <c r="E3" s="40" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="72" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B4" s="66" t="s">
+        <v>951</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>952</v>
+      </c>
+      <c r="D4" s="70" t="s">
         <v>953</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="E4" s="40" t="s">
         <v>954</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="F4" s="40" t="s">
         <v>955</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>956</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="138" t="s">
+        <v>554</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>555</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="D5" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>559</v>
-      </c>
       <c r="E5" s="40" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="G5" s="139"/>
       <c r="H5" s="139"/>
@@ -18502,20 +18477,20 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>629</v>
+      </c>
+      <c r="C6" s="140" t="s">
         <v>630</v>
-      </c>
-      <c r="B6" s="66" t="s">
-        <v>631</v>
-      </c>
-      <c r="C6" s="140" t="s">
-        <v>632</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="40" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="G6" s="139"/>
       <c r="H6" s="139"/>
@@ -18540,22 +18515,22 @@
     </row>
     <row r="7">
       <c r="A7" s="72" t="s">
+        <v>672</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>673</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="D7" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>676</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>677</v>
-      </c>
       <c r="E7" s="40" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="8">
@@ -22560,36 +22535,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="141" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="142" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="143" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="144" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="8">
@@ -22600,41 +22575,41 @@
     </row>
     <row r="10">
       <c r="A10" s="144" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="144" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B11" s="145" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="146" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="147"/>
       <c r="B13" s="148" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="149" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="150" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="151" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="17">
@@ -22643,24 +22618,24 @@
     </row>
     <row r="18">
       <c r="A18" s="144" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B18" s="152" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B19" s="153"/>
     </row>
     <row r="21">
       <c r="A21" s="144" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B21" s="154" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
   </sheetData>
@@ -22686,52 +22661,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="144" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="155" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="155" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="155" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
   </sheetData>
@@ -22757,53 +22732,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B1" s="156" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="138" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
   </sheetData>
@@ -22847,35 +22822,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="157" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C1" s="157" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>1010</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1012</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -22884,13 +22859,13 @@
     </row>
     <row r="4">
       <c r="A4" s="40" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D4" s="158" t="str">
         <f t="shared" si="1"/>
@@ -22899,70 +22874,70 @@
     </row>
     <row r="5">
       <c r="A5" s="40" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>1016</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D7" s="159" t="s">
         <v>1019</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D7" s="159" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>1022</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="160" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B9" s="161" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C9" s="161" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D9" s="161" t="s">
         <v>1025</v>
-      </c>
-      <c r="B9" s="161" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C9" s="161" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D9" s="161" t="s">
-        <v>1027</v>
       </c>
       <c r="E9" s="161"/>
       <c r="F9" s="161"/>
@@ -22989,16 +22964,16 @@
     </row>
     <row r="10">
       <c r="A10" s="160" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B10" s="161" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C10" s="161" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D10" s="161" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="E10" s="162"/>
       <c r="F10" s="162"/>
@@ -23025,16 +23000,16 @@
     </row>
     <row r="11">
       <c r="A11" s="160" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B11" s="161" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C11" s="161" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D11" s="161" t="s">
         <v>1030</v>
-      </c>
-      <c r="B11" s="161" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C11" s="161" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D11" s="161" t="s">
-        <v>1032</v>
       </c>
       <c r="E11" s="162"/>
       <c r="F11" s="162"/>
@@ -23061,16 +23036,16 @@
     </row>
     <row r="12">
       <c r="A12" s="160" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B12" s="161" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C12" s="161" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D12" s="161" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E12" s="162"/>
       <c r="F12" s="162"/>
@@ -23097,16 +23072,16 @@
     </row>
     <row r="13">
       <c r="A13" s="160" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B13" s="160" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C13" s="161" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D13" s="161" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="E13" s="162"/>
       <c r="F13" s="162"/>
@@ -23133,16 +23108,16 @@
     </row>
     <row r="14">
       <c r="A14" s="160" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B14" s="160" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C14" s="161" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D14" s="161" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E14" s="162"/>
       <c r="F14" s="162"/>
@@ -23194,51 +23169,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="163" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="144" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B2" s="144" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C2" s="144" t="s">
         <v>1006</v>
       </c>
-      <c r="B2" s="144" t="s">
+      <c r="D2" s="144" t="s">
         <v>1007</v>
-      </c>
-      <c r="C2" s="144" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D2" s="144" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C5" s="164" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>1043</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C5" s="164" t="s">
-        <v>1042</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>1045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>